<commit_message>
Product Image name, made nullable
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="372">
   <si>
     <t>Name</t>
   </si>
@@ -1146,6 +1146,9 @@
   </si>
   <si>
     <t>Author of a message, which is carried out on the basis of a wishlist product</t>
+  </si>
+  <si>
+    <t>name_nullable</t>
   </si>
 </sst>
 </file>
@@ -1329,6 +1332,18 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="60">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1998,18 +2013,6 @@
     </dxf>
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2237,56 +2240,60 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I44" totalsRowShown="0" dataDxfId="47">
-  <autoFilter ref="A1:I44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I45" totalsRowShown="0" dataDxfId="48">
+  <autoFilter ref="A1:I45"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="46"/>
-    <tableColumn id="2" name="Type" dataDxfId="45"/>
-    <tableColumn id="3" name="Name" dataDxfId="44"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="43"/>
-    <tableColumn id="5" name="Method1" dataDxfId="42"/>
-    <tableColumn id="6" name="Method2" dataDxfId="41"/>
-    <tableColumn id="7" name="Method3" dataDxfId="40"/>
-    <tableColumn id="8" name="Method4" dataDxfId="39"/>
-    <tableColumn id="9" name="Method5" dataDxfId="38"/>
+    <tableColumn id="1" name="Column" dataDxfId="47"/>
+    <tableColumn id="2" name="Type" dataDxfId="46"/>
+    <tableColumn id="3" name="Name" dataDxfId="45"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="44"/>
+    <tableColumn id="5" name="Method1" dataDxfId="43"/>
+    <tableColumn id="6" name="Method2" dataDxfId="42"/>
+    <tableColumn id="7" name="Method3" dataDxfId="41"/>
+    <tableColumn id="8" name="Method4" dataDxfId="40"/>
+    <tableColumn id="9" name="Method5" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K94" totalsRowShown="0" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K94" totalsRowShown="0" dataDxfId="38">
   <autoFilter ref="A1:K94">
-    <filterColumn colId="0"/>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="product_images"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="36"/>
-    <tableColumn id="3" name="Field" dataDxfId="35"/>
-    <tableColumn id="5" name="Type" dataDxfId="34">
+    <tableColumn id="2" name="Table" dataDxfId="37"/>
+    <tableColumn id="3" name="Field" dataDxfId="36"/>
+    <tableColumn id="5" name="Type" dataDxfId="35">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="33">
+    <tableColumn id="4" name="Name" dataDxfId="34">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="32">
+    <tableColumn id="6" name="Arg2" dataDxfId="33">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="31">
+    <tableColumn id="7" name="Method1" dataDxfId="32">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="30">
+    <tableColumn id="8" name="Method2" dataDxfId="31">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="29">
+    <tableColumn id="9" name="Method3" dataDxfId="30">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="28">
+    <tableColumn id="10" name="Method4" dataDxfId="29">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="27">
+    <tableColumn id="11" name="Method5" dataDxfId="28">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="26">
+    <tableColumn id="12" name="Statement" dataDxfId="27">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2295,7 +2302,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R79" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R79" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:R79">
     <filterColumn colId="1">
       <filters>
@@ -2304,46 +2311,46 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="23">
+    <tableColumn id="19" name="TRCode" dataDxfId="24">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="22"/>
-    <tableColumn id="2" name="Record No" dataDxfId="21">
+    <tableColumn id="1" name="Table Name" dataDxfId="23"/>
+    <tableColumn id="2" name="Record No" dataDxfId="22">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="20"/>
-    <tableColumn id="4" name="2" dataDxfId="19"/>
-    <tableColumn id="5" name="3" dataDxfId="18"/>
-    <tableColumn id="6" name="4" dataDxfId="17"/>
-    <tableColumn id="7" name="5" dataDxfId="16"/>
-    <tableColumn id="8" name="6" dataDxfId="15"/>
-    <tableColumn id="9" name="7" dataDxfId="14"/>
-    <tableColumn id="10" name="8" dataDxfId="13"/>
-    <tableColumn id="11" name="9" dataDxfId="12"/>
-    <tableColumn id="12" name="10" dataDxfId="11"/>
-    <tableColumn id="13" name="11" dataDxfId="10"/>
-    <tableColumn id="14" name="12" dataDxfId="9"/>
-    <tableColumn id="15" name="13" dataDxfId="8"/>
-    <tableColumn id="16" name="14" dataDxfId="7"/>
-    <tableColumn id="17" name="15" dataDxfId="6"/>
+    <tableColumn id="3" name="1" dataDxfId="21"/>
+    <tableColumn id="4" name="2" dataDxfId="20"/>
+    <tableColumn id="5" name="3" dataDxfId="19"/>
+    <tableColumn id="6" name="4" dataDxfId="18"/>
+    <tableColumn id="7" name="5" dataDxfId="17"/>
+    <tableColumn id="8" name="6" dataDxfId="16"/>
+    <tableColumn id="9" name="7" dataDxfId="15"/>
+    <tableColumn id="10" name="8" dataDxfId="14"/>
+    <tableColumn id="11" name="9" dataDxfId="13"/>
+    <tableColumn id="12" name="10" dataDxfId="12"/>
+    <tableColumn id="13" name="11" dataDxfId="11"/>
+    <tableColumn id="14" name="12" dataDxfId="10"/>
+    <tableColumn id="15" name="13" dataDxfId="9"/>
+    <tableColumn id="16" name="14" dataDxfId="8"/>
+    <tableColumn id="17" name="15" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E48" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E48" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:E48"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="4"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="3"/>
-    <tableColumn id="20" name="NS" dataDxfId="2">
+    <tableColumn id="1" name="Name" dataDxfId="5"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="4"/>
+    <tableColumn id="20" name="NS" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="1">
+    <tableColumn id="21" name="Model" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="0"/>
+    <tableColumn id="4" name="Query Method" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4910,10 +4917,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -5008,13 +5015,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>221</v>
+        <v>371</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>221</v>
+        <v>95</v>
       </c>
       <c r="D5" s="3">
         <v>64</v>
@@ -5029,16 +5036,16 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>168</v>
+        <v>221</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>168</v>
+        <v>221</v>
       </c>
       <c r="D6" s="3">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>222</v>
@@ -5050,16 +5057,16 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="D7" s="3">
-        <v>1024</v>
+        <v>256</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>222</v>
@@ -5071,40 +5078,38 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>223</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1024</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>220</v>
-      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>228</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>220</v>
@@ -5115,17 +5120,19 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D10" s="3"/>
+        <v>226</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>220</v>
@@ -5136,13 +5143,13 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>224</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
@@ -5157,34 +5164,34 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="3">
-        <v>32</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="D13" s="3">
         <v>32</v>
@@ -5199,16 +5206,16 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D14" s="3">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>222</v>
@@ -5220,16 +5227,16 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D15" s="3">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>222</v>
@@ -5241,13 +5248,13 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D16" s="3">
         <v>256</v>
@@ -5262,13 +5269,13 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D17" s="3">
         <v>256</v>
@@ -5283,13 +5290,13 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D18" s="3">
         <v>256</v>
@@ -5304,13 +5311,13 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D19" s="3">
         <v>256</v>
@@ -5325,126 +5332,126 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
+      </c>
+      <c r="D20" s="3">
+        <v>256</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>220</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D21" s="3">
-        <v>32</v>
+        <v>114</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F21" s="3"/>
+        <v>240</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>241</v>
+      </c>
+      <c r="D22" s="3">
+        <v>32</v>
+      </c>
       <c r="E22" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>220</v>
-      </c>
+      <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D23" s="3">
-        <v>128</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
+      </c>
+      <c r="D24" s="3">
+        <v>128</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>220</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="3" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>245</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>246</v>
+      </c>
       <c r="E25" s="3" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>220</v>
@@ -5455,13 +5462,13 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>224</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
@@ -5476,99 +5483,99 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>280</v>
+        <v>224</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="F27" s="3"/>
+        <v>222</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>224</v>
+        <v>280</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>220</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>280</v>
+        <v>224</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F29" s="3"/>
+        <v>222</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>227</v>
+        <v>280</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>228</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>220</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>252</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="E31" s="3" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>220</v>
@@ -5579,19 +5586,17 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>246</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>220</v>
@@ -5602,55 +5607,57 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="D33" s="3">
-        <v>512</v>
+        <v>254</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F33" s="3"/>
+        <v>255</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D34" s="3"/>
+        <v>256</v>
+      </c>
+      <c r="D34" s="3">
+        <v>512</v>
+      </c>
       <c r="E34" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>220</v>
-      </c>
+      <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="3" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>224</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
@@ -5665,45 +5672,41 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>264</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="3" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>259</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
         <v>260</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>262</v>
@@ -5715,63 +5718,63 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>259</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
         <v>260</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>262</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>259</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
         <v>260</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>262</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>259</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
@@ -5790,45 +5793,45 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>259</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
         <v>260</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>262</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>259</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>257</v>
+        <v>212</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
         <v>260</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>262</v>
@@ -5840,38 +5843,38 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>259</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
         <v>260</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>262</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I43" s="3"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>259</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
@@ -5888,9 +5891,34 @@
       </c>
       <c r="I44" s="3"/>
     </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I45" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A44">
-    <cfRule type="duplicateValues" dxfId="48" priority="27"/>
+  <conditionalFormatting sqref="A2:A45">
+    <cfRule type="duplicateValues" dxfId="0" priority="28"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -5904,8 +5932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K359"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K73" sqref="K73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -5951,7 +5979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" hidden="1">
       <c r="A2" s="1" t="s">
         <v>207</v>
       </c>
@@ -5995,7 +6023,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="1" t="s">
         <v>207</v>
       </c>
@@ -6039,7 +6067,7 @@
         <v>$table-&gt;string('name', 64)-&gt;index();</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" hidden="1">
       <c r="A4" s="1" t="s">
         <v>207</v>
       </c>
@@ -6083,7 +6111,7 @@
         <v>$table-&gt;string('description', 1024)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" hidden="1">
       <c r="A5" s="1" t="s">
         <v>207</v>
       </c>
@@ -6127,7 +6155,7 @@
         <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" hidden="1">
       <c r="A6" s="1" t="s">
         <v>207</v>
       </c>
@@ -6171,7 +6199,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" hidden="1">
       <c r="A7" s="2" t="s">
         <v>209</v>
       </c>
@@ -6215,7 +6243,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" hidden="1">
       <c r="A8" s="2" t="s">
         <v>209</v>
       </c>
@@ -6259,7 +6287,7 @@
         <v>$table-&gt;string('name', 64)-&gt;index();</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" hidden="1">
       <c r="A9" s="2" t="s">
         <v>209</v>
       </c>
@@ -6303,7 +6331,7 @@
         <v>$table-&gt;string('description', 1024)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" hidden="1">
       <c r="A10" s="2" t="s">
         <v>209</v>
       </c>
@@ -6347,7 +6375,7 @@
         <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" hidden="1">
       <c r="A11" s="2" t="s">
         <v>209</v>
       </c>
@@ -6391,7 +6419,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" hidden="1">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
@@ -6435,7 +6463,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" hidden="1">
       <c r="A13" s="3" t="s">
         <v>50</v>
       </c>
@@ -6479,7 +6507,7 @@
         <v>$table-&gt;string('name', 64)-&gt;index();</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" hidden="1">
       <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
@@ -6523,7 +6551,7 @@
         <v>$table-&gt;string('description', 1024)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" hidden="1">
       <c r="A15" s="3" t="s">
         <v>50</v>
       </c>
@@ -6567,7 +6595,7 @@
         <v>$table-&gt;unsignedInteger('brand')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" hidden="1">
       <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
@@ -6611,7 +6639,7 @@
         <v>$table-&gt;unsignedInteger('category')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" hidden="1">
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
@@ -6655,7 +6683,7 @@
         <v>$table-&gt;string('no', 32)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" hidden="1">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
@@ -6699,7 +6727,7 @@
         <v>$table-&gt;string('code', 64)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" hidden="1">
       <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
@@ -6743,7 +6771,7 @@
         <v>$table-&gt;string('size', 32)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" hidden="1">
       <c r="A20" s="3" t="s">
         <v>50</v>
       </c>
@@ -6787,7 +6815,7 @@
         <v>$table-&gt;string('stock', 32)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" hidden="1">
       <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
@@ -6831,7 +6859,7 @@
         <v>$table-&gt;enum('type', ['Public','Private'])-&gt;default('Public')-&gt;index();</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" hidden="1">
       <c r="A22" s="3" t="s">
         <v>50</v>
       </c>
@@ -6875,7 +6903,7 @@
         <v>$table-&gt;string('detail1', 256)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" hidden="1">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
@@ -6919,7 +6947,7 @@
         <v>$table-&gt;string('detail2', 256)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" hidden="1">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -6963,7 +6991,7 @@
         <v>$table-&gt;string('detail3', 256)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" hidden="1">
       <c r="A25" s="3" t="s">
         <v>50</v>
       </c>
@@ -7007,7 +7035,7 @@
         <v>$table-&gt;string('detail4', 256)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" hidden="1">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -7051,7 +7079,7 @@
         <v>$table-&gt;string('detail5', 256)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" hidden="1">
       <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
@@ -7095,7 +7123,7 @@
         <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" hidden="1">
       <c r="A28" s="3" t="s">
         <v>50</v>
       </c>
@@ -7139,7 +7167,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" hidden="1">
       <c r="A29" s="3" t="s">
         <v>50</v>
       </c>
@@ -7183,7 +7211,7 @@
         <v>$table-&gt;foreign('brand')-&gt;references('id')-&gt;on('brands')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" hidden="1">
       <c r="A30" s="3" t="s">
         <v>50</v>
       </c>
@@ -7276,7 +7304,7 @@
         <v>210</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>95</v>
+        <v>371</v>
       </c>
       <c r="C32" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -7292,7 +7320,7 @@
       </c>
       <c r="F32" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;index()</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G32" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -7312,7 +7340,7 @@
       </c>
       <c r="K32" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('name', 64)-&gt;index();</v>
+        <v>$table-&gt;string('name', 64)-&gt;nullable();</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -7579,7 +7607,7 @@
         <v>$table-&gt;foreign('product')-&gt;references('id')-&gt;on('products')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" hidden="1">
       <c r="A39" s="3" t="s">
         <v>211</v>
       </c>
@@ -7623,7 +7651,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" hidden="1">
       <c r="A40" s="3" t="s">
         <v>211</v>
       </c>
@@ -7667,7 +7695,7 @@
         <v>$table-&gt;string('name', 64)-&gt;index();</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" hidden="1">
       <c r="A41" s="3" t="s">
         <v>211</v>
       </c>
@@ -7711,7 +7739,7 @@
         <v>$table-&gt;string('email', 256)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" hidden="1">
       <c r="A42" s="3" t="s">
         <v>211</v>
       </c>
@@ -7755,7 +7783,7 @@
         <v>$table-&gt;string('number', 64)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" hidden="1">
       <c r="A43" s="3" t="s">
         <v>211</v>
       </c>
@@ -7799,7 +7827,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" hidden="1">
       <c r="A44" s="3" t="s">
         <v>213</v>
       </c>
@@ -7843,7 +7871,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" hidden="1">
       <c r="A45" s="3" t="s">
         <v>213</v>
       </c>
@@ -7887,7 +7915,7 @@
         <v>$table-&gt;string('name', 64)-&gt;index();</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" hidden="1">
       <c r="A46" s="3" t="s">
         <v>213</v>
       </c>
@@ -7931,7 +7959,7 @@
         <v>$table-&gt;string('description', 1024)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" hidden="1">
       <c r="A47" s="3" t="s">
         <v>213</v>
       </c>
@@ -7975,7 +8003,7 @@
         <v>$table-&gt;unsignedInteger('author')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" hidden="1">
       <c r="A48" s="3" t="s">
         <v>213</v>
       </c>
@@ -8019,7 +8047,7 @@
         <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" hidden="1">
       <c r="A49" s="3" t="s">
         <v>213</v>
       </c>
@@ -8063,7 +8091,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" hidden="1">
       <c r="A50" s="3" t="s">
         <v>213</v>
       </c>
@@ -8107,7 +8135,7 @@
         <v>$table-&gt;foreign('author')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" hidden="1">
       <c r="A51" s="3" t="s">
         <v>215</v>
       </c>
@@ -8151,7 +8179,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" hidden="1">
       <c r="A52" s="3" t="s">
         <v>215</v>
       </c>
@@ -8195,7 +8223,7 @@
         <v>$table-&gt;unsignedInteger('visitor')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" hidden="1">
       <c r="A53" s="3" t="s">
         <v>215</v>
       </c>
@@ -8239,7 +8267,7 @@
         <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" hidden="1">
       <c r="A54" s="3" t="s">
         <v>215</v>
       </c>
@@ -8283,7 +8311,7 @@
         <v>$table-&gt;enum('viewed', ['Yes','No'])-&gt;default('No')-&gt;index();</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" hidden="1">
       <c r="A55" s="3" t="s">
         <v>215</v>
       </c>
@@ -8327,7 +8355,7 @@
         <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" hidden="1">
       <c r="A56" s="3" t="s">
         <v>215</v>
       </c>
@@ -8371,7 +8399,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" hidden="1">
       <c r="A57" s="3" t="s">
         <v>215</v>
       </c>
@@ -8415,7 +8443,7 @@
         <v>$table-&gt;foreign('visitor')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" hidden="1">
       <c r="A58" s="3" t="s">
         <v>215</v>
       </c>
@@ -8459,7 +8487,7 @@
         <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" hidden="1">
       <c r="A59" s="3" t="s">
         <v>217</v>
       </c>
@@ -8503,7 +8531,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" hidden="1">
       <c r="A60" s="3" t="s">
         <v>217</v>
       </c>
@@ -8547,7 +8575,7 @@
         <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" hidden="1">
       <c r="A61" s="3" t="s">
         <v>217</v>
       </c>
@@ -8591,7 +8619,7 @@
         <v>$table-&gt;string('note', 512)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" hidden="1">
       <c r="A62" s="3" t="s">
         <v>217</v>
       </c>
@@ -8635,7 +8663,7 @@
         <v>$table-&gt;unsignedInteger('author')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" hidden="1">
       <c r="A63" s="3" t="s">
         <v>217</v>
       </c>
@@ -8679,7 +8707,7 @@
         <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" hidden="1">
       <c r="A64" s="3" t="s">
         <v>217</v>
       </c>
@@ -8723,7 +8751,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" hidden="1">
       <c r="A65" s="3" t="s">
         <v>217</v>
       </c>
@@ -8767,7 +8795,7 @@
         <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" hidden="1">
       <c r="A66" s="3" t="s">
         <v>217</v>
       </c>
@@ -8811,7 +8839,7 @@
         <v>$table-&gt;foreign('author')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" hidden="1">
       <c r="A67" s="3" t="s">
         <v>214</v>
       </c>
@@ -8855,7 +8883,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" hidden="1">
       <c r="A68" s="3" t="s">
         <v>214</v>
       </c>
@@ -8899,7 +8927,7 @@
         <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" hidden="1">
       <c r="A69" s="3" t="s">
         <v>214</v>
       </c>
@@ -8943,7 +8971,7 @@
         <v>$table-&gt;unsignedInteger('product')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" hidden="1">
       <c r="A70" s="3" t="s">
         <v>214</v>
       </c>
@@ -8987,7 +9015,7 @@
         <v>$table-&gt;unsignedInteger('added_by')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" hidden="1">
       <c r="A71" s="3" t="s">
         <v>214</v>
       </c>
@@ -9031,7 +9059,7 @@
         <v>$table-&gt;timestamp('added_on')-&gt;default(DB::raw('CURRENT_TIMESTAMP'));</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" hidden="1">
       <c r="A72" s="3" t="s">
         <v>214</v>
       </c>
@@ -9075,7 +9103,7 @@
         <v>$table-&gt;unsignedInteger('removed_by')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" hidden="1">
       <c r="A73" s="3" t="s">
         <v>214</v>
       </c>
@@ -9119,7 +9147,7 @@
         <v>$table-&gt;timestamp('removed_on')-&gt;default(DB::raw('CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP'));</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" hidden="1">
       <c r="A74" s="3" t="s">
         <v>214</v>
       </c>
@@ -9163,7 +9191,7 @@
         <v>$table-&gt;enum('product_status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" hidden="1">
       <c r="A75" s="3" t="s">
         <v>214</v>
       </c>
@@ -9207,7 +9235,7 @@
         <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" hidden="1">
       <c r="A76" s="3" t="s">
         <v>214</v>
       </c>
@@ -9251,7 +9279,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" hidden="1">
       <c r="A77" s="3" t="s">
         <v>214</v>
       </c>
@@ -9295,7 +9323,7 @@
         <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" hidden="1">
       <c r="A78" s="3" t="s">
         <v>214</v>
       </c>
@@ -9339,7 +9367,7 @@
         <v>$table-&gt;foreign('product')-&gt;references('id')-&gt;on('products')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" hidden="1">
       <c r="A79" s="3" t="s">
         <v>214</v>
       </c>
@@ -9383,7 +9411,7 @@
         <v>$table-&gt;foreign('added_by')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" hidden="1">
       <c r="A80" s="3" t="s">
         <v>214</v>
       </c>
@@ -9427,7 +9455,7 @@
         <v>$table-&gt;foreign('removed_by')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" hidden="1">
       <c r="A81" s="3" t="s">
         <v>218</v>
       </c>
@@ -9471,7 +9499,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" hidden="1">
       <c r="A82" s="3" t="s">
         <v>218</v>
       </c>
@@ -9515,7 +9543,7 @@
         <v>$table-&gt;unsignedInteger('wishlist_product')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" hidden="1">
       <c r="A83" s="3" t="s">
         <v>218</v>
       </c>
@@ -9559,7 +9587,7 @@
         <v>$table-&gt;string('note', 512)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" hidden="1">
       <c r="A84" s="3" t="s">
         <v>218</v>
       </c>
@@ -9603,7 +9631,7 @@
         <v>$table-&gt;unsignedInteger('author')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" hidden="1">
       <c r="A85" s="3" t="s">
         <v>218</v>
       </c>
@@ -9647,7 +9675,7 @@
         <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" hidden="1">
       <c r="A86" s="3" t="s">
         <v>218</v>
       </c>
@@ -9691,7 +9719,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" hidden="1">
       <c r="A87" s="3" t="s">
         <v>218</v>
       </c>
@@ -9735,7 +9763,7 @@
         <v>$table-&gt;foreign('wishlist_product')-&gt;references('id')-&gt;on('wishlist_products')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" hidden="1">
       <c r="A88" s="3" t="s">
         <v>218</v>
       </c>
@@ -9779,7 +9807,7 @@
         <v>$table-&gt;foreign('author')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" hidden="1">
       <c r="A89" s="3" t="s">
         <v>216</v>
       </c>
@@ -9823,7 +9851,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" hidden="1">
       <c r="A90" s="3" t="s">
         <v>216</v>
       </c>
@@ -9867,7 +9895,7 @@
         <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" hidden="1">
       <c r="A91" s="3" t="s">
         <v>216</v>
       </c>
@@ -9911,7 +9939,7 @@
         <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" hidden="1">
       <c r="A92" s="3" t="s">
         <v>216</v>
       </c>
@@ -9955,7 +9983,7 @@
         <v>$table-&gt;enum('viewed', ['Yes','No'])-&gt;default('No')-&gt;index();</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" hidden="1">
       <c r="A93" s="3" t="s">
         <v>216</v>
       </c>
@@ -9999,7 +10027,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" hidden="1">
       <c r="A94" s="3" t="s">
         <v>216</v>
       </c>
@@ -14222,7 +14250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Visitors list actions form own and shared wishlists corrected
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="603">
   <si>
     <t>Name</t>
   </si>
@@ -1839,6 +1839,9 @@
   </si>
   <si>
     <t>Form Uploads</t>
+  </si>
+  <si>
+    <t>Own Wishlists</t>
   </si>
 </sst>
 </file>
@@ -3067,7 +3070,7 @@
   <autoFilter ref="A1:R329">
     <filterColumn colId="1">
       <filters>
-        <filter val="Form Layout"/>
+        <filter val="Resource Actions"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -12530,8 +12533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R329"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView topLeftCell="B254" workbookViewId="0">
+      <selection activeCell="G289" sqref="G289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13040,7 +13043,7 @@
       <c r="Q13" s="32"/>
       <c r="R13" s="32"/>
     </row>
-    <row r="14" spans="1:18" hidden="1">
+    <row r="14" spans="1:18">
       <c r="A14" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-0</v>
@@ -13430,7 +13433,7 @@
       <c r="Q23" s="42"/>
       <c r="R23" s="42"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" hidden="1">
       <c r="A24" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Form Layout-0</v>
@@ -18570,7 +18573,7 @@
       <c r="Q163" s="42"/>
       <c r="R163" s="42"/>
     </row>
-    <row r="164" spans="1:18">
+    <row r="164" spans="1:18" hidden="1">
       <c r="A164" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Form Layout-1</v>
@@ -18604,7 +18607,7 @@
       <c r="Q164" s="40"/>
       <c r="R164" s="40"/>
     </row>
-    <row r="165" spans="1:18">
+    <row r="165" spans="1:18" hidden="1">
       <c r="A165" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Form Layout-2</v>
@@ -18638,7 +18641,7 @@
       <c r="Q165" s="40"/>
       <c r="R165" s="40"/>
     </row>
-    <row r="166" spans="1:18">
+    <row r="166" spans="1:18" hidden="1">
       <c r="A166" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Form Layout-3</v>
@@ -21240,7 +21243,7 @@
       <c r="Q241" s="42"/>
       <c r="R241" s="42"/>
     </row>
-    <row r="242" spans="1:18" hidden="1">
+    <row r="242" spans="1:18">
       <c r="A242" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-1</v>
@@ -21312,7 +21315,7 @@
       <c r="Q243" s="42"/>
       <c r="R243" s="42"/>
     </row>
-    <row r="244" spans="1:18" hidden="1">
+    <row r="244" spans="1:18">
       <c r="A244" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-2</v>
@@ -21384,7 +21387,7 @@
       <c r="Q245" s="42"/>
       <c r="R245" s="42"/>
     </row>
-    <row r="246" spans="1:18" hidden="1">
+    <row r="246" spans="1:18">
       <c r="A246" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-3</v>
@@ -21456,7 +21459,7 @@
       <c r="Q247" s="42"/>
       <c r="R247" s="42"/>
     </row>
-    <row r="248" spans="1:18" hidden="1">
+    <row r="248" spans="1:18">
       <c r="A248" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-4</v>
@@ -21528,7 +21531,7 @@
       <c r="Q249" s="42"/>
       <c r="R249" s="42"/>
     </row>
-    <row r="250" spans="1:18" hidden="1">
+    <row r="250" spans="1:18">
       <c r="A250" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-5</v>
@@ -21600,7 +21603,7 @@
       <c r="Q251" s="42"/>
       <c r="R251" s="42"/>
     </row>
-    <row r="252" spans="1:18" hidden="1">
+    <row r="252" spans="1:18">
       <c r="A252" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-6</v>
@@ -21672,7 +21675,7 @@
       <c r="Q253" s="42"/>
       <c r="R253" s="42"/>
     </row>
-    <row r="254" spans="1:18" hidden="1">
+    <row r="254" spans="1:18">
       <c r="A254" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-7</v>
@@ -21744,7 +21747,7 @@
       <c r="Q255" s="42"/>
       <c r="R255" s="42"/>
     </row>
-    <row r="256" spans="1:18" hidden="1">
+    <row r="256" spans="1:18">
       <c r="A256" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-8</v>
@@ -21816,7 +21819,7 @@
       <c r="Q257" s="42"/>
       <c r="R257" s="42"/>
     </row>
-    <row r="258" spans="1:18" hidden="1">
+    <row r="258" spans="1:18">
       <c r="A258" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-9</v>
@@ -21888,7 +21891,7 @@
       <c r="Q259" s="42"/>
       <c r="R259" s="42"/>
     </row>
-    <row r="260" spans="1:18" hidden="1">
+    <row r="260" spans="1:18">
       <c r="A260" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-10</v>
@@ -21960,7 +21963,7 @@
       <c r="Q261" s="42"/>
       <c r="R261" s="42"/>
     </row>
-    <row r="262" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="262" spans="1:18" s="16" customFormat="1">
       <c r="A262" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-11</v>
@@ -21996,7 +21999,7 @@
       <c r="Q262" s="40"/>
       <c r="R262" s="40"/>
     </row>
-    <row r="263" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="263" spans="1:18" s="16" customFormat="1">
       <c r="A263" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-12</v>
@@ -22032,7 +22035,7 @@
       <c r="Q263" s="40"/>
       <c r="R263" s="40"/>
     </row>
-    <row r="264" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="264" spans="1:18" s="16" customFormat="1">
       <c r="A264" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-13</v>
@@ -22068,7 +22071,7 @@
       <c r="Q264" s="40"/>
       <c r="R264" s="40"/>
     </row>
-    <row r="265" spans="1:18" hidden="1">
+    <row r="265" spans="1:18">
       <c r="A265" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-14</v>
@@ -22376,7 +22379,7 @@
       <c r="Q273" s="42"/>
       <c r="R273" s="42"/>
     </row>
-    <row r="274" spans="1:18" hidden="1">
+    <row r="274" spans="1:18">
       <c r="A274" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-15</v>
@@ -22518,7 +22521,7 @@
       <c r="Q277" s="40"/>
       <c r="R277" s="40"/>
     </row>
-    <row r="278" spans="1:18" hidden="1">
+    <row r="278" spans="1:18">
       <c r="A278" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-16</v>
@@ -22690,7 +22693,7 @@
       <c r="Q282" s="42"/>
       <c r="R282" s="42"/>
     </row>
-    <row r="283" spans="1:18" hidden="1">
+    <row r="283" spans="1:18">
       <c r="A283" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-17</v>
@@ -22794,7 +22797,7 @@
       <c r="Q285" s="42"/>
       <c r="R285" s="42"/>
     </row>
-    <row r="286" spans="1:18" hidden="1">
+    <row r="286" spans="1:18">
       <c r="A286" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-18</v>
@@ -22816,7 +22819,7 @@
         <v>567</v>
       </c>
       <c r="G286" s="40" t="s">
-        <v>294</v>
+        <v>602</v>
       </c>
       <c r="H286" s="40"/>
       <c r="I286" s="40"/>
@@ -22898,7 +22901,7 @@
       <c r="Q288" s="42"/>
       <c r="R288" s="42"/>
     </row>
-    <row r="289" spans="1:18" hidden="1">
+    <row r="289" spans="1:18">
       <c r="A289" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-19</v>
@@ -22920,7 +22923,7 @@
         <v>569</v>
       </c>
       <c r="G289" s="40" t="s">
-        <v>294</v>
+        <v>506</v>
       </c>
       <c r="H289" s="40"/>
       <c r="I289" s="40"/>
@@ -23002,7 +23005,7 @@
       <c r="Q291" s="42"/>
       <c r="R291" s="42"/>
     </row>
-    <row r="292" spans="1:18" hidden="1">
+    <row r="292" spans="1:18">
       <c r="A292" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-20</v>
@@ -23106,7 +23109,7 @@
       <c r="Q294" s="42"/>
       <c r="R294" s="42"/>
     </row>
-    <row r="295" spans="1:18" hidden="1">
+    <row r="295" spans="1:18">
       <c r="A295" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-21</v>
@@ -23450,7 +23453,7 @@
       <c r="Q304" s="42"/>
       <c r="R304" s="42"/>
     </row>
-    <row r="305" spans="1:18" hidden="1">
+    <row r="305" spans="1:18">
       <c r="A305" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-22</v>
@@ -23552,7 +23555,7 @@
       <c r="Q307" s="42"/>
       <c r="R307" s="42"/>
     </row>
-    <row r="308" spans="1:18" hidden="1">
+    <row r="308" spans="1:18">
       <c r="A308" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-23</v>
@@ -23656,7 +23659,7 @@
       <c r="Q310" s="42"/>
       <c r="R310" s="42"/>
     </row>
-    <row r="311" spans="1:18" hidden="1">
+    <row r="311" spans="1:18">
       <c r="A311" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-24</v>
@@ -23760,7 +23763,7 @@
       <c r="Q313" s="42"/>
       <c r="R313" s="42"/>
     </row>
-    <row r="314" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="314" spans="1:18" s="16" customFormat="1">
       <c r="A314" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-25</v>
@@ -23864,7 +23867,7 @@
       <c r="Q316" s="42"/>
       <c r="R316" s="42"/>
     </row>
-    <row r="317" spans="1:18" hidden="1">
+    <row r="317" spans="1:18">
       <c r="A317" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-26</v>
@@ -24006,7 +24009,7 @@
       <c r="Q320" s="42"/>
       <c r="R320" s="42"/>
     </row>
-    <row r="321" spans="1:18" hidden="1">
+    <row r="321" spans="1:18">
       <c r="A321" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-27</v>
@@ -24174,7 +24177,7 @@
       <c r="Q325" s="42"/>
       <c r="R325" s="42"/>
     </row>
-    <row r="326" spans="1:18" hidden="1">
+    <row r="326" spans="1:18">
       <c r="A326" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-28</v>
@@ -25583,7 +25586,7 @@
   <dimension ref="A1:T208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25593,14 +25596,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="50" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceFormLayout::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceAction::query()</v>
       </c>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
@@ -25748,35 +25751,35 @@
       </c>
       <c r="D5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>resource_form</v>
+        <v>resource</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>form_field</v>
+        <v>name</v>
       </c>
       <c r="F5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>colspan</v>
+        <v>description</v>
       </c>
       <c r="G5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v/>
+        <v>title</v>
       </c>
       <c r="H5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v/>
+        <v>type</v>
       </c>
       <c r="I5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v/>
+        <v>menu</v>
       </c>
       <c r="J5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v/>
+        <v>icon</v>
       </c>
       <c r="K5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>
-        <v/>
+        <v>set</v>
       </c>
       <c r="L5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0))</f>
@@ -25858,7 +25861,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="48" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceFormLayout::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceAction::query()</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -25891,19 +25894,19 @@
       </c>
       <c r="D9" s="22" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource_form' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '506', </v>
+        <v xml:space="preserve">'name' =&gt; 'CategoryListAction', </v>
       </c>
       <c r="F9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '12', </v>
+        <v xml:space="preserve">'description' =&gt; 'Action to call list of categories', </v>
       </c>
       <c r="G9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Categories', </v>
       </c>
       <c r="H9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25911,7 +25914,7 @@
       </c>
       <c r="I9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Categories', </v>
       </c>
       <c r="J9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25964,19 +25967,19 @@
       </c>
       <c r="D10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_form' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '507', </v>
+        <v xml:space="preserve">'name' =&gt; 'BrandsListAction', </v>
       </c>
       <c r="F10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '6', </v>
+        <v xml:space="preserve">'description' =&gt; 'Action to call list of brands', </v>
       </c>
       <c r="G10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Brands', </v>
       </c>
       <c r="H10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25984,7 +25987,7 @@
       </c>
       <c r="I10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Brands', </v>
       </c>
       <c r="J10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26037,19 +26040,19 @@
       </c>
       <c r="D11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_form' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '508', </v>
+        <v xml:space="preserve">'name' =&gt; 'SizeListAction', </v>
       </c>
       <c r="F11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '6', </v>
+        <v xml:space="preserve">'description' =&gt; 'Action to call list of size', </v>
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Sizes', </v>
       </c>
       <c r="H11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26057,7 +26060,7 @@
       </c>
       <c r="I11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Size', </v>
       </c>
       <c r="J11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26102,27 +26105,27 @@
       </c>
       <c r="B12" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C12" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '504', </v>
       </c>
       <c r="D12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ColorListAction', </v>
       </c>
       <c r="F12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to call list of colors', </v>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Colors', </v>
       </c>
       <c r="H12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26130,7 +26133,7 @@
       </c>
       <c r="I12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Colors', </v>
       </c>
       <c r="J12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26166,7 +26169,7 @@
       </c>
       <c r="R12" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -26175,27 +26178,27 @@
       </c>
       <c r="B13" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C13" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '505', </v>
       </c>
       <c r="D13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '302', </v>
       </c>
       <c r="E13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ProductsListAction', </v>
       </c>
       <c r="F13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products', </v>
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26203,7 +26206,7 @@
       </c>
       <c r="I13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Products', </v>
       </c>
       <c r="J13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26239,7 +26242,7 @@
       </c>
       <c r="R13" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -26248,27 +26251,27 @@
       </c>
       <c r="B14" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C14" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '506', </v>
       </c>
       <c r="D14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VisitorListAction', </v>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all visitor', </v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Visitors', </v>
       </c>
       <c r="H14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26276,7 +26279,7 @@
       </c>
       <c r="I14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Visitors', </v>
       </c>
       <c r="J14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26312,7 +26315,7 @@
       </c>
       <c r="R14" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -26321,27 +26324,27 @@
       </c>
       <c r="B15" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C15" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '507', </v>
       </c>
       <c r="D15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VisitorAddAction', </v>
       </c>
       <c r="F15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to add a visitor', </v>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Add Visitor', </v>
       </c>
       <c r="H15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26349,7 +26352,7 @@
       </c>
       <c r="I15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Create Visitor', </v>
       </c>
       <c r="J15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26385,7 +26388,7 @@
       </c>
       <c r="R15" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -26394,27 +26397,27 @@
       </c>
       <c r="B16" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C16" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '508', </v>
       </c>
       <c r="D16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistListAction', </v>
       </c>
       <c r="F16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlist', </v>
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Wishlists', </v>
       </c>
       <c r="H16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26422,7 +26425,7 @@
       </c>
       <c r="I16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Wishlists', </v>
       </c>
       <c r="J16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26458,7 +26461,7 @@
       </c>
       <c r="R16" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -26467,27 +26470,27 @@
       </c>
       <c r="B17" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C17" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '509', </v>
       </c>
       <c r="D17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistCreateAction', </v>
       </c>
       <c r="F17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to create a wishlist', </v>
       </c>
       <c r="G17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Create a Wish List', </v>
       </c>
       <c r="H17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26495,7 +26498,7 @@
       </c>
       <c r="I17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Create Wish List', </v>
       </c>
       <c r="J17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26531,7 +26534,7 @@
       </c>
       <c r="R17" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -26540,27 +26543,27 @@
       </c>
       <c r="B18" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C18" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '510', </v>
       </c>
       <c r="D18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VendorWishlistAction', </v>
       </c>
       <c r="F18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlists which are shared with vendor', </v>
       </c>
       <c r="G18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Wish Lists', </v>
       </c>
       <c r="H18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26568,7 +26571,7 @@
       </c>
       <c r="I18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Vendor Wishlists', </v>
       </c>
       <c r="J18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26604,7 +26607,7 @@
       </c>
       <c r="R18" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -26613,27 +26616,27 @@
       </c>
       <c r="B19" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C19" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '511', </v>
       </c>
       <c r="D19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'CategoryProductsListAction', </v>
       </c>
       <c r="F19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a category', </v>
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26677,7 +26680,7 @@
       </c>
       <c r="R19" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -26686,27 +26689,27 @@
       </c>
       <c r="B20" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C20" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '512', </v>
       </c>
       <c r="D20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'BrandProductsListAction', </v>
       </c>
       <c r="F20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a brand', </v>
       </c>
       <c r="G20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26750,7 +26753,7 @@
       </c>
       <c r="R20" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -26759,27 +26762,27 @@
       </c>
       <c r="B21" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C21" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '513', </v>
       </c>
       <c r="D21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'SizeProductsListAction', </v>
       </c>
       <c r="F21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a size', </v>
       </c>
       <c r="G21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26823,7 +26826,7 @@
       </c>
       <c r="R21" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -26832,27 +26835,27 @@
       </c>
       <c r="B22" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C22" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '514', </v>
       </c>
       <c r="D22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ColorProductsListAction', </v>
       </c>
       <c r="F22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a color', </v>
       </c>
       <c r="G22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26896,7 +26899,7 @@
       </c>
       <c r="R22" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -26905,27 +26908,27 @@
       </c>
       <c r="B23" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C23" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '515', </v>
       </c>
       <c r="D23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '302', </v>
       </c>
       <c r="E23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'AddProductImageAction', </v>
       </c>
       <c r="F23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to add a image for a product', </v>
       </c>
       <c r="G23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Add Image', </v>
       </c>
       <c r="H23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26969,7 +26972,7 @@
       </c>
       <c r="R23" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -26978,27 +26981,27 @@
       </c>
       <c r="B24" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C24" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '516', </v>
       </c>
       <c r="D24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '302', </v>
       </c>
       <c r="E24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ProductImagesListAction', </v>
       </c>
       <c r="F24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all images of a product', </v>
       </c>
       <c r="G24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Product Images', </v>
       </c>
       <c r="H24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27042,7 +27045,7 @@
       </c>
       <c r="R24" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -27051,27 +27054,27 @@
       </c>
       <c r="B25" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '517', </v>
       </c>
       <c r="D25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '303', </v>
       </c>
       <c r="E25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ImageStatusChangeAction', </v>
       </c>
       <c r="F25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to change status of a image', </v>
       </c>
       <c r="G25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Change Image Status', </v>
       </c>
       <c r="H25" s="22" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
@@ -27115,7 +27118,7 @@
       </c>
       <c r="R25" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -27124,27 +27127,27 @@
       </c>
       <c r="B26" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '518', </v>
       </c>
       <c r="D26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VisitorWishlistListAction', </v>
       </c>
       <c r="F26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlists of a visitor', </v>
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Own Wishlists', </v>
       </c>
       <c r="H26" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27188,7 +27191,7 @@
       </c>
       <c r="R26" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -27197,27 +27200,27 @@
       </c>
       <c r="B27" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '519', </v>
       </c>
       <c r="D27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VisitorSharedWishlistListAction', </v>
       </c>
       <c r="F27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlist shared with this visitor', </v>
       </c>
       <c r="G27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Shared Wishlists', </v>
       </c>
       <c r="H27" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27261,7 +27264,7 @@
       </c>
       <c r="R27" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -27270,27 +27273,27 @@
       </c>
       <c r="B28" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '520', </v>
       </c>
       <c r="D28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistSharesListAction', </v>
       </c>
       <c r="F28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all vistors whom with wishlist shared', </v>
       </c>
       <c r="G28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Shares', </v>
       </c>
       <c r="H28" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27334,7 +27337,7 @@
       </c>
       <c r="R28" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -27343,27 +27346,27 @@
       </c>
       <c r="B29" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '521', </v>
       </c>
       <c r="D29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistProductsListAction', </v>
       </c>
       <c r="F29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'List Item details of a wishlist', </v>
       </c>
       <c r="G29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H29" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27407,7 +27410,7 @@
       </c>
       <c r="R29" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -27416,27 +27419,27 @@
       </c>
       <c r="B30" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '522', </v>
       </c>
       <c r="D30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VisitorDetailsAction', </v>
       </c>
       <c r="F30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to view details of a visitor', </v>
       </c>
       <c r="G30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Details', </v>
       </c>
       <c r="H30" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27480,7 +27483,7 @@
       </c>
       <c r="R30" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -27489,27 +27492,27 @@
       </c>
       <c r="B31" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '523', </v>
       </c>
       <c r="D31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistMessagesListAction', </v>
       </c>
       <c r="F31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all messages in a wishlist', </v>
       </c>
       <c r="G31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Messages', </v>
       </c>
       <c r="H31" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27553,7 +27556,7 @@
       </c>
       <c r="R31" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -27562,27 +27565,27 @@
       </c>
       <c r="B32" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '524', </v>
       </c>
       <c r="D32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ManageWishlistProductsAction', </v>
       </c>
       <c r="F32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to manage products in a wishlist', </v>
       </c>
       <c r="G32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H32" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27626,7 +27629,7 @@
       </c>
       <c r="R32" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -27635,27 +27638,27 @@
       </c>
       <c r="B33" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '525', </v>
       </c>
       <c r="D33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ShareWishlistAction', </v>
       </c>
       <c r="F33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to share wishlist with a visitor', </v>
       </c>
       <c r="G33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Share Wish List', </v>
       </c>
       <c r="H33" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27699,7 +27702,7 @@
       </c>
       <c r="R33" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -27708,27 +27711,27 @@
       </c>
       <c r="B34" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '526', </v>
       </c>
       <c r="D34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistDetailsAction', </v>
       </c>
       <c r="F34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to view details of a wishlist', </v>
       </c>
       <c r="G34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Details', </v>
       </c>
       <c r="H34" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27772,7 +27775,7 @@
       </c>
       <c r="R34" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -27781,27 +27784,27 @@
       </c>
       <c r="B35" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '527', </v>
       </c>
       <c r="D35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'UpdateWishlistDetailsAction', </v>
       </c>
       <c r="F35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to update wish list details', </v>
       </c>
       <c r="G35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Update', </v>
       </c>
       <c r="H35" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27845,7 +27848,7 @@
       </c>
       <c r="R35" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -27854,27 +27857,27 @@
       </c>
       <c r="B36" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '528', </v>
       </c>
       <c r="D36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'AddWishlistNoteAction', </v>
       </c>
       <c r="F36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to add wishlist message', </v>
       </c>
       <c r="G36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Add Note', </v>
       </c>
       <c r="H36" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27918,7 +27921,7 @@
       </c>
       <c r="R36" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -27927,7 +27930,7 @@
       </c>
       <c r="B37" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C37" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -28000,7 +28003,7 @@
       </c>
       <c r="B38" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C38" s="22" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Data view section, 501 miss spelled as 510 corrected
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -3070,7 +3070,7 @@
   <autoFilter ref="A1:R329">
     <filterColumn colId="1">
       <filters>
-        <filter val="Resource Actions"/>
+        <filter val="Data View Section Items"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -12533,8 +12533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R329"/>
   <sheetViews>
-    <sheetView topLeftCell="B254" workbookViewId="0">
-      <selection activeCell="G289" sqref="G289"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13043,7 +13043,7 @@
       <c r="Q13" s="32"/>
       <c r="R13" s="32"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" hidden="1">
       <c r="A14" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-0</v>
@@ -13505,7 +13505,7 @@
       <c r="Q25" s="32"/>
       <c r="R25" s="32"/>
     </row>
-    <row r="26" spans="1:18" hidden="1">
+    <row r="26" spans="1:18">
       <c r="A26" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section Items-0</v>
@@ -19611,7 +19611,7 @@
       <c r="Q193" s="42"/>
       <c r="R193" s="42"/>
     </row>
-    <row r="194" spans="1:18" hidden="1">
+    <row r="194" spans="1:18">
       <c r="A194" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-1</v>
@@ -19624,7 +19624,7 @@
         <v>501</v>
       </c>
       <c r="D194" s="42">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="E194" s="42" t="s">
         <v>477</v>
@@ -19645,7 +19645,7 @@
       <c r="Q194" s="42"/>
       <c r="R194" s="42"/>
     </row>
-    <row r="195" spans="1:18" hidden="1">
+    <row r="195" spans="1:18">
       <c r="A195" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-2</v>
@@ -19658,7 +19658,7 @@
         <v>502</v>
       </c>
       <c r="D195" s="42">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="E195" s="42" t="s">
         <v>478</v>
@@ -19715,7 +19715,7 @@
       <c r="Q196" s="42"/>
       <c r="R196" s="42"/>
     </row>
-    <row r="197" spans="1:18" hidden="1">
+    <row r="197" spans="1:18">
       <c r="A197" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-3</v>
@@ -19749,7 +19749,7 @@
       <c r="Q197" s="42"/>
       <c r="R197" s="42"/>
     </row>
-    <row r="198" spans="1:18" hidden="1">
+    <row r="198" spans="1:18">
       <c r="A198" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-4</v>
@@ -19783,7 +19783,7 @@
       <c r="Q198" s="42"/>
       <c r="R198" s="42"/>
     </row>
-    <row r="199" spans="1:18" hidden="1">
+    <row r="199" spans="1:18">
       <c r="A199" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-5</v>
@@ -19855,7 +19855,7 @@
       <c r="Q200" s="42"/>
       <c r="R200" s="42"/>
     </row>
-    <row r="201" spans="1:18" hidden="1">
+    <row r="201" spans="1:18">
       <c r="A201" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-6</v>
@@ -19889,7 +19889,7 @@
       <c r="Q201" s="40"/>
       <c r="R201" s="40"/>
     </row>
-    <row r="202" spans="1:18" hidden="1">
+    <row r="202" spans="1:18">
       <c r="A202" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-7</v>
@@ -19923,7 +19923,7 @@
       <c r="Q202" s="40"/>
       <c r="R202" s="40"/>
     </row>
-    <row r="203" spans="1:18" hidden="1">
+    <row r="203" spans="1:18">
       <c r="A203" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-8</v>
@@ -20333,7 +20333,7 @@
       <c r="Q214" s="42"/>
       <c r="R214" s="42"/>
     </row>
-    <row r="215" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="215" spans="1:18" s="16" customFormat="1">
       <c r="A215" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-9</v>
@@ -20369,7 +20369,7 @@
       <c r="Q215" s="42"/>
       <c r="R215" s="42"/>
     </row>
-    <row r="216" spans="1:18" hidden="1">
+    <row r="216" spans="1:18">
       <c r="A216" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-10</v>
@@ -20405,7 +20405,7 @@
       <c r="Q216" s="42"/>
       <c r="R216" s="42"/>
     </row>
-    <row r="217" spans="1:18" hidden="1">
+    <row r="217" spans="1:18">
       <c r="A217" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-11</v>
@@ -20475,7 +20475,7 @@
       <c r="Q218" s="42"/>
       <c r="R218" s="42"/>
     </row>
-    <row r="219" spans="1:18" hidden="1">
+    <row r="219" spans="1:18">
       <c r="A219" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-12</v>
@@ -20509,7 +20509,7 @@
       <c r="Q219" s="42"/>
       <c r="R219" s="42"/>
     </row>
-    <row r="220" spans="1:18" hidden="1">
+    <row r="220" spans="1:18">
       <c r="A220" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-13</v>
@@ -20543,7 +20543,7 @@
       <c r="Q220" s="42"/>
       <c r="R220" s="42"/>
     </row>
-    <row r="221" spans="1:18" hidden="1">
+    <row r="221" spans="1:18">
       <c r="A221" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-14</v>
@@ -20613,7 +20613,7 @@
       <c r="Q222" s="42"/>
       <c r="R222" s="42"/>
     </row>
-    <row r="223" spans="1:18" hidden="1">
+    <row r="223" spans="1:18">
       <c r="A223" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-15</v>
@@ -20649,7 +20649,7 @@
       <c r="Q223" s="42"/>
       <c r="R223" s="42"/>
     </row>
-    <row r="224" spans="1:18" hidden="1">
+    <row r="224" spans="1:18">
       <c r="A224" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-16</v>
@@ -20685,7 +20685,7 @@
       <c r="Q224" s="42"/>
       <c r="R224" s="42"/>
     </row>
-    <row r="225" spans="1:18" hidden="1">
+    <row r="225" spans="1:18">
       <c r="A225" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-17</v>
@@ -20757,7 +20757,7 @@
       <c r="Q226" s="42"/>
       <c r="R226" s="42"/>
     </row>
-    <row r="227" spans="1:18" hidden="1">
+    <row r="227" spans="1:18">
       <c r="A227" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-18</v>
@@ -20791,7 +20791,7 @@
       <c r="Q227" s="42"/>
       <c r="R227" s="42"/>
     </row>
-    <row r="228" spans="1:18" hidden="1">
+    <row r="228" spans="1:18">
       <c r="A228" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-19</v>
@@ -21243,7 +21243,7 @@
       <c r="Q241" s="42"/>
       <c r="R241" s="42"/>
     </row>
-    <row r="242" spans="1:18">
+    <row r="242" spans="1:18" hidden="1">
       <c r="A242" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-1</v>
@@ -21315,7 +21315,7 @@
       <c r="Q243" s="42"/>
       <c r="R243" s="42"/>
     </row>
-    <row r="244" spans="1:18">
+    <row r="244" spans="1:18" hidden="1">
       <c r="A244" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-2</v>
@@ -21387,7 +21387,7 @@
       <c r="Q245" s="42"/>
       <c r="R245" s="42"/>
     </row>
-    <row r="246" spans="1:18">
+    <row r="246" spans="1:18" hidden="1">
       <c r="A246" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-3</v>
@@ -21459,7 +21459,7 @@
       <c r="Q247" s="42"/>
       <c r="R247" s="42"/>
     </row>
-    <row r="248" spans="1:18">
+    <row r="248" spans="1:18" hidden="1">
       <c r="A248" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-4</v>
@@ -21531,7 +21531,7 @@
       <c r="Q249" s="42"/>
       <c r="R249" s="42"/>
     </row>
-    <row r="250" spans="1:18">
+    <row r="250" spans="1:18" hidden="1">
       <c r="A250" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-5</v>
@@ -21603,7 +21603,7 @@
       <c r="Q251" s="42"/>
       <c r="R251" s="42"/>
     </row>
-    <row r="252" spans="1:18">
+    <row r="252" spans="1:18" hidden="1">
       <c r="A252" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-6</v>
@@ -21675,7 +21675,7 @@
       <c r="Q253" s="42"/>
       <c r="R253" s="42"/>
     </row>
-    <row r="254" spans="1:18">
+    <row r="254" spans="1:18" hidden="1">
       <c r="A254" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-7</v>
@@ -21747,7 +21747,7 @@
       <c r="Q255" s="42"/>
       <c r="R255" s="42"/>
     </row>
-    <row r="256" spans="1:18">
+    <row r="256" spans="1:18" hidden="1">
       <c r="A256" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-8</v>
@@ -21819,7 +21819,7 @@
       <c r="Q257" s="42"/>
       <c r="R257" s="42"/>
     </row>
-    <row r="258" spans="1:18">
+    <row r="258" spans="1:18" hidden="1">
       <c r="A258" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-9</v>
@@ -21891,7 +21891,7 @@
       <c r="Q259" s="42"/>
       <c r="R259" s="42"/>
     </row>
-    <row r="260" spans="1:18">
+    <row r="260" spans="1:18" hidden="1">
       <c r="A260" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-10</v>
@@ -21963,7 +21963,7 @@
       <c r="Q261" s="42"/>
       <c r="R261" s="42"/>
     </row>
-    <row r="262" spans="1:18" s="16" customFormat="1">
+    <row r="262" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A262" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-11</v>
@@ -21999,7 +21999,7 @@
       <c r="Q262" s="40"/>
       <c r="R262" s="40"/>
     </row>
-    <row r="263" spans="1:18" s="16" customFormat="1">
+    <row r="263" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A263" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-12</v>
@@ -22035,7 +22035,7 @@
       <c r="Q263" s="40"/>
       <c r="R263" s="40"/>
     </row>
-    <row r="264" spans="1:18" s="16" customFormat="1">
+    <row r="264" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A264" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-13</v>
@@ -22071,7 +22071,7 @@
       <c r="Q264" s="40"/>
       <c r="R264" s="40"/>
     </row>
-    <row r="265" spans="1:18">
+    <row r="265" spans="1:18" hidden="1">
       <c r="A265" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-14</v>
@@ -22379,7 +22379,7 @@
       <c r="Q273" s="42"/>
       <c r="R273" s="42"/>
     </row>
-    <row r="274" spans="1:18">
+    <row r="274" spans="1:18" hidden="1">
       <c r="A274" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-15</v>
@@ -22521,7 +22521,7 @@
       <c r="Q277" s="40"/>
       <c r="R277" s="40"/>
     </row>
-    <row r="278" spans="1:18">
+    <row r="278" spans="1:18" hidden="1">
       <c r="A278" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-16</v>
@@ -22693,7 +22693,7 @@
       <c r="Q282" s="42"/>
       <c r="R282" s="42"/>
     </row>
-    <row r="283" spans="1:18">
+    <row r="283" spans="1:18" hidden="1">
       <c r="A283" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-17</v>
@@ -22797,7 +22797,7 @@
       <c r="Q285" s="42"/>
       <c r="R285" s="42"/>
     </row>
-    <row r="286" spans="1:18">
+    <row r="286" spans="1:18" hidden="1">
       <c r="A286" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-18</v>
@@ -22901,7 +22901,7 @@
       <c r="Q288" s="42"/>
       <c r="R288" s="42"/>
     </row>
-    <row r="289" spans="1:18">
+    <row r="289" spans="1:18" hidden="1">
       <c r="A289" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-19</v>
@@ -23005,7 +23005,7 @@
       <c r="Q291" s="42"/>
       <c r="R291" s="42"/>
     </row>
-    <row r="292" spans="1:18">
+    <row r="292" spans="1:18" hidden="1">
       <c r="A292" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-20</v>
@@ -23109,7 +23109,7 @@
       <c r="Q294" s="42"/>
       <c r="R294" s="42"/>
     </row>
-    <row r="295" spans="1:18">
+    <row r="295" spans="1:18" hidden="1">
       <c r="A295" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-21</v>
@@ -23453,7 +23453,7 @@
       <c r="Q304" s="42"/>
       <c r="R304" s="42"/>
     </row>
-    <row r="305" spans="1:18">
+    <row r="305" spans="1:18" hidden="1">
       <c r="A305" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-22</v>
@@ -23555,7 +23555,7 @@
       <c r="Q307" s="42"/>
       <c r="R307" s="42"/>
     </row>
-    <row r="308" spans="1:18">
+    <row r="308" spans="1:18" hidden="1">
       <c r="A308" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-23</v>
@@ -23659,7 +23659,7 @@
       <c r="Q310" s="42"/>
       <c r="R310" s="42"/>
     </row>
-    <row r="311" spans="1:18">
+    <row r="311" spans="1:18" hidden="1">
       <c r="A311" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-24</v>
@@ -23763,7 +23763,7 @@
       <c r="Q313" s="42"/>
       <c r="R313" s="42"/>
     </row>
-    <row r="314" spans="1:18" s="16" customFormat="1">
+    <row r="314" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A314" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-25</v>
@@ -23867,7 +23867,7 @@
       <c r="Q316" s="42"/>
       <c r="R316" s="42"/>
     </row>
-    <row r="317" spans="1:18">
+    <row r="317" spans="1:18" hidden="1">
       <c r="A317" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-26</v>
@@ -24009,7 +24009,7 @@
       <c r="Q320" s="42"/>
       <c r="R320" s="42"/>
     </row>
-    <row r="321" spans="1:18">
+    <row r="321" spans="1:18" hidden="1">
       <c r="A321" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-27</v>
@@ -24177,7 +24177,7 @@
       <c r="Q325" s="42"/>
       <c r="R325" s="42"/>
     </row>
-    <row r="326" spans="1:18">
+    <row r="326" spans="1:18" hidden="1">
       <c r="A326" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-28</v>
@@ -25586,7 +25586,7 @@
   <dimension ref="A1:T208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25596,14 +25596,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="50" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceAction::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceDataViewSectionItem::query()</v>
       </c>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
@@ -25751,35 +25751,35 @@
       </c>
       <c r="D5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>resource</v>
+        <v>section</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>name</v>
+        <v>label</v>
       </c>
       <c r="F5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>description</v>
+        <v>attribute</v>
       </c>
       <c r="G5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>title</v>
+        <v>relation</v>
       </c>
       <c r="H5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>type</v>
+        <v/>
       </c>
       <c r="I5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>menu</v>
+        <v/>
       </c>
       <c r="J5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v>icon</v>
+        <v/>
       </c>
       <c r="K5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>
-        <v>set</v>
+        <v/>
       </c>
       <c r="L5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0))</f>
@@ -25861,7 +25861,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="48" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceAction::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceDataViewSectionItem::query()</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -25894,19 +25894,19 @@
       </c>
       <c r="D9" s="22" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'section' =&gt; '501', </v>
       </c>
       <c r="E9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'CategoryListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Email Address', </v>
       </c>
       <c r="F9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to call list of categories', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'email', </v>
       </c>
       <c r="G9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Categories', </v>
+        <v/>
       </c>
       <c r="H9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25914,7 +25914,7 @@
       </c>
       <c r="I9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Categories', </v>
+        <v/>
       </c>
       <c r="J9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25967,19 +25967,19 @@
       </c>
       <c r="D10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'section' =&gt; '501', </v>
       </c>
       <c r="E10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'BrandsListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Contact Number', </v>
       </c>
       <c r="F10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to call list of brands', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'number', </v>
       </c>
       <c r="G10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Brands', </v>
+        <v/>
       </c>
       <c r="H10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25987,7 +25987,7 @@
       </c>
       <c r="I10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Brands', </v>
+        <v/>
       </c>
       <c r="J10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26040,19 +26040,19 @@
       </c>
       <c r="D11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'section' =&gt; '502', </v>
       </c>
       <c r="E11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'SizeListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Name', </v>
       </c>
       <c r="F11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to call list of size', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Sizes', </v>
+        <v/>
       </c>
       <c r="H11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26060,7 +26060,7 @@
       </c>
       <c r="I11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Size', </v>
+        <v/>
       </c>
       <c r="J11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26113,19 +26113,19 @@
       </c>
       <c r="D12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'section' =&gt; '502', </v>
       </c>
       <c r="E12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'ColorListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Description', </v>
       </c>
       <c r="F12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to call list of colors', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'description', </v>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Colors', </v>
+        <v/>
       </c>
       <c r="H12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26133,7 +26133,7 @@
       </c>
       <c r="I12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Colors', </v>
+        <v/>
       </c>
       <c r="J12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26186,19 +26186,19 @@
       </c>
       <c r="D13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '302', </v>
+        <v xml:space="preserve">'section' =&gt; '502', </v>
       </c>
       <c r="E13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'ProductsListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Products', </v>
       </c>
       <c r="F13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v xml:space="preserve">'relation' =&gt; '518', </v>
       </c>
       <c r="H13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26206,7 +26206,7 @@
       </c>
       <c r="I13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Products', </v>
+        <v/>
       </c>
       <c r="J13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26259,19 +26259,19 @@
       </c>
       <c r="D14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v xml:space="preserve">'section' =&gt; '503', </v>
       </c>
       <c r="E14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Name', </v>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all visitor', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Visitors', </v>
+        <v/>
       </c>
       <c r="H14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26279,7 +26279,7 @@
       </c>
       <c r="I14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Visitors', </v>
+        <v/>
       </c>
       <c r="J14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26332,19 +26332,19 @@
       </c>
       <c r="D15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v xml:space="preserve">'section' =&gt; '503', </v>
       </c>
       <c r="E15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorAddAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Description', </v>
       </c>
       <c r="F15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to add a visitor', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'description', </v>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Add Visitor', </v>
+        <v/>
       </c>
       <c r="H15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26352,7 +26352,7 @@
       </c>
       <c r="I15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Create Visitor', </v>
+        <v/>
       </c>
       <c r="J15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26405,19 +26405,19 @@
       </c>
       <c r="D16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'section' =&gt; '503', </v>
       </c>
       <c r="E16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Products', </v>
       </c>
       <c r="F16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlist', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Wishlists', </v>
+        <v xml:space="preserve">'relation' =&gt; '518', </v>
       </c>
       <c r="H16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26425,7 +26425,7 @@
       </c>
       <c r="I16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Wishlists', </v>
+        <v/>
       </c>
       <c r="J16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26478,19 +26478,19 @@
       </c>
       <c r="D17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'section' =&gt; '504', </v>
       </c>
       <c r="E17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistCreateAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Author', </v>
       </c>
       <c r="F17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to create a wishlist', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Create a Wish List', </v>
+        <v xml:space="preserve">'relation' =&gt; '513', </v>
       </c>
       <c r="H17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26498,7 +26498,7 @@
       </c>
       <c r="I17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Create Wish List', </v>
+        <v/>
       </c>
       <c r="J17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26551,19 +26551,19 @@
       </c>
       <c r="D18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'section' =&gt; '504', </v>
       </c>
       <c r="E18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'VendorWishlistAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Shared with Vendor', </v>
       </c>
       <c r="F18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlists which are shared with vendor', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'status', </v>
       </c>
       <c r="G18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Wish Lists', </v>
+        <v xml:space="preserve">'relation' =&gt; '514', </v>
       </c>
       <c r="H18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26571,7 +26571,7 @@
       </c>
       <c r="I18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Vendor Wishlists', </v>
+        <v/>
       </c>
       <c r="J18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26624,19 +26624,19 @@
       </c>
       <c r="D19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'section' =&gt; '504', </v>
       </c>
       <c r="E19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'CategoryProductsListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Description', </v>
       </c>
       <c r="F19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a category', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'description', </v>
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v/>
       </c>
       <c r="H19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26697,19 +26697,19 @@
       </c>
       <c r="D20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'section' =&gt; '505', </v>
       </c>
       <c r="E20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'BrandProductsListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Name', </v>
       </c>
       <c r="F20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a brand', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v/>
       </c>
       <c r="H20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26770,19 +26770,19 @@
       </c>
       <c r="D21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'section' =&gt; '505', </v>
       </c>
       <c r="E21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'SizeProductsListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Email', </v>
       </c>
       <c r="F21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a size', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'email', </v>
       </c>
       <c r="G21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v/>
       </c>
       <c r="H21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26843,19 +26843,19 @@
       </c>
       <c r="D22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'section' =&gt; '505', </v>
       </c>
       <c r="E22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'ColorProductsListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Number', </v>
       </c>
       <c r="F22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a color', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'number', </v>
       </c>
       <c r="G22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v/>
       </c>
       <c r="H22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26916,19 +26916,19 @@
       </c>
       <c r="D23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '302', </v>
+        <v xml:space="preserve">'section' =&gt; '506', </v>
       </c>
       <c r="E23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'AddProductImageAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Product', </v>
       </c>
       <c r="F23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to add a image for a product', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Add Image', </v>
+        <v xml:space="preserve">'relation' =&gt; '526', </v>
       </c>
       <c r="H23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26989,19 +26989,19 @@
       </c>
       <c r="D24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '302', </v>
+        <v xml:space="preserve">'section' =&gt; '506', </v>
       </c>
       <c r="E24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'ProductImagesListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Added By', </v>
       </c>
       <c r="F24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all images of a product', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Product Images', </v>
+        <v xml:space="preserve">'relation' =&gt; '523', </v>
       </c>
       <c r="H24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27062,19 +27062,19 @@
       </c>
       <c r="D25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '303', </v>
+        <v xml:space="preserve">'section' =&gt; '506', </v>
       </c>
       <c r="E25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'ImageStatusChangeAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Removed By', </v>
       </c>
       <c r="F25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to change status of a image', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Change Image Status', </v>
+        <v xml:space="preserve">'relation' =&gt; '524', </v>
       </c>
       <c r="H25" s="22" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
@@ -27135,19 +27135,19 @@
       </c>
       <c r="D26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v xml:space="preserve">'section' =&gt; '507', </v>
       </c>
       <c r="E26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorWishlistListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Note', </v>
       </c>
       <c r="F26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlists of a visitor', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'note', </v>
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Own Wishlists', </v>
+        <v/>
       </c>
       <c r="H26" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27208,19 +27208,19 @@
       </c>
       <c r="D27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v xml:space="preserve">'section' =&gt; '507', </v>
       </c>
       <c r="E27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorSharedWishlistListAction', </v>
+        <v xml:space="preserve">'label' =&gt; 'Author', </v>
       </c>
       <c r="F27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlist shared with this visitor', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="G27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Shared Wishlists', </v>
+        <v xml:space="preserve">'relation' =&gt; '521', </v>
       </c>
       <c r="H27" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27273,27 +27273,27 @@
       </c>
       <c r="B28" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v>;</v>
       </c>
       <c r="C28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '520', </v>
+        <v/>
       </c>
       <c r="D28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v/>
       </c>
       <c r="E28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistSharesListAction', </v>
+        <v/>
       </c>
       <c r="F28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all vistors whom with wishlist shared', </v>
+        <v/>
       </c>
       <c r="G28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Shares', </v>
+        <v/>
       </c>
       <c r="H28" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27337,7 +27337,7 @@
       </c>
       <c r="R28" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -27346,27 +27346,27 @@
       </c>
       <c r="B29" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '521', </v>
+        <v/>
       </c>
       <c r="D29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v/>
       </c>
       <c r="E29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistProductsListAction', </v>
+        <v/>
       </c>
       <c r="F29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'List Item details of a wishlist', </v>
+        <v/>
       </c>
       <c r="G29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v/>
       </c>
       <c r="H29" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27410,7 +27410,7 @@
       </c>
       <c r="R29" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -27419,27 +27419,27 @@
       </c>
       <c r="B30" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '522', </v>
+        <v/>
       </c>
       <c r="D30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v/>
       </c>
       <c r="E30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorDetailsAction', </v>
+        <v/>
       </c>
       <c r="F30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to view details of a visitor', </v>
+        <v/>
       </c>
       <c r="G30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Details', </v>
+        <v/>
       </c>
       <c r="H30" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27483,7 +27483,7 @@
       </c>
       <c r="R30" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -27492,27 +27492,27 @@
       </c>
       <c r="B31" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '523', </v>
+        <v/>
       </c>
       <c r="D31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v/>
       </c>
       <c r="E31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistMessagesListAction', </v>
+        <v/>
       </c>
       <c r="F31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all messages in a wishlist', </v>
+        <v/>
       </c>
       <c r="G31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Messages', </v>
+        <v/>
       </c>
       <c r="H31" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27556,7 +27556,7 @@
       </c>
       <c r="R31" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -27565,27 +27565,27 @@
       </c>
       <c r="B32" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '524', </v>
+        <v/>
       </c>
       <c r="D32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v/>
       </c>
       <c r="E32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'ManageWishlistProductsAction', </v>
+        <v/>
       </c>
       <c r="F32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to manage products in a wishlist', </v>
+        <v/>
       </c>
       <c r="G32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v/>
       </c>
       <c r="H32" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27629,7 +27629,7 @@
       </c>
       <c r="R32" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -27638,27 +27638,27 @@
       </c>
       <c r="B33" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '525', </v>
+        <v/>
       </c>
       <c r="D33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v/>
       </c>
       <c r="E33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'ShareWishlistAction', </v>
+        <v/>
       </c>
       <c r="F33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to share wishlist with a visitor', </v>
+        <v/>
       </c>
       <c r="G33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Share Wish List', </v>
+        <v/>
       </c>
       <c r="H33" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27702,7 +27702,7 @@
       </c>
       <c r="R33" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -27711,27 +27711,27 @@
       </c>
       <c r="B34" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '526', </v>
+        <v/>
       </c>
       <c r="D34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v/>
       </c>
       <c r="E34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistDetailsAction', </v>
+        <v/>
       </c>
       <c r="F34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to view details of a wishlist', </v>
+        <v/>
       </c>
       <c r="G34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Details', </v>
+        <v/>
       </c>
       <c r="H34" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27775,7 +27775,7 @@
       </c>
       <c r="R34" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -27784,27 +27784,27 @@
       </c>
       <c r="B35" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '527', </v>
+        <v/>
       </c>
       <c r="D35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v/>
       </c>
       <c r="E35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'UpdateWishlistDetailsAction', </v>
+        <v/>
       </c>
       <c r="F35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to update wish list details', </v>
+        <v/>
       </c>
       <c r="G35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Update', </v>
+        <v/>
       </c>
       <c r="H35" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27848,7 +27848,7 @@
       </c>
       <c r="R35" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -27857,27 +27857,27 @@
       </c>
       <c r="B36" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '528', </v>
+        <v/>
       </c>
       <c r="D36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v/>
       </c>
       <c r="E36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'AddWishlistNoteAction', </v>
+        <v/>
       </c>
       <c r="F36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to add wishlist message', </v>
+        <v/>
       </c>
       <c r="G36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Add Note', </v>
+        <v/>
       </c>
       <c r="H36" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27921,7 +27921,7 @@
       </c>
       <c r="R36" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -27930,7 +27930,7 @@
       </c>
       <c r="B37" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v/>
       </c>
       <c r="C37" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -28003,7 +28003,7 @@
       </c>
       <c r="B38" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v/>
       </c>
       <c r="C38" s="22" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
For visitors data view, wishlist to products relation are added
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -3070,8 +3070,7 @@
   <autoFilter ref="A1:R329">
     <filterColumn colId="1">
       <filters>
-        <filter val="Data View Section"/>
-        <filter val="Data View Section Items"/>
+        <filter val="Resource Data Relation"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -12535,7 +12534,7 @@
   <dimension ref="A1:R329"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D200" sqref="D200"/>
+      <selection activeCell="F207" sqref="F207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13326,7 +13325,7 @@
       <c r="Q20" s="32"/>
       <c r="R20" s="32"/>
     </row>
-    <row r="21" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="21" spans="1:18" s="16" customFormat="1">
       <c r="A21" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-0</v>
@@ -13468,7 +13467,7 @@
       <c r="Q24" s="32"/>
       <c r="R24" s="32"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" hidden="1">
       <c r="A25" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section-0</v>
@@ -13506,7 +13505,7 @@
       <c r="Q25" s="32"/>
       <c r="R25" s="32"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" hidden="1">
       <c r="A26" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section Items-0</v>
@@ -19514,7 +19513,7 @@
       <c r="Q190" s="42"/>
       <c r="R190" s="42"/>
     </row>
-    <row r="191" spans="1:18" hidden="1">
+    <row r="191" spans="1:18">
       <c r="A191" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-1</v>
@@ -19532,7 +19531,9 @@
       <c r="E191" s="42">
         <v>511</v>
       </c>
-      <c r="F191" s="42"/>
+      <c r="F191" s="42">
+        <v>518</v>
+      </c>
       <c r="G191" s="42"/>
       <c r="H191" s="42"/>
       <c r="I191" s="42"/>
@@ -19546,7 +19547,7 @@
       <c r="Q191" s="42"/>
       <c r="R191" s="42"/>
     </row>
-    <row r="192" spans="1:18" hidden="1">
+    <row r="192" spans="1:18">
       <c r="A192" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-2</v>
@@ -19564,7 +19565,9 @@
       <c r="E192" s="42">
         <v>512</v>
       </c>
-      <c r="F192" s="42"/>
+      <c r="F192" s="42">
+        <v>518</v>
+      </c>
       <c r="G192" s="42"/>
       <c r="H192" s="42"/>
       <c r="I192" s="42"/>
@@ -19578,7 +19581,7 @@
       <c r="Q192" s="42"/>
       <c r="R192" s="42"/>
     </row>
-    <row r="193" spans="1:18">
+    <row r="193" spans="1:18" hidden="1">
       <c r="A193" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section-1</v>
@@ -19612,7 +19615,7 @@
       <c r="Q193" s="42"/>
       <c r="R193" s="42"/>
     </row>
-    <row r="194" spans="1:18">
+    <row r="194" spans="1:18" hidden="1">
       <c r="A194" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-1</v>
@@ -19646,7 +19649,7 @@
       <c r="Q194" s="42"/>
       <c r="R194" s="42"/>
     </row>
-    <row r="195" spans="1:18">
+    <row r="195" spans="1:18" hidden="1">
       <c r="A195" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-2</v>
@@ -19680,7 +19683,7 @@
       <c r="Q195" s="42"/>
       <c r="R195" s="42"/>
     </row>
-    <row r="196" spans="1:18">
+    <row r="196" spans="1:18" hidden="1">
       <c r="A196" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section-2</v>
@@ -19716,7 +19719,7 @@
       <c r="Q196" s="42"/>
       <c r="R196" s="42"/>
     </row>
-    <row r="197" spans="1:18">
+    <row r="197" spans="1:18" hidden="1">
       <c r="A197" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-3</v>
@@ -19750,7 +19753,7 @@
       <c r="Q197" s="42"/>
       <c r="R197" s="42"/>
     </row>
-    <row r="198" spans="1:18">
+    <row r="198" spans="1:18" hidden="1">
       <c r="A198" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-4</v>
@@ -19784,7 +19787,7 @@
       <c r="Q198" s="42"/>
       <c r="R198" s="42"/>
     </row>
-    <row r="199" spans="1:18">
+    <row r="199" spans="1:18" hidden="1">
       <c r="A199" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-5</v>
@@ -19820,7 +19823,7 @@
       <c r="Q199" s="42"/>
       <c r="R199" s="42"/>
     </row>
-    <row r="200" spans="1:18">
+    <row r="200" spans="1:18" hidden="1">
       <c r="A200" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section-3</v>
@@ -19856,7 +19859,7 @@
       <c r="Q200" s="42"/>
       <c r="R200" s="42"/>
     </row>
-    <row r="201" spans="1:18">
+    <row r="201" spans="1:18" hidden="1">
       <c r="A201" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-6</v>
@@ -19890,7 +19893,7 @@
       <c r="Q201" s="40"/>
       <c r="R201" s="40"/>
     </row>
-    <row r="202" spans="1:18">
+    <row r="202" spans="1:18" hidden="1">
       <c r="A202" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-7</v>
@@ -19924,7 +19927,7 @@
       <c r="Q202" s="40"/>
       <c r="R202" s="40"/>
     </row>
-    <row r="203" spans="1:18">
+    <row r="203" spans="1:18" hidden="1">
       <c r="A203" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-8</v>
@@ -20068,7 +20071,7 @@
       <c r="Q206" s="42"/>
       <c r="R206" s="42"/>
     </row>
-    <row r="207" spans="1:18" hidden="1">
+    <row r="207" spans="1:18">
       <c r="A207" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-3</v>
@@ -20100,7 +20103,7 @@
       <c r="Q207" s="42"/>
       <c r="R207" s="42"/>
     </row>
-    <row r="208" spans="1:18" hidden="1">
+    <row r="208" spans="1:18">
       <c r="A208" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-4</v>
@@ -20132,7 +20135,7 @@
       <c r="Q208" s="42"/>
       <c r="R208" s="42"/>
     </row>
-    <row r="209" spans="1:18" hidden="1">
+    <row r="209" spans="1:18">
       <c r="A209" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-5</v>
@@ -20164,7 +20167,7 @@
       <c r="Q209" s="42"/>
       <c r="R209" s="42"/>
     </row>
-    <row r="210" spans="1:18" hidden="1">
+    <row r="210" spans="1:18">
       <c r="A210" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-6</v>
@@ -20198,7 +20201,7 @@
       <c r="Q210" s="42"/>
       <c r="R210" s="42"/>
     </row>
-    <row r="211" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="211" spans="1:18" s="16" customFormat="1">
       <c r="A211" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-7</v>
@@ -20232,7 +20235,7 @@
       <c r="Q211" s="42"/>
       <c r="R211" s="42"/>
     </row>
-    <row r="212" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="212" spans="1:18" s="16" customFormat="1">
       <c r="A212" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-8</v>
@@ -20266,7 +20269,7 @@
       <c r="Q212" s="42"/>
       <c r="R212" s="42"/>
     </row>
-    <row r="213" spans="1:18" hidden="1">
+    <row r="213" spans="1:18">
       <c r="A213" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-9</v>
@@ -20300,7 +20303,7 @@
       <c r="Q213" s="42"/>
       <c r="R213" s="42"/>
     </row>
-    <row r="214" spans="1:18">
+    <row r="214" spans="1:18" hidden="1">
       <c r="A214" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section-4</v>
@@ -20334,7 +20337,7 @@
       <c r="Q214" s="42"/>
       <c r="R214" s="42"/>
     </row>
-    <row r="215" spans="1:18" s="16" customFormat="1">
+    <row r="215" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A215" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-9</v>
@@ -20370,7 +20373,7 @@
       <c r="Q215" s="42"/>
       <c r="R215" s="42"/>
     </row>
-    <row r="216" spans="1:18">
+    <row r="216" spans="1:18" hidden="1">
       <c r="A216" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-10</v>
@@ -20406,7 +20409,7 @@
       <c r="Q216" s="42"/>
       <c r="R216" s="42"/>
     </row>
-    <row r="217" spans="1:18">
+    <row r="217" spans="1:18" hidden="1">
       <c r="A217" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-11</v>
@@ -20440,7 +20443,7 @@
       <c r="Q217" s="42"/>
       <c r="R217" s="42"/>
     </row>
-    <row r="218" spans="1:18">
+    <row r="218" spans="1:18" hidden="1">
       <c r="A218" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section-5</v>
@@ -20476,7 +20479,7 @@
       <c r="Q218" s="42"/>
       <c r="R218" s="42"/>
     </row>
-    <row r="219" spans="1:18">
+    <row r="219" spans="1:18" hidden="1">
       <c r="A219" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-12</v>
@@ -20510,7 +20513,7 @@
       <c r="Q219" s="42"/>
       <c r="R219" s="42"/>
     </row>
-    <row r="220" spans="1:18">
+    <row r="220" spans="1:18" hidden="1">
       <c r="A220" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-13</v>
@@ -20544,7 +20547,7 @@
       <c r="Q220" s="42"/>
       <c r="R220" s="42"/>
     </row>
-    <row r="221" spans="1:18">
+    <row r="221" spans="1:18" hidden="1">
       <c r="A221" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-14</v>
@@ -20578,7 +20581,7 @@
       <c r="Q221" s="42"/>
       <c r="R221" s="42"/>
     </row>
-    <row r="222" spans="1:18">
+    <row r="222" spans="1:18" hidden="1">
       <c r="A222" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section-6</v>
@@ -20614,7 +20617,7 @@
       <c r="Q222" s="42"/>
       <c r="R222" s="42"/>
     </row>
-    <row r="223" spans="1:18">
+    <row r="223" spans="1:18" hidden="1">
       <c r="A223" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-15</v>
@@ -20650,7 +20653,7 @@
       <c r="Q223" s="42"/>
       <c r="R223" s="42"/>
     </row>
-    <row r="224" spans="1:18">
+    <row r="224" spans="1:18" hidden="1">
       <c r="A224" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-16</v>
@@ -20686,7 +20689,7 @@
       <c r="Q224" s="42"/>
       <c r="R224" s="42"/>
     </row>
-    <row r="225" spans="1:18">
+    <row r="225" spans="1:18" hidden="1">
       <c r="A225" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-17</v>
@@ -20722,7 +20725,7 @@
       <c r="Q225" s="42"/>
       <c r="R225" s="42"/>
     </row>
-    <row r="226" spans="1:18">
+    <row r="226" spans="1:18" hidden="1">
       <c r="A226" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section-7</v>
@@ -20758,7 +20761,7 @@
       <c r="Q226" s="42"/>
       <c r="R226" s="42"/>
     </row>
-    <row r="227" spans="1:18">
+    <row r="227" spans="1:18" hidden="1">
       <c r="A227" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-18</v>
@@ -20792,7 +20795,7 @@
       <c r="Q227" s="42"/>
       <c r="R227" s="42"/>
     </row>
-    <row r="228" spans="1:18">
+    <row r="228" spans="1:18" hidden="1">
       <c r="A228" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Data View Section items-19</v>
@@ -25587,7 +25590,7 @@
   <dimension ref="A1:T208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:R17"/>
+      <selection activeCell="B6" sqref="B6:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25597,14 +25600,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>162</v>
+        <v>503</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="50" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceDataViewSection::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceDataRelation::query()</v>
       </c>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
@@ -25756,19 +25759,19 @@
       </c>
       <c r="E5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>title</v>
+        <v>relation</v>
       </c>
       <c r="F5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>title_field</v>
+        <v>nest_relation1</v>
       </c>
       <c r="G5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>relation</v>
+        <v/>
       </c>
       <c r="H5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>colspan</v>
+        <v/>
       </c>
       <c r="I5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
@@ -25862,7 +25865,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="48" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceDataViewSection::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceDataRelation::query()</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -25899,11 +25902,11 @@
       </c>
       <c r="E9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relation' =&gt; '511', </v>
       </c>
       <c r="F9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title_field' =&gt; 'name', </v>
+        <v xml:space="preserve">'nest_relation1' =&gt; '518', </v>
       </c>
       <c r="G9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25911,7 +25914,7 @@
       </c>
       <c r="H9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25972,19 +25975,19 @@
       </c>
       <c r="E10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Wish Lists', </v>
+        <v xml:space="preserve">'relation' =&gt; '512', </v>
       </c>
       <c r="F10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'nest_relation1' =&gt; '518', </v>
       </c>
       <c r="G10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '511', </v>
+        <v/>
       </c>
       <c r="H10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '6', </v>
+        <v/>
       </c>
       <c r="I10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26041,11 +26044,11 @@
       </c>
       <c r="D11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '501', </v>
+        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
       </c>
       <c r="E11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Shared Wishlists', </v>
+        <v xml:space="preserve">'relation' =&gt; '513', </v>
       </c>
       <c r="F11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26053,11 +26056,11 @@
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '512', </v>
+        <v/>
       </c>
       <c r="H11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '6', </v>
+        <v/>
       </c>
       <c r="I11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26118,11 +26121,11 @@
       </c>
       <c r="E12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relation' =&gt; '514', </v>
       </c>
       <c r="F12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title_field' =&gt; 'name', </v>
+        <v/>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26130,7 +26133,7 @@
       </c>
       <c r="H12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26191,7 +26194,7 @@
       </c>
       <c r="E13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Sharing With', </v>
+        <v xml:space="preserve">'relation' =&gt; '515', </v>
       </c>
       <c r="F13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26199,11 +26202,11 @@
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '515', </v>
+        <v/>
       </c>
       <c r="H13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26264,19 +26267,19 @@
       </c>
       <c r="E14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v xml:space="preserve">'relation' =&gt; '516', </v>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'nest_relation1' =&gt; '521', </v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '517', </v>
+        <v/>
       </c>
       <c r="H14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26337,19 +26340,19 @@
       </c>
       <c r="E15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Messages/Notes', </v>
+        <v xml:space="preserve">'relation' =&gt; '517', </v>
       </c>
       <c r="F15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'nest_relation1' =&gt; '526', </v>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '516', </v>
+        <v/>
       </c>
       <c r="H15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'colspan' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26398,23 +26401,23 @@
       </c>
       <c r="B16" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C16" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '508', </v>
       </c>
       <c r="D16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
       </c>
       <c r="E16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relation' =&gt; '517', </v>
       </c>
       <c r="F16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'nest_relation1' =&gt; '523', </v>
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26462,7 +26465,7 @@
       </c>
       <c r="R16" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -26471,23 +26474,23 @@
       </c>
       <c r="B17" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C17" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '509', </v>
       </c>
       <c r="D17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
       </c>
       <c r="E17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relation' =&gt; '517', </v>
       </c>
       <c r="F17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'nest_relation1' =&gt; '524', </v>
       </c>
       <c r="G17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26535,7 +26538,7 @@
       </c>
       <c r="R17" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -26544,7 +26547,7 @@
       </c>
       <c r="B18" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C18" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -26617,7 +26620,7 @@
       </c>
       <c r="B19" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C19" s="22" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
List actions of wishlist, title corrected
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="605">
   <si>
     <t>Name</t>
   </si>
@@ -1784,9 +1784,6 @@
     <t>Action to list all messages in a wishlist</t>
   </si>
   <si>
-    <t>Messages</t>
-  </si>
-  <si>
     <t>ManageWishlistProductsAction</t>
   </si>
   <si>
@@ -1842,6 +1839,15 @@
   </si>
   <si>
     <t>Own Wishlists</t>
+  </si>
+  <si>
+    <t>View Items</t>
+  </si>
+  <si>
+    <t>View Messages</t>
+  </si>
+  <si>
+    <t>Add/Remove Products</t>
   </si>
 </sst>
 </file>
@@ -3070,7 +3076,7 @@
   <autoFilter ref="A1:R329">
     <filterColumn colId="1">
       <filters>
-        <filter val="Resource Data Relation"/>
+        <filter val="Resource Actions"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -12533,8 +12539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R329"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F207" sqref="F207"/>
+    <sheetView topLeftCell="B254" workbookViewId="0">
+      <selection activeCell="G314" sqref="G314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13043,7 +13049,7 @@
       <c r="Q13" s="32"/>
       <c r="R13" s="32"/>
     </row>
-    <row r="14" spans="1:18" hidden="1">
+    <row r="14" spans="1:18">
       <c r="A14" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-0</v>
@@ -13325,7 +13331,7 @@
       <c r="Q20" s="32"/>
       <c r="R20" s="32"/>
     </row>
-    <row r="21" spans="1:18" s="16" customFormat="1">
+    <row r="21" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A21" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-0</v>
@@ -13689,7 +13695,7 @@
         <v>Form Uploads-0</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C31" s="12">
         <f>IF(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])=1,0,IF(ISNUMBER(VLOOKUP([Table Name],SeedMap[],6,0)),COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])+VLOOKUP([Table Name],SeedMap[],6,0)-1,COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1))</f>
@@ -18391,7 +18397,7 @@
         <v>462</v>
       </c>
       <c r="G158" s="42" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H158" s="42"/>
       <c r="I158" s="42"/>
@@ -19513,7 +19519,7 @@
       <c r="Q190" s="42"/>
       <c r="R190" s="42"/>
     </row>
-    <row r="191" spans="1:18">
+    <row r="191" spans="1:18" hidden="1">
       <c r="A191" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-1</v>
@@ -19547,7 +19553,7 @@
       <c r="Q191" s="42"/>
       <c r="R191" s="42"/>
     </row>
-    <row r="192" spans="1:18">
+    <row r="192" spans="1:18" hidden="1">
       <c r="A192" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-2</v>
@@ -20071,7 +20077,7 @@
       <c r="Q206" s="42"/>
       <c r="R206" s="42"/>
     </row>
-    <row r="207" spans="1:18">
+    <row r="207" spans="1:18" hidden="1">
       <c r="A207" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-3</v>
@@ -20103,7 +20109,7 @@
       <c r="Q207" s="42"/>
       <c r="R207" s="42"/>
     </row>
-    <row r="208" spans="1:18">
+    <row r="208" spans="1:18" hidden="1">
       <c r="A208" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-4</v>
@@ -20135,7 +20141,7 @@
       <c r="Q208" s="42"/>
       <c r="R208" s="42"/>
     </row>
-    <row r="209" spans="1:18">
+    <row r="209" spans="1:18" hidden="1">
       <c r="A209" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-5</v>
@@ -20167,7 +20173,7 @@
       <c r="Q209" s="42"/>
       <c r="R209" s="42"/>
     </row>
-    <row r="210" spans="1:18">
+    <row r="210" spans="1:18" hidden="1">
       <c r="A210" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-6</v>
@@ -20201,7 +20207,7 @@
       <c r="Q210" s="42"/>
       <c r="R210" s="42"/>
     </row>
-    <row r="211" spans="1:18" s="16" customFormat="1">
+    <row r="211" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A211" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-7</v>
@@ -20235,7 +20241,7 @@
       <c r="Q211" s="42"/>
       <c r="R211" s="42"/>
     </row>
-    <row r="212" spans="1:18" s="16" customFormat="1">
+    <row r="212" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A212" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-8</v>
@@ -20269,7 +20275,7 @@
       <c r="Q212" s="42"/>
       <c r="R212" s="42"/>
     </row>
-    <row r="213" spans="1:18">
+    <row r="213" spans="1:18" hidden="1">
       <c r="A213" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Data Relation-9</v>
@@ -21247,7 +21253,7 @@
       <c r="Q241" s="42"/>
       <c r="R241" s="42"/>
     </row>
-    <row r="242" spans="1:18" hidden="1">
+    <row r="242" spans="1:18">
       <c r="A242" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-1</v>
@@ -21319,7 +21325,7 @@
       <c r="Q243" s="42"/>
       <c r="R243" s="42"/>
     </row>
-    <row r="244" spans="1:18" hidden="1">
+    <row r="244" spans="1:18">
       <c r="A244" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-2</v>
@@ -21391,7 +21397,7 @@
       <c r="Q245" s="42"/>
       <c r="R245" s="42"/>
     </row>
-    <row r="246" spans="1:18" hidden="1">
+    <row r="246" spans="1:18">
       <c r="A246" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-3</v>
@@ -21463,7 +21469,7 @@
       <c r="Q247" s="42"/>
       <c r="R247" s="42"/>
     </row>
-    <row r="248" spans="1:18" hidden="1">
+    <row r="248" spans="1:18">
       <c r="A248" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-4</v>
@@ -21535,7 +21541,7 @@
       <c r="Q249" s="42"/>
       <c r="R249" s="42"/>
     </row>
-    <row r="250" spans="1:18" hidden="1">
+    <row r="250" spans="1:18">
       <c r="A250" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-5</v>
@@ -21607,7 +21613,7 @@
       <c r="Q251" s="42"/>
       <c r="R251" s="42"/>
     </row>
-    <row r="252" spans="1:18" hidden="1">
+    <row r="252" spans="1:18">
       <c r="A252" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-6</v>
@@ -21679,7 +21685,7 @@
       <c r="Q253" s="42"/>
       <c r="R253" s="42"/>
     </row>
-    <row r="254" spans="1:18" hidden="1">
+    <row r="254" spans="1:18">
       <c r="A254" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-7</v>
@@ -21751,7 +21757,7 @@
       <c r="Q255" s="42"/>
       <c r="R255" s="42"/>
     </row>
-    <row r="256" spans="1:18" hidden="1">
+    <row r="256" spans="1:18">
       <c r="A256" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-8</v>
@@ -21823,7 +21829,7 @@
       <c r="Q257" s="42"/>
       <c r="R257" s="42"/>
     </row>
-    <row r="258" spans="1:18" hidden="1">
+    <row r="258" spans="1:18">
       <c r="A258" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-9</v>
@@ -21895,7 +21901,7 @@
       <c r="Q259" s="42"/>
       <c r="R259" s="42"/>
     </row>
-    <row r="260" spans="1:18" hidden="1">
+    <row r="260" spans="1:18">
       <c r="A260" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-10</v>
@@ -21967,7 +21973,7 @@
       <c r="Q261" s="42"/>
       <c r="R261" s="42"/>
     </row>
-    <row r="262" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="262" spans="1:18" s="16" customFormat="1">
       <c r="A262" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-11</v>
@@ -22003,7 +22009,7 @@
       <c r="Q262" s="40"/>
       <c r="R262" s="40"/>
     </row>
-    <row r="263" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="263" spans="1:18" s="16" customFormat="1">
       <c r="A263" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-12</v>
@@ -22039,7 +22045,7 @@
       <c r="Q263" s="40"/>
       <c r="R263" s="40"/>
     </row>
-    <row r="264" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="264" spans="1:18" s="16" customFormat="1">
       <c r="A264" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-13</v>
@@ -22075,7 +22081,7 @@
       <c r="Q264" s="40"/>
       <c r="R264" s="40"/>
     </row>
-    <row r="265" spans="1:18" hidden="1">
+    <row r="265" spans="1:18">
       <c r="A265" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-14</v>
@@ -22383,7 +22389,7 @@
       <c r="Q273" s="42"/>
       <c r="R273" s="42"/>
     </row>
-    <row r="274" spans="1:18" hidden="1">
+    <row r="274" spans="1:18">
       <c r="A274" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-15</v>
@@ -22525,7 +22531,7 @@
       <c r="Q277" s="40"/>
       <c r="R277" s="40"/>
     </row>
-    <row r="278" spans="1:18" hidden="1">
+    <row r="278" spans="1:18">
       <c r="A278" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-16</v>
@@ -22697,7 +22703,7 @@
       <c r="Q282" s="42"/>
       <c r="R282" s="42"/>
     </row>
-    <row r="283" spans="1:18" hidden="1">
+    <row r="283" spans="1:18">
       <c r="A283" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-17</v>
@@ -22801,7 +22807,7 @@
       <c r="Q285" s="42"/>
       <c r="R285" s="42"/>
     </row>
-    <row r="286" spans="1:18" hidden="1">
+    <row r="286" spans="1:18">
       <c r="A286" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-18</v>
@@ -22823,7 +22829,7 @@
         <v>567</v>
       </c>
       <c r="G286" s="40" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H286" s="40"/>
       <c r="I286" s="40"/>
@@ -22905,7 +22911,7 @@
       <c r="Q288" s="42"/>
       <c r="R288" s="42"/>
     </row>
-    <row r="289" spans="1:18" hidden="1">
+    <row r="289" spans="1:18">
       <c r="A289" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-19</v>
@@ -23009,7 +23015,7 @@
       <c r="Q291" s="42"/>
       <c r="R291" s="42"/>
     </row>
-    <row r="292" spans="1:18" hidden="1">
+    <row r="292" spans="1:18">
       <c r="A292" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-20</v>
@@ -23113,7 +23119,7 @@
       <c r="Q294" s="42"/>
       <c r="R294" s="42"/>
     </row>
-    <row r="295" spans="1:18" hidden="1">
+    <row r="295" spans="1:18">
       <c r="A295" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-21</v>
@@ -23135,7 +23141,7 @@
         <v>574</v>
       </c>
       <c r="G295" s="40" t="s">
-        <v>288</v>
+        <v>602</v>
       </c>
       <c r="H295" s="40"/>
       <c r="I295" s="40"/>
@@ -23457,7 +23463,7 @@
       <c r="Q304" s="42"/>
       <c r="R304" s="42"/>
     </row>
-    <row r="305" spans="1:18" hidden="1">
+    <row r="305" spans="1:18">
       <c r="A305" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-22</v>
@@ -23559,7 +23565,7 @@
       <c r="Q307" s="42"/>
       <c r="R307" s="42"/>
     </row>
-    <row r="308" spans="1:18" hidden="1">
+    <row r="308" spans="1:18">
       <c r="A308" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-23</v>
@@ -23581,7 +23587,7 @@
         <v>582</v>
       </c>
       <c r="G308" s="40" t="s">
-        <v>583</v>
+        <v>603</v>
       </c>
       <c r="H308" s="40"/>
       <c r="I308" s="40"/>
@@ -23663,7 +23669,7 @@
       <c r="Q310" s="42"/>
       <c r="R310" s="42"/>
     </row>
-    <row r="311" spans="1:18" hidden="1">
+    <row r="311" spans="1:18">
       <c r="A311" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-24</v>
@@ -23679,13 +23685,13 @@
         <v>305</v>
       </c>
       <c r="E311" s="40" t="s">
+        <v>583</v>
+      </c>
+      <c r="F311" s="40" t="s">
         <v>584</v>
       </c>
-      <c r="F311" s="40" t="s">
-        <v>585</v>
-      </c>
       <c r="G311" s="40" t="s">
-        <v>288</v>
+        <v>604</v>
       </c>
       <c r="H311" s="40"/>
       <c r="I311" s="40"/>
@@ -23715,7 +23721,7 @@
         <v>524</v>
       </c>
       <c r="E312" s="40" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F312" s="40"/>
       <c r="G312" s="40">
@@ -23767,7 +23773,7 @@
       <c r="Q313" s="42"/>
       <c r="R313" s="42"/>
     </row>
-    <row r="314" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="314" spans="1:18" s="16" customFormat="1">
       <c r="A314" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-25</v>
@@ -23783,13 +23789,13 @@
         <v>305</v>
       </c>
       <c r="E314" s="42" t="s">
+        <v>588</v>
+      </c>
+      <c r="F314" s="42" t="s">
         <v>589</v>
       </c>
-      <c r="F314" s="42" t="s">
+      <c r="G314" s="42" t="s">
         <v>590</v>
-      </c>
-      <c r="G314" s="42" t="s">
-        <v>591</v>
       </c>
       <c r="H314" s="42"/>
       <c r="I314" s="42"/>
@@ -23871,7 +23877,7 @@
       <c r="Q316" s="42"/>
       <c r="R316" s="42"/>
     </row>
-    <row r="317" spans="1:18" hidden="1">
+    <row r="317" spans="1:18">
       <c r="A317" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-26</v>
@@ -23887,10 +23893,10 @@
         <v>305</v>
       </c>
       <c r="E317" s="40" t="s">
+        <v>586</v>
+      </c>
+      <c r="F317" s="40" t="s">
         <v>587</v>
-      </c>
-      <c r="F317" s="40" t="s">
-        <v>588</v>
       </c>
       <c r="G317" s="40" t="s">
         <v>579</v>
@@ -23989,13 +23995,13 @@
         <v>305</v>
       </c>
       <c r="E320" s="42" t="s">
+        <v>591</v>
+      </c>
+      <c r="F320" s="42" t="s">
         <v>592</v>
       </c>
-      <c r="F320" s="42" t="s">
+      <c r="G320" s="42" t="s">
         <v>593</v>
-      </c>
-      <c r="G320" s="42" t="s">
-        <v>594</v>
       </c>
       <c r="H320" s="42" t="s">
         <v>317</v>
@@ -24013,7 +24019,7 @@
       <c r="Q320" s="42"/>
       <c r="R320" s="42"/>
     </row>
-    <row r="321" spans="1:18" hidden="1">
+    <row r="321" spans="1:18">
       <c r="A321" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-27</v>
@@ -24029,10 +24035,10 @@
         <v>305</v>
       </c>
       <c r="E321" s="40" t="s">
+        <v>594</v>
+      </c>
+      <c r="F321" s="40" t="s">
         <v>595</v>
-      </c>
-      <c r="F321" s="40" t="s">
-        <v>596</v>
       </c>
       <c r="G321" s="40" t="s">
         <v>488</v>
@@ -24181,7 +24187,7 @@
       <c r="Q325" s="42"/>
       <c r="R325" s="42"/>
     </row>
-    <row r="326" spans="1:18" hidden="1">
+    <row r="326" spans="1:18">
       <c r="A326" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-28</v>
@@ -24197,13 +24203,13 @@
         <v>305</v>
       </c>
       <c r="E326" s="42" t="s">
+        <v>596</v>
+      </c>
+      <c r="F326" s="42" t="s">
         <v>597</v>
       </c>
-      <c r="F326" s="42" t="s">
+      <c r="G326" s="42" t="s">
         <v>598</v>
-      </c>
-      <c r="G326" s="42" t="s">
-        <v>599</v>
       </c>
       <c r="H326" s="42"/>
       <c r="I326" s="42"/>
@@ -24801,7 +24807,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>86</v>
@@ -25589,8 +25595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:R6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25600,14 +25606,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>503</v>
+        <v>133</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="50" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceDataRelation::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceAction::query()</v>
       </c>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
@@ -25755,35 +25761,35 @@
       </c>
       <c r="D5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>resource_data</v>
+        <v>resource</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>relation</v>
+        <v>name</v>
       </c>
       <c r="F5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>nest_relation1</v>
+        <v>description</v>
       </c>
       <c r="G5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v/>
+        <v>title</v>
       </c>
       <c r="H5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v/>
+        <v>type</v>
       </c>
       <c r="I5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v/>
+        <v>menu</v>
       </c>
       <c r="J5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v/>
+        <v>icon</v>
       </c>
       <c r="K5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>
-        <v/>
+        <v>set</v>
       </c>
       <c r="L5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0))</f>
@@ -25865,7 +25871,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="48" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceDataRelation::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceAction::query()</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -25898,19 +25904,19 @@
       </c>
       <c r="D9" s="22" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource_data' =&gt; '501', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '511', </v>
+        <v xml:space="preserve">'name' =&gt; 'CategoryListAction', </v>
       </c>
       <c r="F9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'nest_relation1' =&gt; '518', </v>
+        <v xml:space="preserve">'description' =&gt; 'Action to call list of categories', </v>
       </c>
       <c r="G9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Categories', </v>
       </c>
       <c r="H9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25918,7 +25924,7 @@
       </c>
       <c r="I9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Categories', </v>
       </c>
       <c r="J9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25971,19 +25977,19 @@
       </c>
       <c r="D10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '501', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '512', </v>
+        <v xml:space="preserve">'name' =&gt; 'BrandsListAction', </v>
       </c>
       <c r="F10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'nest_relation1' =&gt; '518', </v>
+        <v xml:space="preserve">'description' =&gt; 'Action to call list of brands', </v>
       </c>
       <c r="G10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Brands', </v>
       </c>
       <c r="H10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25991,7 +25997,7 @@
       </c>
       <c r="I10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Brands', </v>
       </c>
       <c r="J10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26044,19 +26050,19 @@
       </c>
       <c r="D11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '513', </v>
+        <v xml:space="preserve">'name' =&gt; 'SizeListAction', </v>
       </c>
       <c r="F11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to call list of size', </v>
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Sizes', </v>
       </c>
       <c r="H11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26064,7 +26070,7 @@
       </c>
       <c r="I11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Size', </v>
       </c>
       <c r="J11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26117,19 +26123,19 @@
       </c>
       <c r="D12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '514', </v>
+        <v xml:space="preserve">'name' =&gt; 'ColorListAction', </v>
       </c>
       <c r="F12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to call list of colors', </v>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Colors', </v>
       </c>
       <c r="H12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26137,7 +26143,7 @@
       </c>
       <c r="I12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Colors', </v>
       </c>
       <c r="J12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26190,19 +26196,19 @@
       </c>
       <c r="D13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '302', </v>
       </c>
       <c r="E13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '515', </v>
+        <v xml:space="preserve">'name' =&gt; 'ProductsListAction', </v>
       </c>
       <c r="F13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products', </v>
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26210,7 +26216,7 @@
       </c>
       <c r="I13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Products', </v>
       </c>
       <c r="J13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26263,19 +26269,19 @@
       </c>
       <c r="D14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '516', </v>
+        <v xml:space="preserve">'name' =&gt; 'VisitorListAction', </v>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'nest_relation1' =&gt; '521', </v>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all visitor', </v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Visitors', </v>
       </c>
       <c r="H14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26283,7 +26289,7 @@
       </c>
       <c r="I14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Visitors', </v>
       </c>
       <c r="J14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26336,19 +26342,19 @@
       </c>
       <c r="D15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '517', </v>
+        <v xml:space="preserve">'name' =&gt; 'VisitorAddAction', </v>
       </c>
       <c r="F15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'nest_relation1' =&gt; '526', </v>
+        <v xml:space="preserve">'description' =&gt; 'Action to add a visitor', </v>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Add Visitor', </v>
       </c>
       <c r="H15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26356,7 +26362,7 @@
       </c>
       <c r="I15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Create Visitor', </v>
       </c>
       <c r="J15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26409,19 +26415,19 @@
       </c>
       <c r="D16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '517', </v>
+        <v xml:space="preserve">'name' =&gt; 'WishlistListAction', </v>
       </c>
       <c r="F16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'nest_relation1' =&gt; '523', </v>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlist', </v>
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Wishlists', </v>
       </c>
       <c r="H16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26429,7 +26435,7 @@
       </c>
       <c r="I16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Wishlists', </v>
       </c>
       <c r="J16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26482,19 +26488,19 @@
       </c>
       <c r="D17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '517', </v>
+        <v xml:space="preserve">'name' =&gt; 'WishlistCreateAction', </v>
       </c>
       <c r="F17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'nest_relation1' =&gt; '524', </v>
+        <v xml:space="preserve">'description' =&gt; 'Action to create a wishlist', </v>
       </c>
       <c r="G17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Create a Wish List', </v>
       </c>
       <c r="H17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26502,7 +26508,7 @@
       </c>
       <c r="I17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Create Wish List', </v>
       </c>
       <c r="J17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26547,27 +26553,27 @@
       </c>
       <c r="B18" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C18" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '510', </v>
       </c>
       <c r="D18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VendorWishlistAction', </v>
       </c>
       <c r="F18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlists which are shared with vendor', </v>
       </c>
       <c r="G18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Wish Lists', </v>
       </c>
       <c r="H18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26575,7 +26581,7 @@
       </c>
       <c r="I18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'menu' =&gt; 'Vendor Wishlists', </v>
       </c>
       <c r="J18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26611,7 +26617,7 @@
       </c>
       <c r="R18" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -26620,27 +26626,27 @@
       </c>
       <c r="B19" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C19" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '511', </v>
       </c>
       <c r="D19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'CategoryProductsListAction', </v>
       </c>
       <c r="F19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a category', </v>
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26684,7 +26690,7 @@
       </c>
       <c r="R19" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -26693,27 +26699,27 @@
       </c>
       <c r="B20" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C20" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '512', </v>
       </c>
       <c r="D20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'BrandProductsListAction', </v>
       </c>
       <c r="F20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a brand', </v>
       </c>
       <c r="G20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26757,7 +26763,7 @@
       </c>
       <c r="R20" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -26766,27 +26772,27 @@
       </c>
       <c r="B21" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C21" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '513', </v>
       </c>
       <c r="D21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'SizeProductsListAction', </v>
       </c>
       <c r="F21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a size', </v>
       </c>
       <c r="G21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26830,7 +26836,7 @@
       </c>
       <c r="R21" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -26839,27 +26845,27 @@
       </c>
       <c r="B22" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C22" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '514', </v>
       </c>
       <c r="D22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ColorProductsListAction', </v>
       </c>
       <c r="F22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a color', </v>
       </c>
       <c r="G22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Products', </v>
       </c>
       <c r="H22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26903,7 +26909,7 @@
       </c>
       <c r="R22" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -26912,27 +26918,27 @@
       </c>
       <c r="B23" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C23" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '515', </v>
       </c>
       <c r="D23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '302', </v>
       </c>
       <c r="E23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'AddProductImageAction', </v>
       </c>
       <c r="F23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to add a image for a product', </v>
       </c>
       <c r="G23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Add Image', </v>
       </c>
       <c r="H23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26976,7 +26982,7 @@
       </c>
       <c r="R23" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -26985,27 +26991,27 @@
       </c>
       <c r="B24" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C24" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '516', </v>
       </c>
       <c r="D24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '302', </v>
       </c>
       <c r="E24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ProductImagesListAction', </v>
       </c>
       <c r="F24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all images of a product', </v>
       </c>
       <c r="G24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Product Images', </v>
       </c>
       <c r="H24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27049,7 +27055,7 @@
       </c>
       <c r="R24" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -27058,27 +27064,27 @@
       </c>
       <c r="B25" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '517', </v>
       </c>
       <c r="D25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '303', </v>
       </c>
       <c r="E25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ImageStatusChangeAction', </v>
       </c>
       <c r="F25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to change status of a image', </v>
       </c>
       <c r="G25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Change Image Status', </v>
       </c>
       <c r="H25" s="22" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
@@ -27122,7 +27128,7 @@
       </c>
       <c r="R25" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -27131,27 +27137,27 @@
       </c>
       <c r="B26" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '518', </v>
       </c>
       <c r="D26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VisitorWishlistListAction', </v>
       </c>
       <c r="F26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlists of a visitor', </v>
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Own Wishlists', </v>
       </c>
       <c r="H26" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27195,7 +27201,7 @@
       </c>
       <c r="R26" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -27204,27 +27210,27 @@
       </c>
       <c r="B27" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '519', </v>
       </c>
       <c r="D27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VisitorSharedWishlistListAction', </v>
       </c>
       <c r="F27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlist shared with this visitor', </v>
       </c>
       <c r="G27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Shared Wishlists', </v>
       </c>
       <c r="H27" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27268,7 +27274,7 @@
       </c>
       <c r="R27" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -27277,27 +27283,27 @@
       </c>
       <c r="B28" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '520', </v>
       </c>
       <c r="D28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistSharesListAction', </v>
       </c>
       <c r="F28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all vistors whom with wishlist shared', </v>
       </c>
       <c r="G28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Shares', </v>
       </c>
       <c r="H28" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27341,7 +27347,7 @@
       </c>
       <c r="R28" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -27350,27 +27356,27 @@
       </c>
       <c r="B29" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '521', </v>
       </c>
       <c r="D29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistProductsListAction', </v>
       </c>
       <c r="F29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'List Item details of a wishlist', </v>
       </c>
       <c r="G29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'View Items', </v>
       </c>
       <c r="H29" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27414,7 +27420,7 @@
       </c>
       <c r="R29" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -27423,27 +27429,27 @@
       </c>
       <c r="B30" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '522', </v>
       </c>
       <c r="D30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '304', </v>
       </c>
       <c r="E30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'VisitorDetailsAction', </v>
       </c>
       <c r="F30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to view details of a visitor', </v>
       </c>
       <c r="G30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Details', </v>
       </c>
       <c r="H30" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27487,7 +27493,7 @@
       </c>
       <c r="R30" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -27496,27 +27502,27 @@
       </c>
       <c r="B31" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '523', </v>
       </c>
       <c r="D31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistMessagesListAction', </v>
       </c>
       <c r="F31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to list all messages in a wishlist', </v>
       </c>
       <c r="G31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'View Messages', </v>
       </c>
       <c r="H31" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27560,7 +27566,7 @@
       </c>
       <c r="R31" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -27569,27 +27575,27 @@
       </c>
       <c r="B32" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '524', </v>
       </c>
       <c r="D32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ManageWishlistProductsAction', </v>
       </c>
       <c r="F32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to manage products in a wishlist', </v>
       </c>
       <c r="G32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Add/Remove Products', </v>
       </c>
       <c r="H32" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27633,7 +27639,7 @@
       </c>
       <c r="R32" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -27642,27 +27648,27 @@
       </c>
       <c r="B33" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '525', </v>
       </c>
       <c r="D33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'ShareWishlistAction', </v>
       </c>
       <c r="F33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to share wishlist with a visitor', </v>
       </c>
       <c r="G33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Share Wish List', </v>
       </c>
       <c r="H33" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27706,7 +27712,7 @@
       </c>
       <c r="R33" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -27715,27 +27721,27 @@
       </c>
       <c r="B34" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '526', </v>
       </c>
       <c r="D34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'WishlistDetailsAction', </v>
       </c>
       <c r="F34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to view details of a wishlist', </v>
       </c>
       <c r="G34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Details', </v>
       </c>
       <c r="H34" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27779,7 +27785,7 @@
       </c>
       <c r="R34" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -27788,27 +27794,27 @@
       </c>
       <c r="B35" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '527', </v>
       </c>
       <c r="D35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'UpdateWishlistDetailsAction', </v>
       </c>
       <c r="F35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to update wish list details', </v>
       </c>
       <c r="G35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Update', </v>
       </c>
       <c r="H35" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27852,7 +27858,7 @@
       </c>
       <c r="R35" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -27861,27 +27867,27 @@
       </c>
       <c r="B36" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '528', </v>
       </c>
       <c r="D36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'AddWishlistNoteAction', </v>
       </c>
       <c r="F36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Action to add wishlist message', </v>
       </c>
       <c r="G36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'title' =&gt; 'Add Note', </v>
       </c>
       <c r="H36" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27925,7 +27931,7 @@
       </c>
       <c r="R36" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -27934,7 +27940,7 @@
       </c>
       <c r="B37" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C37" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -28007,7 +28013,7 @@
       </c>
       <c r="B38" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C38" s="22" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Relation to notes from wishlist mistyped, corrected
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -3076,7 +3076,7 @@
   <autoFilter ref="A1:R329">
     <filterColumn colId="1">
       <filters>
-        <filter val="Resource Actions"/>
+        <filter val="Resource Action Method"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -12539,8 +12539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R329"/>
   <sheetViews>
-    <sheetView topLeftCell="B254" workbookViewId="0">
-      <selection activeCell="G314" sqref="G314"/>
+    <sheetView topLeftCell="B255" workbookViewId="0">
+      <selection activeCell="G312" sqref="G312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13049,7 +13049,7 @@
       <c r="Q13" s="32"/>
       <c r="R13" s="32"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" hidden="1">
       <c r="A14" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-0</v>
@@ -13093,7 +13093,7 @@
       <c r="Q14" s="32"/>
       <c r="R14" s="32"/>
     </row>
-    <row r="15" spans="1:18" hidden="1">
+    <row r="15" spans="1:18">
       <c r="A15" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-0</v>
@@ -21253,7 +21253,7 @@
       <c r="Q241" s="42"/>
       <c r="R241" s="42"/>
     </row>
-    <row r="242" spans="1:18">
+    <row r="242" spans="1:18" hidden="1">
       <c r="A242" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-1</v>
@@ -21291,7 +21291,7 @@
       <c r="Q242" s="42"/>
       <c r="R242" s="42"/>
     </row>
-    <row r="243" spans="1:18" hidden="1">
+    <row r="243" spans="1:18">
       <c r="A243" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-1</v>
@@ -21325,7 +21325,7 @@
       <c r="Q243" s="42"/>
       <c r="R243" s="42"/>
     </row>
-    <row r="244" spans="1:18">
+    <row r="244" spans="1:18" hidden="1">
       <c r="A244" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-2</v>
@@ -21363,7 +21363,7 @@
       <c r="Q244" s="40"/>
       <c r="R244" s="40"/>
     </row>
-    <row r="245" spans="1:18" hidden="1">
+    <row r="245" spans="1:18">
       <c r="A245" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-2</v>
@@ -21397,7 +21397,7 @@
       <c r="Q245" s="42"/>
       <c r="R245" s="42"/>
     </row>
-    <row r="246" spans="1:18">
+    <row r="246" spans="1:18" hidden="1">
       <c r="A246" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-3</v>
@@ -21435,7 +21435,7 @@
       <c r="Q246" s="40"/>
       <c r="R246" s="40"/>
     </row>
-    <row r="247" spans="1:18" hidden="1">
+    <row r="247" spans="1:18">
       <c r="A247" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-3</v>
@@ -21469,7 +21469,7 @@
       <c r="Q247" s="42"/>
       <c r="R247" s="42"/>
     </row>
-    <row r="248" spans="1:18">
+    <row r="248" spans="1:18" hidden="1">
       <c r="A248" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-4</v>
@@ -21507,7 +21507,7 @@
       <c r="Q248" s="40"/>
       <c r="R248" s="40"/>
     </row>
-    <row r="249" spans="1:18" hidden="1">
+    <row r="249" spans="1:18">
       <c r="A249" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-4</v>
@@ -21541,7 +21541,7 @@
       <c r="Q249" s="42"/>
       <c r="R249" s="42"/>
     </row>
-    <row r="250" spans="1:18">
+    <row r="250" spans="1:18" hidden="1">
       <c r="A250" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-5</v>
@@ -21579,7 +21579,7 @@
       <c r="Q250" s="40"/>
       <c r="R250" s="40"/>
     </row>
-    <row r="251" spans="1:18" hidden="1">
+    <row r="251" spans="1:18">
       <c r="A251" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-5</v>
@@ -21613,7 +21613,7 @@
       <c r="Q251" s="42"/>
       <c r="R251" s="42"/>
     </row>
-    <row r="252" spans="1:18">
+    <row r="252" spans="1:18" hidden="1">
       <c r="A252" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-6</v>
@@ -21651,7 +21651,7 @@
       <c r="Q252" s="40"/>
       <c r="R252" s="40"/>
     </row>
-    <row r="253" spans="1:18" hidden="1">
+    <row r="253" spans="1:18">
       <c r="A253" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-6</v>
@@ -21685,7 +21685,7 @@
       <c r="Q253" s="42"/>
       <c r="R253" s="42"/>
     </row>
-    <row r="254" spans="1:18">
+    <row r="254" spans="1:18" hidden="1">
       <c r="A254" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-7</v>
@@ -21723,7 +21723,7 @@
       <c r="Q254" s="40"/>
       <c r="R254" s="40"/>
     </row>
-    <row r="255" spans="1:18" hidden="1">
+    <row r="255" spans="1:18">
       <c r="A255" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-7</v>
@@ -21757,7 +21757,7 @@
       <c r="Q255" s="42"/>
       <c r="R255" s="42"/>
     </row>
-    <row r="256" spans="1:18">
+    <row r="256" spans="1:18" hidden="1">
       <c r="A256" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-8</v>
@@ -21795,7 +21795,7 @@
       <c r="Q256" s="40"/>
       <c r="R256" s="40"/>
     </row>
-    <row r="257" spans="1:18" hidden="1">
+    <row r="257" spans="1:18">
       <c r="A257" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-8</v>
@@ -21829,7 +21829,7 @@
       <c r="Q257" s="42"/>
       <c r="R257" s="42"/>
     </row>
-    <row r="258" spans="1:18">
+    <row r="258" spans="1:18" hidden="1">
       <c r="A258" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-9</v>
@@ -21867,7 +21867,7 @@
       <c r="Q258" s="40"/>
       <c r="R258" s="40"/>
     </row>
-    <row r="259" spans="1:18" hidden="1">
+    <row r="259" spans="1:18">
       <c r="A259" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-9</v>
@@ -21901,7 +21901,7 @@
       <c r="Q259" s="42"/>
       <c r="R259" s="42"/>
     </row>
-    <row r="260" spans="1:18">
+    <row r="260" spans="1:18" hidden="1">
       <c r="A260" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-10</v>
@@ -21939,7 +21939,7 @@
       <c r="Q260" s="40"/>
       <c r="R260" s="40"/>
     </row>
-    <row r="261" spans="1:18" hidden="1">
+    <row r="261" spans="1:18">
       <c r="A261" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-10</v>
@@ -21973,7 +21973,7 @@
       <c r="Q261" s="42"/>
       <c r="R261" s="42"/>
     </row>
-    <row r="262" spans="1:18" s="16" customFormat="1">
+    <row r="262" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A262" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-11</v>
@@ -22009,7 +22009,7 @@
       <c r="Q262" s="40"/>
       <c r="R262" s="40"/>
     </row>
-    <row r="263" spans="1:18" s="16" customFormat="1">
+    <row r="263" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A263" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-12</v>
@@ -22045,7 +22045,7 @@
       <c r="Q263" s="40"/>
       <c r="R263" s="40"/>
     </row>
-    <row r="264" spans="1:18" s="16" customFormat="1">
+    <row r="264" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A264" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-13</v>
@@ -22081,7 +22081,7 @@
       <c r="Q264" s="40"/>
       <c r="R264" s="40"/>
     </row>
-    <row r="265" spans="1:18">
+    <row r="265" spans="1:18" hidden="1">
       <c r="A265" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-14</v>
@@ -22117,7 +22117,7 @@
       <c r="Q265" s="40"/>
       <c r="R265" s="40"/>
     </row>
-    <row r="266" spans="1:18" hidden="1">
+    <row r="266" spans="1:18">
       <c r="A266" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-11</v>
@@ -22153,7 +22153,7 @@
       <c r="Q266" s="42"/>
       <c r="R266" s="42"/>
     </row>
-    <row r="267" spans="1:18" hidden="1">
+    <row r="267" spans="1:18">
       <c r="A267" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-12</v>
@@ -22189,7 +22189,7 @@
       <c r="Q267" s="42"/>
       <c r="R267" s="42"/>
     </row>
-    <row r="268" spans="1:18" hidden="1">
+    <row r="268" spans="1:18">
       <c r="A268" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-13</v>
@@ -22225,7 +22225,7 @@
       <c r="Q268" s="42"/>
       <c r="R268" s="42"/>
     </row>
-    <row r="269" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="269" spans="1:18" s="16" customFormat="1">
       <c r="A269" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-14</v>
@@ -22389,7 +22389,7 @@
       <c r="Q273" s="42"/>
       <c r="R273" s="42"/>
     </row>
-    <row r="274" spans="1:18">
+    <row r="274" spans="1:18" hidden="1">
       <c r="A274" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-15</v>
@@ -22425,7 +22425,7 @@
       <c r="Q274" s="42"/>
       <c r="R274" s="42"/>
     </row>
-    <row r="275" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="275" spans="1:18" s="16" customFormat="1">
       <c r="A275" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-15</v>
@@ -22531,7 +22531,7 @@
       <c r="Q277" s="40"/>
       <c r="R277" s="40"/>
     </row>
-    <row r="278" spans="1:18">
+    <row r="278" spans="1:18" hidden="1">
       <c r="A278" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-16</v>
@@ -22635,7 +22635,7 @@
       <c r="Q280" s="42"/>
       <c r="R280" s="42"/>
     </row>
-    <row r="281" spans="1:18" hidden="1">
+    <row r="281" spans="1:18">
       <c r="A281" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-16</v>
@@ -22703,7 +22703,7 @@
       <c r="Q282" s="42"/>
       <c r="R282" s="42"/>
     </row>
-    <row r="283" spans="1:18">
+    <row r="283" spans="1:18" hidden="1">
       <c r="A283" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-17</v>
@@ -22739,7 +22739,7 @@
       <c r="Q283" s="42"/>
       <c r="R283" s="42"/>
     </row>
-    <row r="284" spans="1:18" hidden="1">
+    <row r="284" spans="1:18">
       <c r="A284" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-17</v>
@@ -22807,7 +22807,7 @@
       <c r="Q285" s="42"/>
       <c r="R285" s="42"/>
     </row>
-    <row r="286" spans="1:18">
+    <row r="286" spans="1:18" hidden="1">
       <c r="A286" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-18</v>
@@ -22843,7 +22843,7 @@
       <c r="Q286" s="40"/>
       <c r="R286" s="40"/>
     </row>
-    <row r="287" spans="1:18" hidden="1">
+    <row r="287" spans="1:18">
       <c r="A287" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-18</v>
@@ -22911,7 +22911,7 @@
       <c r="Q288" s="42"/>
       <c r="R288" s="42"/>
     </row>
-    <row r="289" spans="1:18">
+    <row r="289" spans="1:18" hidden="1">
       <c r="A289" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-19</v>
@@ -22947,7 +22947,7 @@
       <c r="Q289" s="40"/>
       <c r="R289" s="40"/>
     </row>
-    <row r="290" spans="1:18" hidden="1">
+    <row r="290" spans="1:18">
       <c r="A290" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-19</v>
@@ -23015,7 +23015,7 @@
       <c r="Q291" s="42"/>
       <c r="R291" s="42"/>
     </row>
-    <row r="292" spans="1:18">
+    <row r="292" spans="1:18" hidden="1">
       <c r="A292" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-20</v>
@@ -23051,7 +23051,7 @@
       <c r="Q292" s="40"/>
       <c r="R292" s="40"/>
     </row>
-    <row r="293" spans="1:18" hidden="1">
+    <row r="293" spans="1:18">
       <c r="A293" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-20</v>
@@ -23119,7 +23119,7 @@
       <c r="Q294" s="42"/>
       <c r="R294" s="42"/>
     </row>
-    <row r="295" spans="1:18">
+    <row r="295" spans="1:18" hidden="1">
       <c r="A295" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-21</v>
@@ -23155,7 +23155,7 @@
       <c r="Q295" s="40"/>
       <c r="R295" s="40"/>
     </row>
-    <row r="296" spans="1:18" hidden="1">
+    <row r="296" spans="1:18">
       <c r="A296" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-21</v>
@@ -23463,7 +23463,7 @@
       <c r="Q304" s="42"/>
       <c r="R304" s="42"/>
     </row>
-    <row r="305" spans="1:18">
+    <row r="305" spans="1:18" hidden="1">
       <c r="A305" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-22</v>
@@ -23499,7 +23499,7 @@
       <c r="Q305" s="40"/>
       <c r="R305" s="40"/>
     </row>
-    <row r="306" spans="1:18" hidden="1">
+    <row r="306" spans="1:18">
       <c r="A306" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-22</v>
@@ -23565,7 +23565,7 @@
       <c r="Q307" s="42"/>
       <c r="R307" s="42"/>
     </row>
-    <row r="308" spans="1:18">
+    <row r="308" spans="1:18" hidden="1">
       <c r="A308" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-23</v>
@@ -23601,7 +23601,7 @@
       <c r="Q308" s="40"/>
       <c r="R308" s="40"/>
     </row>
-    <row r="309" spans="1:18" hidden="1">
+    <row r="309" spans="1:18">
       <c r="A309" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-23</v>
@@ -23621,7 +23621,7 @@
       </c>
       <c r="F309" s="42"/>
       <c r="G309" s="42">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="H309" s="42">
         <v>509</v>
@@ -23669,7 +23669,7 @@
       <c r="Q310" s="42"/>
       <c r="R310" s="42"/>
     </row>
-    <row r="311" spans="1:18">
+    <row r="311" spans="1:18" hidden="1">
       <c r="A311" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-24</v>
@@ -23705,7 +23705,7 @@
       <c r="Q311" s="40"/>
       <c r="R311" s="40"/>
     </row>
-    <row r="312" spans="1:18" hidden="1">
+    <row r="312" spans="1:18">
       <c r="A312" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-24</v>
@@ -23773,7 +23773,7 @@
       <c r="Q313" s="42"/>
       <c r="R313" s="42"/>
     </row>
-    <row r="314" spans="1:18" s="16" customFormat="1">
+    <row r="314" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A314" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-25</v>
@@ -23809,7 +23809,7 @@
       <c r="Q314" s="42"/>
       <c r="R314" s="42"/>
     </row>
-    <row r="315" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="315" spans="1:18" s="16" customFormat="1">
       <c r="A315" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-25</v>
@@ -23877,7 +23877,7 @@
       <c r="Q316" s="42"/>
       <c r="R316" s="42"/>
     </row>
-    <row r="317" spans="1:18">
+    <row r="317" spans="1:18" hidden="1">
       <c r="A317" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-26</v>
@@ -23913,7 +23913,7 @@
       <c r="Q317" s="40"/>
       <c r="R317" s="40"/>
     </row>
-    <row r="318" spans="1:18" hidden="1">
+    <row r="318" spans="1:18">
       <c r="A318" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-26</v>
@@ -24019,7 +24019,7 @@
       <c r="Q320" s="42"/>
       <c r="R320" s="42"/>
     </row>
-    <row r="321" spans="1:18">
+    <row r="321" spans="1:18" hidden="1">
       <c r="A321" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-27</v>
@@ -24055,7 +24055,7 @@
       <c r="Q321" s="40"/>
       <c r="R321" s="40"/>
     </row>
-    <row r="322" spans="1:18" hidden="1">
+    <row r="322" spans="1:18">
       <c r="A322" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-27</v>
@@ -24187,7 +24187,7 @@
       <c r="Q325" s="42"/>
       <c r="R325" s="42"/>
     </row>
-    <row r="326" spans="1:18">
+    <row r="326" spans="1:18" hidden="1">
       <c r="A326" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Actions-28</v>
@@ -24223,7 +24223,7 @@
       <c r="Q326" s="42"/>
       <c r="R326" s="42"/>
     </row>
-    <row r="327" spans="1:18" hidden="1">
+    <row r="327" spans="1:18">
       <c r="A327" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-28</v>
@@ -25595,8 +25595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25606,14 +25606,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="50" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceAction::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceActionMethod::query()</v>
       </c>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
@@ -25761,35 +25761,35 @@
       </c>
       <c r="D5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>resource</v>
+        <v>resource_action</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>name</v>
+        <v>type</v>
       </c>
       <c r="F5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>description</v>
+        <v>method</v>
       </c>
       <c r="G5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>title</v>
+        <v>idn1</v>
       </c>
       <c r="H5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>type</v>
+        <v>idn2</v>
       </c>
       <c r="I5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>menu</v>
+        <v>idn3</v>
       </c>
       <c r="J5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v>icon</v>
+        <v>idn4</v>
       </c>
       <c r="K5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>
-        <v>set</v>
+        <v>idn5</v>
       </c>
       <c r="L5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0))</f>
@@ -25871,7 +25871,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="48" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceAction::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceActionMethod::query()</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -25904,19 +25904,19 @@
       </c>
       <c r="D9" s="22" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '501', </v>
       </c>
       <c r="E9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'CategoryListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'List', </v>
       </c>
       <c r="F9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to call list of categories', </v>
+        <v/>
       </c>
       <c r="G9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Categories', </v>
+        <v xml:space="preserve">'idn1' =&gt; '501', </v>
       </c>
       <c r="H9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25924,7 +25924,7 @@
       </c>
       <c r="I9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Categories', </v>
+        <v/>
       </c>
       <c r="J9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25977,19 +25977,19 @@
       </c>
       <c r="D10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '502', </v>
       </c>
       <c r="E10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'BrandsListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'List', </v>
       </c>
       <c r="F10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to call list of brands', </v>
+        <v/>
       </c>
       <c r="G10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Brands', </v>
+        <v xml:space="preserve">'idn1' =&gt; '502', </v>
       </c>
       <c r="H10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25997,7 +25997,7 @@
       </c>
       <c r="I10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Brands', </v>
+        <v/>
       </c>
       <c r="J10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26050,19 +26050,19 @@
       </c>
       <c r="D11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '503', </v>
       </c>
       <c r="E11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'SizeListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'List', </v>
       </c>
       <c r="F11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to call list of size', </v>
+        <v/>
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Sizes', </v>
+        <v xml:space="preserve">'idn1' =&gt; '503', </v>
       </c>
       <c r="H11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26070,7 +26070,7 @@
       </c>
       <c r="I11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Size', </v>
+        <v/>
       </c>
       <c r="J11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26123,19 +26123,19 @@
       </c>
       <c r="D12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '504', </v>
       </c>
       <c r="E12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'ColorListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'List', </v>
       </c>
       <c r="F12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to call list of colors', </v>
+        <v/>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Colors', </v>
+        <v xml:space="preserve">'idn1' =&gt; '504', </v>
       </c>
       <c r="H12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26143,7 +26143,7 @@
       </c>
       <c r="I12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Colors', </v>
+        <v/>
       </c>
       <c r="J12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26196,19 +26196,19 @@
       </c>
       <c r="D13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '302', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '505', </v>
       </c>
       <c r="E13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'ProductsListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'List', </v>
       </c>
       <c r="F13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products', </v>
+        <v/>
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v xml:space="preserve">'idn1' =&gt; '505', </v>
       </c>
       <c r="H13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26216,7 +26216,7 @@
       </c>
       <c r="I13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Products', </v>
+        <v/>
       </c>
       <c r="J13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26269,19 +26269,19 @@
       </c>
       <c r="D14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '506', </v>
       </c>
       <c r="E14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'List', </v>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all visitor', </v>
+        <v/>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Visitors', </v>
+        <v xml:space="preserve">'idn1' =&gt; '506', </v>
       </c>
       <c r="H14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26289,7 +26289,7 @@
       </c>
       <c r="I14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Visitors', </v>
+        <v/>
       </c>
       <c r="J14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26342,19 +26342,19 @@
       </c>
       <c r="D15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '507', </v>
       </c>
       <c r="E15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorAddAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'Form', </v>
       </c>
       <c r="F15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to add a visitor', </v>
+        <v/>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Add Visitor', </v>
+        <v xml:space="preserve">'idn1' =&gt; '503', </v>
       </c>
       <c r="H15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26362,7 +26362,7 @@
       </c>
       <c r="I15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Create Visitor', </v>
+        <v/>
       </c>
       <c r="J15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26415,19 +26415,19 @@
       </c>
       <c r="D16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '508', </v>
       </c>
       <c r="E16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'List', </v>
       </c>
       <c r="F16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlist', </v>
+        <v/>
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Wishlists', </v>
+        <v xml:space="preserve">'idn1' =&gt; '507', </v>
       </c>
       <c r="H16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26435,7 +26435,7 @@
       </c>
       <c r="I16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Wishlists', </v>
+        <v/>
       </c>
       <c r="J16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26488,19 +26488,19 @@
       </c>
       <c r="D17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '509', </v>
       </c>
       <c r="E17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistCreateAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'Form', </v>
       </c>
       <c r="F17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to create a wishlist', </v>
+        <v/>
       </c>
       <c r="G17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Create a Wish List', </v>
+        <v xml:space="preserve">'idn1' =&gt; '504', </v>
       </c>
       <c r="H17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26508,7 +26508,7 @@
       </c>
       <c r="I17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Create Wish List', </v>
+        <v/>
       </c>
       <c r="J17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26561,19 +26561,19 @@
       </c>
       <c r="D18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '510', </v>
       </c>
       <c r="E18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'VendorWishlistAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'List', </v>
       </c>
       <c r="F18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlists which are shared with vendor', </v>
+        <v/>
       </c>
       <c r="G18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Wish Lists', </v>
+        <v xml:space="preserve">'idn1' =&gt; '508', </v>
       </c>
       <c r="H18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26581,7 +26581,7 @@
       </c>
       <c r="I18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'menu' =&gt; 'Vendor Wishlists', </v>
+        <v/>
       </c>
       <c r="J18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26634,23 +26634,23 @@
       </c>
       <c r="D19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '511', </v>
       </c>
       <c r="E19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'CategoryProductsListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a category', </v>
+        <v/>
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v xml:space="preserve">'idn1' =&gt; '501', </v>
       </c>
       <c r="H19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '505', </v>
       </c>
       <c r="I19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26707,23 +26707,23 @@
       </c>
       <c r="D20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '512', </v>
       </c>
       <c r="E20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'BrandProductsListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a brand', </v>
+        <v/>
       </c>
       <c r="G20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v xml:space="preserve">'idn1' =&gt; '502', </v>
       </c>
       <c r="H20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '505', </v>
       </c>
       <c r="I20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26780,23 +26780,23 @@
       </c>
       <c r="D21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '513', </v>
       </c>
       <c r="E21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'SizeProductsListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a size', </v>
+        <v/>
       </c>
       <c r="G21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v xml:space="preserve">'idn1' =&gt; '503', </v>
       </c>
       <c r="H21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '505', </v>
       </c>
       <c r="I21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26853,23 +26853,23 @@
       </c>
       <c r="D22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '301', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '514', </v>
       </c>
       <c r="E22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'ColorProductsListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all products of a color', </v>
+        <v/>
       </c>
       <c r="G22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Products', </v>
+        <v xml:space="preserve">'idn1' =&gt; '504', </v>
       </c>
       <c r="H22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '505', </v>
       </c>
       <c r="I22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26926,23 +26926,23 @@
       </c>
       <c r="D23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '302', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '515', </v>
       </c>
       <c r="E23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'AddProductImageAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'AddRelation', </v>
       </c>
       <c r="F23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to add a image for a product', </v>
+        <v/>
       </c>
       <c r="G23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Add Image', </v>
+        <v xml:space="preserve">'idn1' =&gt; '509', </v>
       </c>
       <c r="H23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '501', </v>
       </c>
       <c r="I23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26999,23 +26999,23 @@
       </c>
       <c r="D24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource' =&gt; '302', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '516', </v>
       </c>
       <c r="E24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'ProductImagesListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all images of a product', </v>
+        <v/>
       </c>
       <c r="G24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'title' =&gt; 'Product Images', </v>
+        <v xml:space="preserve">'idn1' =&gt; '509', </v>
       </c>
       <c r="H24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '510', </v>
       </c>
       <c r="I24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27072,23 +27072,23 @@
       </c>
       <c r="D25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '303', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '517', </v>
       </c>
       <c r="E25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'ImageStatusChangeAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'FormWithData', </v>
       </c>
       <c r="F25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to change status of a image', </v>
+        <v/>
       </c>
       <c r="G25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Change Image Status', </v>
+        <v xml:space="preserve">'idn1' =&gt; '502', </v>
       </c>
       <c r="H25" s="22" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '502', </v>
       </c>
       <c r="I25" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27145,23 +27145,23 @@
       </c>
       <c r="D26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '518', </v>
       </c>
       <c r="E26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorWishlistListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlists of a visitor', </v>
+        <v/>
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Own Wishlists', </v>
+        <v xml:space="preserve">'idn1' =&gt; '511', </v>
       </c>
       <c r="H26" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '507', </v>
       </c>
       <c r="I26" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27218,23 +27218,23 @@
       </c>
       <c r="D27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '519', </v>
       </c>
       <c r="E27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorSharedWishlistListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all wishlist shared with this visitor', </v>
+        <v/>
       </c>
       <c r="G27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Shared Wishlists', </v>
+        <v xml:space="preserve">'idn1' =&gt; '512', </v>
       </c>
       <c r="H27" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '507', </v>
       </c>
       <c r="I27" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27291,23 +27291,23 @@
       </c>
       <c r="D28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '520', </v>
       </c>
       <c r="E28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistSharesListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all vistors whom with wishlist shared', </v>
+        <v/>
       </c>
       <c r="G28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Shares', </v>
+        <v xml:space="preserve">'idn1' =&gt; '515', </v>
       </c>
       <c r="H28" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '506', </v>
       </c>
       <c r="I28" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27364,23 +27364,23 @@
       </c>
       <c r="D29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '521', </v>
       </c>
       <c r="E29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistProductsListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'List Item details of a wishlist', </v>
+        <v/>
       </c>
       <c r="G29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'View Items', </v>
+        <v xml:space="preserve">'idn1' =&gt; '517', </v>
       </c>
       <c r="H29" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '511', </v>
       </c>
       <c r="I29" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27437,19 +27437,19 @@
       </c>
       <c r="D30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '304', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '522', </v>
       </c>
       <c r="E30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'VisitorDetailsAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'Data', </v>
       </c>
       <c r="F30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to view details of a visitor', </v>
+        <v/>
       </c>
       <c r="G30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Details', </v>
+        <v xml:space="preserve">'idn1' =&gt; '501', </v>
       </c>
       <c r="H30" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27510,23 +27510,23 @@
       </c>
       <c r="D31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '523', </v>
       </c>
       <c r="E31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistMessagesListAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
       </c>
       <c r="F31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to list all messages in a wishlist', </v>
+        <v/>
       </c>
       <c r="G31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'View Messages', </v>
+        <v xml:space="preserve">'idn1' =&gt; '516', </v>
       </c>
       <c r="H31" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '509', </v>
       </c>
       <c r="I31" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27583,23 +27583,23 @@
       </c>
       <c r="D32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '524', </v>
       </c>
       <c r="E32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'ManageWishlistProductsAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'ManageRelation', </v>
       </c>
       <c r="F32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to manage products in a wishlist', </v>
+        <v/>
       </c>
       <c r="G32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Add/Remove Products', </v>
+        <v xml:space="preserve">'idn1' =&gt; '518', </v>
       </c>
       <c r="H32" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '505', </v>
       </c>
       <c r="I32" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27656,23 +27656,23 @@
       </c>
       <c r="D33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '525', </v>
       </c>
       <c r="E33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'ShareWishlistAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'AddRelation', </v>
       </c>
       <c r="F33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to share wishlist with a visitor', </v>
+        <v/>
       </c>
       <c r="G33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Share Wish List', </v>
+        <v xml:space="preserve">'idn1' =&gt; '528', </v>
       </c>
       <c r="H33" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '506', </v>
       </c>
       <c r="I33" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27729,19 +27729,19 @@
       </c>
       <c r="D34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '526', </v>
       </c>
       <c r="E34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'WishlistDetailsAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'Data', </v>
       </c>
       <c r="F34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to view details of a wishlist', </v>
+        <v/>
       </c>
       <c r="G34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Details', </v>
+        <v xml:space="preserve">'idn1' =&gt; '503', </v>
       </c>
       <c r="H34" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27802,23 +27802,23 @@
       </c>
       <c r="D35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '527', </v>
       </c>
       <c r="E35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'UpdateWishlistDetailsAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'FormWithData', </v>
       </c>
       <c r="F35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to update wish list details', </v>
+        <v/>
       </c>
       <c r="G35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Update', </v>
+        <v xml:space="preserve">'idn1' =&gt; '505', </v>
       </c>
       <c r="H35" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '503', </v>
       </c>
       <c r="I35" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27875,23 +27875,23 @@
       </c>
       <c r="D36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '305', </v>
+        <v xml:space="preserve">'resource_action' =&gt; '528', </v>
       </c>
       <c r="E36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'AddWishlistNoteAction', </v>
+        <v xml:space="preserve">'type' =&gt; 'AddRelation', </v>
       </c>
       <c r="F36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Action to add wishlist message', </v>
+        <v/>
       </c>
       <c r="G36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'title' =&gt; 'Add Note', </v>
+        <v xml:space="preserve">'idn1' =&gt; '516', </v>
       </c>
       <c r="H36" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'idn2' =&gt; '507', </v>
       </c>
       <c r="I36" s="22" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
Field option added for Wishlist products
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="605">
   <si>
     <t>Name</t>
   </si>
@@ -3072,11 +3072,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R329" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A1:R329">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R330" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:R330">
     <filterColumn colId="1">
       <filters>
-        <filter val="Resource Action Method"/>
+        <filter val="Resource Form Field Data"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -12537,10 +12537,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R329"/>
+  <dimension ref="A1:R330"/>
   <sheetViews>
-    <sheetView topLeftCell="B255" workbookViewId="0">
-      <selection activeCell="G312" sqref="G312"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F173" sqref="F173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13009,7 +13009,7 @@
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
     </row>
-    <row r="13" spans="1:18" hidden="1">
+    <row r="13" spans="1:18">
       <c r="A13" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-0</v>
@@ -13093,7 +13093,7 @@
       <c r="Q14" s="32"/>
       <c r="R14" s="32"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" hidden="1">
       <c r="A15" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-0</v>
@@ -18037,7 +18037,7 @@
       <c r="Q147" s="42"/>
       <c r="R147" s="42"/>
     </row>
-    <row r="148" spans="1:18" hidden="1">
+    <row r="148" spans="1:18">
       <c r="A148" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-1</v>
@@ -18069,7 +18069,7 @@
       <c r="Q148" s="42"/>
       <c r="R148" s="42"/>
     </row>
-    <row r="149" spans="1:18" hidden="1">
+    <row r="149" spans="1:18">
       <c r="A149" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-2</v>
@@ -18101,7 +18101,7 @@
       <c r="Q149" s="42"/>
       <c r="R149" s="42"/>
     </row>
-    <row r="150" spans="1:18" hidden="1">
+    <row r="150" spans="1:18">
       <c r="A150" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-3</v>
@@ -18133,7 +18133,7 @@
       <c r="Q150" s="42"/>
       <c r="R150" s="42"/>
     </row>
-    <row r="151" spans="1:18" hidden="1">
+    <row r="151" spans="1:18">
       <c r="A151" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-4</v>
@@ -18239,7 +18239,7 @@
       <c r="Q153" s="42"/>
       <c r="R153" s="42"/>
     </row>
-    <row r="154" spans="1:18" hidden="1">
+    <row r="154" spans="1:18">
       <c r="A154" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-5</v>
@@ -18483,7 +18483,7 @@
       <c r="Q160" s="42"/>
       <c r="R160" s="42"/>
     </row>
-    <row r="161" spans="1:18" hidden="1">
+    <row r="161" spans="1:18">
       <c r="A161" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-6</v>
@@ -18515,7 +18515,7 @@
       <c r="Q161" s="42"/>
       <c r="R161" s="42"/>
     </row>
-    <row r="162" spans="1:18" hidden="1">
+    <row r="162" spans="1:18">
       <c r="A162" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-7</v>
@@ -18547,7 +18547,7 @@
       <c r="Q162" s="42"/>
       <c r="R162" s="42"/>
     </row>
-    <row r="163" spans="1:18" hidden="1">
+    <row r="163" spans="1:18">
       <c r="A163" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-8</v>
@@ -18827,7 +18827,7 @@
       <c r="Q170" s="42"/>
       <c r="R170" s="42"/>
     </row>
-    <row r="171" spans="1:18" hidden="1">
+    <row r="171" spans="1:18">
       <c r="A171" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-9</v>
@@ -18859,7 +18859,7 @@
       <c r="Q171" s="42"/>
       <c r="R171" s="42"/>
     </row>
-    <row r="172" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="172" spans="1:18" s="16" customFormat="1">
       <c r="A172" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-10</v>
@@ -18891,7 +18891,7 @@
       <c r="Q172" s="42"/>
       <c r="R172" s="42"/>
     </row>
-    <row r="173" spans="1:18" hidden="1">
+    <row r="173" spans="1:18">
       <c r="A173" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-11</v>
@@ -19035,7 +19035,7 @@
       <c r="Q176" s="40"/>
       <c r="R176" s="40"/>
     </row>
-    <row r="177" spans="1:18" hidden="1">
+    <row r="177" spans="1:18">
       <c r="A177" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-12</v>
@@ -19067,7 +19067,7 @@
       <c r="Q177" s="40"/>
       <c r="R177" s="40"/>
     </row>
-    <row r="178" spans="1:18" hidden="1">
+    <row r="178" spans="1:18">
       <c r="A178" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-13</v>
@@ -19209,7 +19209,7 @@
       <c r="Q181" s="42"/>
       <c r="R181" s="42"/>
     </row>
-    <row r="182" spans="1:18" hidden="1">
+    <row r="182" spans="1:18">
       <c r="A182" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-14</v>
@@ -19241,7 +19241,7 @@
       <c r="Q182" s="40"/>
       <c r="R182" s="40"/>
     </row>
-    <row r="183" spans="1:18" hidden="1">
+    <row r="183" spans="1:18">
       <c r="A183" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-15</v>
@@ -19419,7 +19419,7 @@
       <c r="Q187" s="42"/>
       <c r="R187" s="42"/>
     </row>
-    <row r="188" spans="1:18" hidden="1">
+    <row r="188" spans="1:18">
       <c r="A188" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-16</v>
@@ -19451,7 +19451,7 @@
       <c r="Q188" s="40"/>
       <c r="R188" s="40"/>
     </row>
-    <row r="189" spans="1:18" hidden="1">
+    <row r="189" spans="1:18">
       <c r="A189" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-17</v>
@@ -21291,7 +21291,7 @@
       <c r="Q242" s="42"/>
       <c r="R242" s="42"/>
     </row>
-    <row r="243" spans="1:18">
+    <row r="243" spans="1:18" hidden="1">
       <c r="A243" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-1</v>
@@ -21363,7 +21363,7 @@
       <c r="Q244" s="40"/>
       <c r="R244" s="40"/>
     </row>
-    <row r="245" spans="1:18">
+    <row r="245" spans="1:18" hidden="1">
       <c r="A245" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-2</v>
@@ -21435,7 +21435,7 @@
       <c r="Q246" s="40"/>
       <c r="R246" s="40"/>
     </row>
-    <row r="247" spans="1:18">
+    <row r="247" spans="1:18" hidden="1">
       <c r="A247" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-3</v>
@@ -21507,7 +21507,7 @@
       <c r="Q248" s="40"/>
       <c r="R248" s="40"/>
     </row>
-    <row r="249" spans="1:18">
+    <row r="249" spans="1:18" hidden="1">
       <c r="A249" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-4</v>
@@ -21579,7 +21579,7 @@
       <c r="Q250" s="40"/>
       <c r="R250" s="40"/>
     </row>
-    <row r="251" spans="1:18">
+    <row r="251" spans="1:18" hidden="1">
       <c r="A251" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-5</v>
@@ -21651,7 +21651,7 @@
       <c r="Q252" s="40"/>
       <c r="R252" s="40"/>
     </row>
-    <row r="253" spans="1:18">
+    <row r="253" spans="1:18" hidden="1">
       <c r="A253" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-6</v>
@@ -21723,7 +21723,7 @@
       <c r="Q254" s="40"/>
       <c r="R254" s="40"/>
     </row>
-    <row r="255" spans="1:18">
+    <row r="255" spans="1:18" hidden="1">
       <c r="A255" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-7</v>
@@ -21795,7 +21795,7 @@
       <c r="Q256" s="40"/>
       <c r="R256" s="40"/>
     </row>
-    <row r="257" spans="1:18">
+    <row r="257" spans="1:18" hidden="1">
       <c r="A257" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-8</v>
@@ -21867,7 +21867,7 @@
       <c r="Q258" s="40"/>
       <c r="R258" s="40"/>
     </row>
-    <row r="259" spans="1:18">
+    <row r="259" spans="1:18" hidden="1">
       <c r="A259" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-9</v>
@@ -21939,7 +21939,7 @@
       <c r="Q260" s="40"/>
       <c r="R260" s="40"/>
     </row>
-    <row r="261" spans="1:18">
+    <row r="261" spans="1:18" hidden="1">
       <c r="A261" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-10</v>
@@ -22117,7 +22117,7 @@
       <c r="Q265" s="40"/>
       <c r="R265" s="40"/>
     </row>
-    <row r="266" spans="1:18">
+    <row r="266" spans="1:18" hidden="1">
       <c r="A266" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-11</v>
@@ -22153,7 +22153,7 @@
       <c r="Q266" s="42"/>
       <c r="R266" s="42"/>
     </row>
-    <row r="267" spans="1:18">
+    <row r="267" spans="1:18" hidden="1">
       <c r="A267" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-12</v>
@@ -22189,7 +22189,7 @@
       <c r="Q267" s="42"/>
       <c r="R267" s="42"/>
     </row>
-    <row r="268" spans="1:18">
+    <row r="268" spans="1:18" hidden="1">
       <c r="A268" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-13</v>
@@ -22225,7 +22225,7 @@
       <c r="Q268" s="42"/>
       <c r="R268" s="42"/>
     </row>
-    <row r="269" spans="1:18" s="16" customFormat="1">
+    <row r="269" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A269" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-14</v>
@@ -22425,7 +22425,7 @@
       <c r="Q274" s="42"/>
       <c r="R274" s="42"/>
     </row>
-    <row r="275" spans="1:18" s="16" customFormat="1">
+    <row r="275" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A275" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-15</v>
@@ -22635,7 +22635,7 @@
       <c r="Q280" s="42"/>
       <c r="R280" s="42"/>
     </row>
-    <row r="281" spans="1:18">
+    <row r="281" spans="1:18" hidden="1">
       <c r="A281" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-16</v>
@@ -22739,7 +22739,7 @@
       <c r="Q283" s="42"/>
       <c r="R283" s="42"/>
     </row>
-    <row r="284" spans="1:18">
+    <row r="284" spans="1:18" hidden="1">
       <c r="A284" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-17</v>
@@ -22843,7 +22843,7 @@
       <c r="Q286" s="40"/>
       <c r="R286" s="40"/>
     </row>
-    <row r="287" spans="1:18">
+    <row r="287" spans="1:18" hidden="1">
       <c r="A287" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-18</v>
@@ -22947,7 +22947,7 @@
       <c r="Q289" s="40"/>
       <c r="R289" s="40"/>
     </row>
-    <row r="290" spans="1:18">
+    <row r="290" spans="1:18" hidden="1">
       <c r="A290" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-19</v>
@@ -23051,7 +23051,7 @@
       <c r="Q292" s="40"/>
       <c r="R292" s="40"/>
     </row>
-    <row r="293" spans="1:18">
+    <row r="293" spans="1:18" hidden="1">
       <c r="A293" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-20</v>
@@ -23155,7 +23155,7 @@
       <c r="Q295" s="40"/>
       <c r="R295" s="40"/>
     </row>
-    <row r="296" spans="1:18">
+    <row r="296" spans="1:18" hidden="1">
       <c r="A296" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-21</v>
@@ -23499,7 +23499,7 @@
       <c r="Q305" s="40"/>
       <c r="R305" s="40"/>
     </row>
-    <row r="306" spans="1:18">
+    <row r="306" spans="1:18" hidden="1">
       <c r="A306" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-22</v>
@@ -23601,7 +23601,7 @@
       <c r="Q308" s="40"/>
       <c r="R308" s="40"/>
     </row>
-    <row r="309" spans="1:18">
+    <row r="309" spans="1:18" hidden="1">
       <c r="A309" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-23</v>
@@ -23705,7 +23705,7 @@
       <c r="Q311" s="40"/>
       <c r="R311" s="40"/>
     </row>
-    <row r="312" spans="1:18">
+    <row r="312" spans="1:18" hidden="1">
       <c r="A312" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-24</v>
@@ -23809,7 +23809,7 @@
       <c r="Q314" s="42"/>
       <c r="R314" s="42"/>
     </row>
-    <row r="315" spans="1:18" s="16" customFormat="1">
+    <row r="315" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A315" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-25</v>
@@ -23913,7 +23913,7 @@
       <c r="Q317" s="40"/>
       <c r="R317" s="40"/>
     </row>
-    <row r="318" spans="1:18">
+    <row r="318" spans="1:18" hidden="1">
       <c r="A318" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-26</v>
@@ -24055,7 +24055,7 @@
       <c r="Q321" s="40"/>
       <c r="R321" s="40"/>
     </row>
-    <row r="322" spans="1:18">
+    <row r="322" spans="1:18" hidden="1">
       <c r="A322" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-27</v>
@@ -24223,7 +24223,7 @@
       <c r="Q326" s="42"/>
       <c r="R326" s="42"/>
     </row>
-    <row r="327" spans="1:18">
+    <row r="327" spans="1:18" hidden="1">
       <c r="A327" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-28</v>
@@ -24322,6 +24322,42 @@
       <c r="P329" s="42"/>
       <c r="Q329" s="42"/>
       <c r="R329" s="42"/>
+    </row>
+    <row r="330" spans="1:18" hidden="1">
+      <c r="A330" s="41" t="str">
+        <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
+        <v>Field Options-4</v>
+      </c>
+      <c r="B330" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="C330" s="41">
+        <f>IF(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])=1,0,IF(ISNUMBER(VLOOKUP([Table Name],SeedMap[],6,0)),COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])+VLOOKUP([Table Name],SeedMap[],6,0)-1,COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1))</f>
+        <v>504</v>
+      </c>
+      <c r="D330" s="42">
+        <v>511</v>
+      </c>
+      <c r="E330" s="42" t="s">
+        <v>495</v>
+      </c>
+      <c r="F330" s="42"/>
+      <c r="G330" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H330" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="I330" s="42"/>
+      <c r="J330" s="42"/>
+      <c r="K330" s="42"/>
+      <c r="L330" s="42"/>
+      <c r="M330" s="42"/>
+      <c r="N330" s="42"/>
+      <c r="O330" s="42"/>
+      <c r="P330" s="42"/>
+      <c r="Q330" s="42"/>
+      <c r="R330" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25595,8 +25631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:R38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25606,14 +25642,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="50" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceActionMethod::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldOption::query()</v>
       </c>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
@@ -25761,7 +25797,7 @@
       </c>
       <c r="D5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>resource_action</v>
+        <v>form_field</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
@@ -25769,27 +25805,27 @@
       </c>
       <c r="F5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>method</v>
+        <v>detail</v>
       </c>
       <c r="G5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>idn1</v>
+        <v>value_attr</v>
       </c>
       <c r="H5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>idn2</v>
+        <v>label_attr</v>
       </c>
       <c r="I5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>idn3</v>
+        <v>preload</v>
       </c>
       <c r="J5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v>idn4</v>
+        <v/>
       </c>
       <c r="K5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>
-        <v>idn5</v>
+        <v/>
       </c>
       <c r="L5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0))</f>
@@ -25871,7 +25907,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="48" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceActionMethod::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldOption::query()</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -25904,11 +25940,11 @@
       </c>
       <c r="D9" s="22" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource_action' =&gt; '501', </v>
+        <v xml:space="preserve">'form_field' =&gt; '504', </v>
       </c>
       <c r="E9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'List', </v>
+        <v xml:space="preserve">'type' =&gt; 'enum', </v>
       </c>
       <c r="F9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25916,7 +25952,7 @@
       </c>
       <c r="G9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '501', </v>
+        <v/>
       </c>
       <c r="H9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25977,11 +26013,11 @@
       </c>
       <c r="D10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '502', </v>
+        <v xml:space="preserve">'form_field' =&gt; '505', </v>
       </c>
       <c r="E10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'List', </v>
+        <v xml:space="preserve">'type' =&gt; 'enum', </v>
       </c>
       <c r="F10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25989,7 +26025,7 @@
       </c>
       <c r="G10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '502', </v>
+        <v/>
       </c>
       <c r="H10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26050,11 +26086,11 @@
       </c>
       <c r="D11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '503', </v>
+        <v xml:space="preserve">'form_field' =&gt; '515', </v>
       </c>
       <c r="E11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'List', </v>
+        <v xml:space="preserve">'type' =&gt; 'Foreign', </v>
       </c>
       <c r="F11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26062,11 +26098,11 @@
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '503', </v>
+        <v xml:space="preserve">'value_attr' =&gt; 'id', </v>
       </c>
       <c r="H11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'label_attr' =&gt; 'name', </v>
       </c>
       <c r="I11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26123,11 +26159,11 @@
       </c>
       <c r="D12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '504', </v>
+        <v xml:space="preserve">'form_field' =&gt; '511', </v>
       </c>
       <c r="E12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'List', </v>
+        <v xml:space="preserve">'type' =&gt; 'Foreign', </v>
       </c>
       <c r="F12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26135,11 +26171,11 @@
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '504', </v>
+        <v xml:space="preserve">'value_attr' =&gt; 'id', </v>
       </c>
       <c r="H12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'label_attr' =&gt; 'name', </v>
       </c>
       <c r="I12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26188,19 +26224,19 @@
       </c>
       <c r="B13" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v>;</v>
       </c>
       <c r="C13" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '505', </v>
+        <v/>
       </c>
       <c r="D13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '505', </v>
+        <v/>
       </c>
       <c r="E13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'List', </v>
+        <v/>
       </c>
       <c r="F13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26208,7 +26244,7 @@
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '505', </v>
+        <v/>
       </c>
       <c r="H13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26252,7 +26288,7 @@
       </c>
       <c r="R13" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -26261,19 +26297,19 @@
       </c>
       <c r="B14" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C14" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '506', </v>
+        <v/>
       </c>
       <c r="D14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '506', </v>
+        <v/>
       </c>
       <c r="E14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'List', </v>
+        <v/>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26281,7 +26317,7 @@
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '506', </v>
+        <v/>
       </c>
       <c r="H14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26325,7 +26361,7 @@
       </c>
       <c r="R14" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -26334,19 +26370,19 @@
       </c>
       <c r="B15" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C15" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '507', </v>
+        <v/>
       </c>
       <c r="D15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '507', </v>
+        <v/>
       </c>
       <c r="E15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'Form', </v>
+        <v/>
       </c>
       <c r="F15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26354,7 +26390,7 @@
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '503', </v>
+        <v/>
       </c>
       <c r="H15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26398,7 +26434,7 @@
       </c>
       <c r="R15" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -26407,19 +26443,19 @@
       </c>
       <c r="B16" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C16" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '508', </v>
+        <v/>
       </c>
       <c r="D16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '508', </v>
+        <v/>
       </c>
       <c r="E16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'List', </v>
+        <v/>
       </c>
       <c r="F16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26427,7 +26463,7 @@
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '507', </v>
+        <v/>
       </c>
       <c r="H16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26471,7 +26507,7 @@
       </c>
       <c r="R16" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -26480,19 +26516,19 @@
       </c>
       <c r="B17" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C17" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '509', </v>
+        <v/>
       </c>
       <c r="D17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '509', </v>
+        <v/>
       </c>
       <c r="E17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'Form', </v>
+        <v/>
       </c>
       <c r="F17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26500,7 +26536,7 @@
       </c>
       <c r="G17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '504', </v>
+        <v/>
       </c>
       <c r="H17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26544,7 +26580,7 @@
       </c>
       <c r="R17" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -26553,19 +26589,19 @@
       </c>
       <c r="B18" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C18" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '510', </v>
+        <v/>
       </c>
       <c r="D18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '510', </v>
+        <v/>
       </c>
       <c r="E18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'List', </v>
+        <v/>
       </c>
       <c r="F18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26573,7 +26609,7 @@
       </c>
       <c r="G18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '508', </v>
+        <v/>
       </c>
       <c r="H18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26617,7 +26653,7 @@
       </c>
       <c r="R18" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -26626,19 +26662,19 @@
       </c>
       <c r="B19" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C19" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '511', </v>
+        <v/>
       </c>
       <c r="D19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '511', </v>
+        <v/>
       </c>
       <c r="E19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26646,11 +26682,11 @@
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '501', </v>
+        <v/>
       </c>
       <c r="H19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn2' =&gt; '505', </v>
+        <v/>
       </c>
       <c r="I19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26690,7 +26726,7 @@
       </c>
       <c r="R19" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -26699,19 +26735,19 @@
       </c>
       <c r="B20" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C20" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '512', </v>
+        <v/>
       </c>
       <c r="D20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '512', </v>
+        <v/>
       </c>
       <c r="E20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26719,11 +26755,11 @@
       </c>
       <c r="G20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '502', </v>
+        <v/>
       </c>
       <c r="H20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn2' =&gt; '505', </v>
+        <v/>
       </c>
       <c r="I20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26763,7 +26799,7 @@
       </c>
       <c r="R20" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -26772,19 +26808,19 @@
       </c>
       <c r="B21" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C21" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '513', </v>
+        <v/>
       </c>
       <c r="D21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '513', </v>
+        <v/>
       </c>
       <c r="E21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26792,11 +26828,11 @@
       </c>
       <c r="G21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '503', </v>
+        <v/>
       </c>
       <c r="H21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn2' =&gt; '505', </v>
+        <v/>
       </c>
       <c r="I21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26836,7 +26872,7 @@
       </c>
       <c r="R21" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -26845,19 +26881,19 @@
       </c>
       <c r="B22" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C22" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '514', </v>
+        <v/>
       </c>
       <c r="D22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '514', </v>
+        <v/>
       </c>
       <c r="E22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26865,11 +26901,11 @@
       </c>
       <c r="G22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '504', </v>
+        <v/>
       </c>
       <c r="H22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn2' =&gt; '505', </v>
+        <v/>
       </c>
       <c r="I22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26909,7 +26945,7 @@
       </c>
       <c r="R22" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -26918,19 +26954,19 @@
       </c>
       <c r="B23" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C23" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '515', </v>
+        <v/>
       </c>
       <c r="D23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '515', </v>
+        <v/>
       </c>
       <c r="E23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'AddRelation', </v>
+        <v/>
       </c>
       <c r="F23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26938,11 +26974,11 @@
       </c>
       <c r="G23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '509', </v>
+        <v/>
       </c>
       <c r="H23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn2' =&gt; '501', </v>
+        <v/>
       </c>
       <c r="I23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26982,7 +27018,7 @@
       </c>
       <c r="R23" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -26991,19 +27027,19 @@
       </c>
       <c r="B24" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C24" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '516', </v>
+        <v/>
       </c>
       <c r="D24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_action' =&gt; '516', </v>
+        <v/>
       </c>
       <c r="E24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27011,11 +27047,11 @@
       </c>
       <c r="G24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn1' =&gt; '509', </v>
+        <v/>
       </c>
       <c r="H24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'idn2' =&gt; '510', </v>
+        <v/>
       </c>
       <c r="I24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27055,7 +27091,7 @@
       </c>
       <c r="R24" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -27064,19 +27100,19 @@
       </c>
       <c r="B25" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '517', </v>
+        <v/>
       </c>
       <c r="D25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '517', </v>
+        <v/>
       </c>
       <c r="E25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'FormWithData', </v>
+        <v/>
       </c>
       <c r="F25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27084,11 +27120,11 @@
       </c>
       <c r="G25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '502', </v>
+        <v/>
       </c>
       <c r="H25" s="22" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'idn2' =&gt; '502', </v>
+        <v/>
       </c>
       <c r="I25" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27128,7 +27164,7 @@
       </c>
       <c r="R25" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -27137,19 +27173,19 @@
       </c>
       <c r="B26" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '518', </v>
+        <v/>
       </c>
       <c r="D26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '518', </v>
+        <v/>
       </c>
       <c r="E26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27157,11 +27193,11 @@
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '511', </v>
+        <v/>
       </c>
       <c r="H26" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'idn2' =&gt; '507', </v>
+        <v/>
       </c>
       <c r="I26" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27201,7 +27237,7 @@
       </c>
       <c r="R26" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -27210,19 +27246,19 @@
       </c>
       <c r="B27" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '519', </v>
+        <v/>
       </c>
       <c r="D27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '519', </v>
+        <v/>
       </c>
       <c r="E27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27230,11 +27266,11 @@
       </c>
       <c r="G27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '512', </v>
+        <v/>
       </c>
       <c r="H27" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'idn2' =&gt; '507', </v>
+        <v/>
       </c>
       <c r="I27" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27274,7 +27310,7 @@
       </c>
       <c r="R27" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -27283,19 +27319,19 @@
       </c>
       <c r="B28" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '520', </v>
+        <v/>
       </c>
       <c r="D28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '520', </v>
+        <v/>
       </c>
       <c r="E28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27303,11 +27339,11 @@
       </c>
       <c r="G28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '515', </v>
+        <v/>
       </c>
       <c r="H28" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'idn2' =&gt; '506', </v>
+        <v/>
       </c>
       <c r="I28" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27347,7 +27383,7 @@
       </c>
       <c r="R28" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -27356,19 +27392,19 @@
       </c>
       <c r="B29" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '521', </v>
+        <v/>
       </c>
       <c r="D29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '521', </v>
+        <v/>
       </c>
       <c r="E29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27376,11 +27412,11 @@
       </c>
       <c r="G29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '517', </v>
+        <v/>
       </c>
       <c r="H29" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'idn2' =&gt; '511', </v>
+        <v/>
       </c>
       <c r="I29" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27420,7 +27456,7 @@
       </c>
       <c r="R29" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -27429,19 +27465,19 @@
       </c>
       <c r="B30" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '522', </v>
+        <v/>
       </c>
       <c r="D30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '522', </v>
+        <v/>
       </c>
       <c r="E30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'Data', </v>
+        <v/>
       </c>
       <c r="F30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27449,7 +27485,7 @@
       </c>
       <c r="G30" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '501', </v>
+        <v/>
       </c>
       <c r="H30" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27493,7 +27529,7 @@
       </c>
       <c r="R30" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -27502,19 +27538,19 @@
       </c>
       <c r="B31" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '523', </v>
+        <v/>
       </c>
       <c r="D31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '523', </v>
+        <v/>
       </c>
       <c r="E31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'ListRelation', </v>
+        <v/>
       </c>
       <c r="F31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27522,11 +27558,11 @@
       </c>
       <c r="G31" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '516', </v>
+        <v/>
       </c>
       <c r="H31" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'idn2' =&gt; '509', </v>
+        <v/>
       </c>
       <c r="I31" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27566,7 +27602,7 @@
       </c>
       <c r="R31" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -27575,19 +27611,19 @@
       </c>
       <c r="B32" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '524', </v>
+        <v/>
       </c>
       <c r="D32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '524', </v>
+        <v/>
       </c>
       <c r="E32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'ManageRelation', </v>
+        <v/>
       </c>
       <c r="F32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27595,11 +27631,11 @@
       </c>
       <c r="G32" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '518', </v>
+        <v/>
       </c>
       <c r="H32" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'idn2' =&gt; '505', </v>
+        <v/>
       </c>
       <c r="I32" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27639,7 +27675,7 @@
       </c>
       <c r="R32" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -27648,19 +27684,19 @@
       </c>
       <c r="B33" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '525', </v>
+        <v/>
       </c>
       <c r="D33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '525', </v>
+        <v/>
       </c>
       <c r="E33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'AddRelation', </v>
+        <v/>
       </c>
       <c r="F33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27668,11 +27704,11 @@
       </c>
       <c r="G33" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '528', </v>
+        <v/>
       </c>
       <c r="H33" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'idn2' =&gt; '506', </v>
+        <v/>
       </c>
       <c r="I33" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27712,7 +27748,7 @@
       </c>
       <c r="R33" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -27721,19 +27757,19 @@
       </c>
       <c r="B34" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '526', </v>
+        <v/>
       </c>
       <c r="D34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '526', </v>
+        <v/>
       </c>
       <c r="E34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'Data', </v>
+        <v/>
       </c>
       <c r="F34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27741,7 +27777,7 @@
       </c>
       <c r="G34" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '503', </v>
+        <v/>
       </c>
       <c r="H34" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27785,7 +27821,7 @@
       </c>
       <c r="R34" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -27794,19 +27830,19 @@
       </c>
       <c r="B35" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '527', </v>
+        <v/>
       </c>
       <c r="D35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '527', </v>
+        <v/>
       </c>
       <c r="E35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'FormWithData', </v>
+        <v/>
       </c>
       <c r="F35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27814,11 +27850,11 @@
       </c>
       <c r="G35" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '505', </v>
+        <v/>
       </c>
       <c r="H35" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'idn2' =&gt; '503', </v>
+        <v/>
       </c>
       <c r="I35" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27858,7 +27894,7 @@
       </c>
       <c r="R35" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -27867,19 +27903,19 @@
       </c>
       <c r="B36" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '528', </v>
+        <v/>
       </c>
       <c r="D36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource_action' =&gt; '528', </v>
+        <v/>
       </c>
       <c r="E36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'AddRelation', </v>
+        <v/>
       </c>
       <c r="F36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27887,11 +27923,11 @@
       </c>
       <c r="G36" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'idn1' =&gt; '516', </v>
+        <v/>
       </c>
       <c r="H36" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'idn2' =&gt; '507', </v>
+        <v/>
       </c>
       <c r="I36" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -27931,7 +27967,7 @@
       </c>
       <c r="R36" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -27940,7 +27976,7 @@
       </c>
       <c r="B37" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v/>
       </c>
       <c r="C37" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -28013,7 +28049,7 @@
       </c>
       <c r="B38" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v/>
       </c>
       <c r="C38" s="22" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Field data changed to products from items for wishlist products
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tables" sheetId="1" r:id="rId1"/>
@@ -12539,8 +12539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F173" sqref="F173"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18910,7 +18910,7 @@
         <v>239</v>
       </c>
       <c r="F173" s="42">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="G173" s="42"/>
       <c r="H173" s="42"/>
@@ -25631,8 +25631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T208"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25642,14 +25642,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="50" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldOption::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldData::query()</v>
       </c>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
@@ -25801,23 +25801,23 @@
       </c>
       <c r="E5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>type</v>
+        <v>attribute</v>
       </c>
       <c r="F5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>detail</v>
+        <v>relation</v>
       </c>
       <c r="G5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>value_attr</v>
+        <v>nest_relation1</v>
       </c>
       <c r="H5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>label_attr</v>
+        <v>nest_relation2</v>
       </c>
       <c r="I5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>preload</v>
+        <v>nest_relation3</v>
       </c>
       <c r="J5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
@@ -25907,7 +25907,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="48" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldOption::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldData::query()</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -25940,11 +25940,11 @@
       </c>
       <c r="D9" s="22" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'form_field' =&gt; '504', </v>
+        <v xml:space="preserve">'form_field' =&gt; '501', </v>
       </c>
       <c r="E9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'enum', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'product', </v>
       </c>
       <c r="F9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26013,11 +26013,11 @@
       </c>
       <c r="D10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '505', </v>
+        <v xml:space="preserve">'form_field' =&gt; '502', </v>
       </c>
       <c r="E10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'enum', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="F10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26086,11 +26086,11 @@
       </c>
       <c r="D11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '515', </v>
+        <v xml:space="preserve">'form_field' =&gt; '503', </v>
       </c>
       <c r="E11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'Foreign', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'image', </v>
       </c>
       <c r="F11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26098,11 +26098,11 @@
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'value_attr' =&gt; 'id', </v>
+        <v/>
       </c>
       <c r="H11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'label_attr' =&gt; 'name', </v>
+        <v/>
       </c>
       <c r="I11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26159,11 +26159,11 @@
       </c>
       <c r="D12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '511', </v>
+        <v xml:space="preserve">'form_field' =&gt; '504', </v>
       </c>
       <c r="E12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'Foreign', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'default', </v>
       </c>
       <c r="F12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26171,11 +26171,11 @@
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'value_attr' =&gt; 'id', </v>
+        <v/>
       </c>
       <c r="H12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'label_attr' =&gt; 'name', </v>
+        <v/>
       </c>
       <c r="I12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26224,19 +26224,19 @@
       </c>
       <c r="B13" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C13" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '505', </v>
       </c>
       <c r="D13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '505', </v>
       </c>
       <c r="E13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'status', </v>
       </c>
       <c r="F13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26288,7 +26288,7 @@
       </c>
       <c r="R13" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -26297,19 +26297,19 @@
       </c>
       <c r="B14" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C14" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '506', </v>
       </c>
       <c r="D14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '506', </v>
       </c>
       <c r="E14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26361,7 +26361,7 @@
       </c>
       <c r="R14" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -26370,19 +26370,19 @@
       </c>
       <c r="B15" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C15" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '507', </v>
       </c>
       <c r="D15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '507', </v>
       </c>
       <c r="E15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'email', </v>
       </c>
       <c r="F15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26434,7 +26434,7 @@
       </c>
       <c r="R15" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -26443,19 +26443,19 @@
       </c>
       <c r="B16" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C16" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '508', </v>
       </c>
       <c r="D16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '508', </v>
       </c>
       <c r="E16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'number', </v>
       </c>
       <c r="F16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26507,7 +26507,7 @@
       </c>
       <c r="R16" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -26516,19 +26516,19 @@
       </c>
       <c r="B17" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C17" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '509', </v>
       </c>
       <c r="D17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '509', </v>
       </c>
       <c r="E17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="F17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26580,7 +26580,7 @@
       </c>
       <c r="R17" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -26589,19 +26589,19 @@
       </c>
       <c r="B18" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C18" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '510', </v>
       </c>
       <c r="D18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '510', </v>
       </c>
       <c r="E18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'description', </v>
       </c>
       <c r="F18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26653,7 +26653,7 @@
       </c>
       <c r="R18" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -26662,23 +26662,23 @@
       </c>
       <c r="B19" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C19" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '511', </v>
       </c>
       <c r="D19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '511', </v>
       </c>
       <c r="E19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'product', </v>
       </c>
       <c r="F19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relation' =&gt; '518', </v>
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26726,7 +26726,7 @@
       </c>
       <c r="R19" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -26735,19 +26735,19 @@
       </c>
       <c r="B20" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C20" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '512', </v>
       </c>
       <c r="D20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '512', </v>
       </c>
       <c r="E20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="F20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26799,7 +26799,7 @@
       </c>
       <c r="R20" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -26808,19 +26808,19 @@
       </c>
       <c r="B21" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C21" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '513', </v>
       </c>
       <c r="D21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '513', </v>
       </c>
       <c r="E21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'description', </v>
       </c>
       <c r="F21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26872,7 +26872,7 @@
       </c>
       <c r="R21" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -26881,19 +26881,19 @@
       </c>
       <c r="B22" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C22" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '514', </v>
       </c>
       <c r="D22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '514', </v>
       </c>
       <c r="E22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'wishlist', </v>
       </c>
       <c r="F22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26945,7 +26945,7 @@
       </c>
       <c r="R22" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -26954,19 +26954,19 @@
       </c>
       <c r="B23" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C23" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '515', </v>
       </c>
       <c r="D23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '515', </v>
       </c>
       <c r="E23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'visitor', </v>
       </c>
       <c r="F23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27018,7 +27018,7 @@
       </c>
       <c r="R23" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -27027,19 +27027,19 @@
       </c>
       <c r="B24" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C24" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '516', </v>
       </c>
       <c r="D24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '516', </v>
       </c>
       <c r="E24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'wishlist', </v>
       </c>
       <c r="F24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27091,7 +27091,7 @@
       </c>
       <c r="R24" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -27100,19 +27100,19 @@
       </c>
       <c r="B25" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'id' =&gt; '517', </v>
       </c>
       <c r="D25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'form_field' =&gt; '517', </v>
       </c>
       <c r="E25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'attribute' =&gt; 'note', </v>
       </c>
       <c r="F25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27164,7 +27164,7 @@
       </c>
       <c r="R25" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -27173,7 +27173,7 @@
       </c>
       <c r="B26" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27246,7 +27246,7 @@
       </c>
       <c r="B27" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Listing column added to item group master for web listing
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2057" uniqueCount="606">
   <si>
     <t>Name</t>
   </si>
@@ -1848,6 +1848,9 @@
   </si>
   <si>
     <t>Add/Remove Products</t>
+  </si>
+  <si>
+    <t>list</t>
   </si>
 </sst>
 </file>
@@ -2068,7 +2071,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="64">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2975,37 +2990,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J54" totalsRowShown="0" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J54" totalsRowShown="0" dataDxfId="63">
   <autoFilter ref="A1:J54">
     <filterColumn colId="3"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="61"/>
-    <tableColumn id="10" name="Table" dataDxfId="60">
+    <tableColumn id="2" name="Name" dataDxfId="62"/>
+    <tableColumn id="10" name="Table" dataDxfId="61">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="59">
+    <tableColumn id="5" name="Singular Name" dataDxfId="60">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="58">
+    <tableColumn id="8" name="Model NS" dataDxfId="59">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="57">
+    <tableColumn id="4" name="Class Name" dataDxfId="58">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="56">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="57">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="55">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="56">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="54">
+    <tableColumn id="3" name="Model Statement" dataDxfId="55">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="53">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="54">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="52">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="53">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3014,56 +3029,60 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I81" totalsRowShown="0" dataDxfId="50">
-  <autoFilter ref="A1:I81"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I82" totalsRowShown="0" dataDxfId="51">
+  <autoFilter ref="A1:I82"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="49"/>
-    <tableColumn id="2" name="Type" dataDxfId="48"/>
-    <tableColumn id="3" name="Name" dataDxfId="47"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="46"/>
-    <tableColumn id="5" name="Method1" dataDxfId="45"/>
-    <tableColumn id="6" name="Method2" dataDxfId="44"/>
-    <tableColumn id="7" name="Method3" dataDxfId="43"/>
-    <tableColumn id="8" name="Method4" dataDxfId="42"/>
-    <tableColumn id="9" name="Method5" dataDxfId="41"/>
+    <tableColumn id="1" name="Column" dataDxfId="50"/>
+    <tableColumn id="2" name="Type" dataDxfId="49"/>
+    <tableColumn id="3" name="Name" dataDxfId="48"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="47"/>
+    <tableColumn id="5" name="Method1" dataDxfId="46"/>
+    <tableColumn id="6" name="Method2" dataDxfId="45"/>
+    <tableColumn id="7" name="Method3" dataDxfId="44"/>
+    <tableColumn id="8" name="Method4" dataDxfId="43"/>
+    <tableColumn id="9" name="Method5" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K113" totalsRowShown="0" dataDxfId="40">
-  <autoFilter ref="A1:K113">
-    <filterColumn colId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K114" totalsRowShown="0" dataDxfId="41">
+  <autoFilter ref="A1:K114">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="item_group_master"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="39"/>
-    <tableColumn id="3" name="Field" dataDxfId="38"/>
-    <tableColumn id="5" name="Type" dataDxfId="37">
+    <tableColumn id="2" name="Table" dataDxfId="40"/>
+    <tableColumn id="3" name="Field" dataDxfId="39"/>
+    <tableColumn id="5" name="Type" dataDxfId="38">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="36">
+    <tableColumn id="4" name="Name" dataDxfId="37">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="35">
+    <tableColumn id="6" name="Arg2" dataDxfId="36">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="34">
+    <tableColumn id="7" name="Method1" dataDxfId="35">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="33">
+    <tableColumn id="8" name="Method2" dataDxfId="34">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="32">
+    <tableColumn id="9" name="Method3" dataDxfId="33">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="31">
+    <tableColumn id="10" name="Method4" dataDxfId="32">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="30">
+    <tableColumn id="11" name="Method5" dataDxfId="31">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="29">
+    <tableColumn id="12" name="Statement" dataDxfId="30">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3072,7 +3091,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R330" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R330" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:R330">
     <filterColumn colId="1">
       <filters>
@@ -3081,51 +3100,51 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="26">
+    <tableColumn id="19" name="TRCode" dataDxfId="27">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="25"/>
-    <tableColumn id="2" name="Record No" dataDxfId="24">
+    <tableColumn id="1" name="Table Name" dataDxfId="26"/>
+    <tableColumn id="2" name="Record No" dataDxfId="25">
       <calculatedColumnFormula>IF(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])=1,0,IF(ISNUMBER(VLOOKUP([Table Name],SeedMap[],6,0)),COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])+VLOOKUP([Table Name],SeedMap[],6,0)-1,COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="23"/>
-    <tableColumn id="4" name="2" dataDxfId="22"/>
-    <tableColumn id="5" name="3" dataDxfId="21"/>
-    <tableColumn id="6" name="4" dataDxfId="20"/>
-    <tableColumn id="7" name="5" dataDxfId="19"/>
-    <tableColumn id="8" name="6" dataDxfId="18"/>
-    <tableColumn id="9" name="7" dataDxfId="17"/>
-    <tableColumn id="10" name="8" dataDxfId="16"/>
-    <tableColumn id="11" name="9" dataDxfId="15"/>
-    <tableColumn id="12" name="10" dataDxfId="14"/>
-    <tableColumn id="13" name="11" dataDxfId="13"/>
-    <tableColumn id="14" name="12" dataDxfId="12"/>
-    <tableColumn id="15" name="13" dataDxfId="11"/>
-    <tableColumn id="16" name="14" dataDxfId="10"/>
-    <tableColumn id="17" name="15" dataDxfId="9"/>
+    <tableColumn id="3" name="1" dataDxfId="24"/>
+    <tableColumn id="4" name="2" dataDxfId="23"/>
+    <tableColumn id="5" name="3" dataDxfId="22"/>
+    <tableColumn id="6" name="4" dataDxfId="21"/>
+    <tableColumn id="7" name="5" dataDxfId="20"/>
+    <tableColumn id="8" name="6" dataDxfId="19"/>
+    <tableColumn id="9" name="7" dataDxfId="18"/>
+    <tableColumn id="10" name="8" dataDxfId="17"/>
+    <tableColumn id="11" name="9" dataDxfId="16"/>
+    <tableColumn id="12" name="10" dataDxfId="15"/>
+    <tableColumn id="13" name="11" dataDxfId="14"/>
+    <tableColumn id="14" name="12" dataDxfId="13"/>
+    <tableColumn id="15" name="13" dataDxfId="12"/>
+    <tableColumn id="16" name="14" dataDxfId="11"/>
+    <tableColumn id="17" name="15" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:G49" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:G49" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="A1:G49">
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="6"/>
-    <tableColumn id="3" name="Table Name" dataDxfId="5"/>
-    <tableColumn id="20" name="NS" dataDxfId="4">
+    <tableColumn id="1" name="Name" dataDxfId="7"/>
+    <tableColumn id="3" name="Table Name" dataDxfId="6"/>
+    <tableColumn id="20" name="NS" dataDxfId="5">
       <calculatedColumnFormula>VLOOKUP([Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="3">
+    <tableColumn id="21" name="Model" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP([Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="2"/>
-    <tableColumn id="2" name="Last ID" dataDxfId="1"/>
-    <tableColumn id="5" name="AI Change Query" dataDxfId="0">
+    <tableColumn id="4" name="Query Method" dataDxfId="3"/>
+    <tableColumn id="2" name="Last ID" dataDxfId="2"/>
+    <tableColumn id="5" name="AI Change Query" dataDxfId="1">
       <calculatedColumnFormula>IF(ISNUMBER([Last ID]),"ALTER TABLE `" &amp; [Table Name] &amp; "`  AUTO_INCREMENT=" &amp; [Last ID]+1,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5653,10 +5672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -7448,9 +7467,30 @@
       <c r="H81" s="33"/>
       <c r="I81" s="33"/>
     </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="33" t="s">
+        <v>605</v>
+      </c>
+      <c r="B82" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="C82" s="33" t="s">
+        <v>605</v>
+      </c>
+      <c r="D82" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="E82" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="F82" s="33"/>
+      <c r="G82" s="33"/>
+      <c r="H82" s="33"/>
+      <c r="I82" s="33"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A81">
-    <cfRule type="duplicateValues" dxfId="51" priority="29"/>
+  <conditionalFormatting sqref="A2:A82">
+    <cfRule type="duplicateValues" dxfId="52" priority="29"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -7464,8 +7504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K361"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K100" sqref="K100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -7736,7 +7776,7 @@
         <v>364</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>235</v>
+        <v>605</v>
       </c>
       <c r="C7" s="35" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -7744,19 +7784,19 @@
       </c>
       <c r="D7" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'type'</v>
+        <v>'list'</v>
       </c>
       <c r="E7" s="36" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Public','Private'])</v>
+        <v>, ['Yes','No'])</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Public')</v>
+        <v>-&gt;default('Yes')</v>
       </c>
       <c r="G7" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H7" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -7772,7 +7812,7 @@
       </c>
       <c r="K7" s="35" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('type', ['Public','Private'])-&gt;default('Public')-&gt;index();</v>
+        <v>$table-&gt;enum('list', ['Yes','No'])-&gt;default('Yes');</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -7780,7 +7820,7 @@
         <v>364</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="C8" s="35" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -7788,15 +7828,15 @@
       </c>
       <c r="D8" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'status'</v>
+        <v>'type'</v>
       </c>
       <c r="E8" s="36" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Active','Inactive'])</v>
+        <v>, ['Public','Private'])</v>
       </c>
       <c r="F8" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Active')</v>
+        <v>-&gt;default('Public')</v>
       </c>
       <c r="G8" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -7816,7 +7856,7 @@
       </c>
       <c r="K8" s="35" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+        <v>$table-&gt;enum('type', ['Public','Private'])-&gt;default('Public')-&gt;index();</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -7824,27 +7864,27 @@
         <v>364</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="C9" s="35" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D9" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'status'</v>
       </c>
       <c r="E9" s="36" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Active','Inactive'])</v>
       </c>
       <c r="F9" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('Active')</v>
       </c>
       <c r="G9" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H9" s="35" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -7860,103 +7900,103 @@
       </c>
       <c r="K9" s="35" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="35" t="s">
+        <v>364</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="35" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>timestamps(</v>
+      </c>
+      <c r="D10" s="35" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v/>
+      </c>
+      <c r="E10" s="36" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F10" s="35" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G10" s="35" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H10" s="35" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I10" s="35" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J10" s="35" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K10" s="35" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:11" hidden="1">
+      <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3" t="str">
+      <c r="C11" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
         <v>increments(</v>
       </c>
-      <c r="D10" s="3" t="str">
+      <c r="D11" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
         <v>'id'</v>
       </c>
-      <c r="E10" s="6" t="str">
+      <c r="E11" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
         <v>)</v>
       </c>
-      <c r="F10" s="3" t="str">
+      <c r="F11" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
         <v/>
       </c>
-      <c r="G10" s="3" t="str">
+      <c r="G11" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
         <v/>
       </c>
-      <c r="H10" s="3" t="str">
+      <c r="H11" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
         <v/>
       </c>
-      <c r="I10" s="3" t="str">
+      <c r="I11" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
         <v/>
       </c>
-      <c r="J10" s="3" t="str">
+      <c r="J11" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
         <v/>
       </c>
-      <c r="K10" s="3" t="str">
+      <c r="K11" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="C11" s="3" t="str">
-        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>string(</v>
-      </c>
-      <c r="D11" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'name'</v>
-      </c>
-      <c r="E11" s="6" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 64)</v>
-      </c>
-      <c r="F11" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
-      </c>
-      <c r="G11" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
-      </c>
-      <c r="H11" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
-      </c>
-      <c r="I11" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
-      </c>
-      <c r="J11" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
-        <v/>
-      </c>
-      <c r="K11" s="3" t="str">
-        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('name', 64)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" hidden="1">
       <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>229</v>
+        <v>337</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -7964,7 +8004,7 @@
       </c>
       <c r="D12" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'code'</v>
+        <v>'name'</v>
       </c>
       <c r="E12" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -7992,15 +8032,15 @@
       </c>
       <c r="K12" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('code', 64)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>$table-&gt;string('name', 64)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" hidden="1">
       <c r="A13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>95</v>
+      <c r="B13" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="C13" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8008,11 +8048,11 @@
       </c>
       <c r="D13" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'description'</v>
+        <v>'code'</v>
       </c>
       <c r="E13" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 1024)</v>
+        <v>, 64)</v>
       </c>
       <c r="F13" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -8036,15 +8076,15 @@
       </c>
       <c r="K13" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('description', 1024)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>$table-&gt;string('code', 64)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" hidden="1">
       <c r="A14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>338</v>
+      <c r="B14" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8052,11 +8092,11 @@
       </c>
       <c r="D14" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration'</v>
+        <v>'description'</v>
       </c>
       <c r="E14" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 800)</v>
+        <v>, 1024)</v>
       </c>
       <c r="F14" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -8080,15 +8120,15 @@
       </c>
       <c r="K14" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="16" customFormat="1">
+        <v>$table-&gt;string('description', 1024)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="16" customFormat="1" hidden="1">
       <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C15" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8096,7 +8136,7 @@
       </c>
       <c r="D15" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration2'</v>
+        <v>'narration'</v>
       </c>
       <c r="E15" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8124,15 +8164,15 @@
       </c>
       <c r="K15" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration2', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>$table-&gt;string('narration', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" hidden="1">
       <c r="A16" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8140,7 +8180,7 @@
       </c>
       <c r="D16" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration3'</v>
+        <v>'narration2'</v>
       </c>
       <c r="E16" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8168,15 +8208,15 @@
       </c>
       <c r="K16" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration3', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>$table-&gt;string('narration2', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" hidden="1">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C17" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8184,7 +8224,7 @@
       </c>
       <c r="D17" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration4'</v>
+        <v>'narration3'</v>
       </c>
       <c r="E17" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8212,15 +8252,15 @@
       </c>
       <c r="K17" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration4', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>$table-&gt;string('narration3', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" hidden="1">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C18" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8228,7 +8268,7 @@
       </c>
       <c r="D18" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration5'</v>
+        <v>'narration4'</v>
       </c>
       <c r="E18" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8256,15 +8296,15 @@
       </c>
       <c r="K18" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration5', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>$table-&gt;string('narration4', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" hidden="1">
       <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C19" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8272,7 +8312,7 @@
       </c>
       <c r="D19" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration6'</v>
+        <v>'narration5'</v>
       </c>
       <c r="E19" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8300,15 +8340,15 @@
       </c>
       <c r="K19" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration6', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>$table-&gt;string('narration5', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" hidden="1">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C20" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8316,7 +8356,7 @@
       </c>
       <c r="D20" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration7'</v>
+        <v>'narration6'</v>
       </c>
       <c r="E20" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8344,15 +8384,15 @@
       </c>
       <c r="K20" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration7', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>$table-&gt;string('narration6', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" hidden="1">
       <c r="A21" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C21" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8360,7 +8400,7 @@
       </c>
       <c r="D21" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration8'</v>
+        <v>'narration7'</v>
       </c>
       <c r="E21" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8388,15 +8428,15 @@
       </c>
       <c r="K21" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration8', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>$table-&gt;string('narration7', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" hidden="1">
       <c r="A22" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C22" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8404,7 +8444,7 @@
       </c>
       <c r="D22" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration9'</v>
+        <v>'narration8'</v>
       </c>
       <c r="E22" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8432,15 +8472,15 @@
       </c>
       <c r="K22" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration9', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>$table-&gt;string('narration8', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" hidden="1">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C23" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8448,7 +8488,7 @@
       </c>
       <c r="D23" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'narration10'</v>
+        <v>'narration9'</v>
       </c>
       <c r="E23" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8476,15 +8516,15 @@
       </c>
       <c r="K23" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('narration10', 800)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>$table-&gt;string('narration9', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" hidden="1">
       <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C24" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8492,11 +8532,11 @@
       </c>
       <c r="D24" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'refno'</v>
+        <v>'narration10'</v>
       </c>
       <c r="E24" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 60)</v>
+        <v>, 800)</v>
       </c>
       <c r="F24" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -8520,15 +8560,15 @@
       </c>
       <c r="K24" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('refno', 60)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>$table-&gt;string('narration10', 800)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" hidden="1">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C25" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8536,7 +8576,7 @@
       </c>
       <c r="D25" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'ref2no'</v>
+        <v>'refno'</v>
       </c>
       <c r="E25" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8564,31 +8604,31 @@
       </c>
       <c r="K25" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('ref2no', 60)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>$table-&gt;string('refno', 60)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" hidden="1">
       <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C26" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>enum(</v>
+        <v>string(</v>
       </c>
       <c r="D26" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'itemserial'</v>
+        <v>'ref2no'</v>
       </c>
       <c r="E26" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Yes','No'])</v>
+        <v>, 60)</v>
       </c>
       <c r="F26" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('No')</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G26" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -8608,103 +8648,103 @@
       </c>
       <c r="K26" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('itemserial', ['Yes','No'])-&gt;default('No');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>$table-&gt;string('ref2no', 60)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" hidden="1">
       <c r="A27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="C27" s="33" t="str">
+      <c r="B27" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C27" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
         <v>enum(</v>
       </c>
-      <c r="D27" s="33" t="str">
+      <c r="D27" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'itemserial'</v>
+      </c>
+      <c r="E27" s="6" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, ['Yes','No'])</v>
+      </c>
+      <c r="F27" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;default('No')</v>
+      </c>
+      <c r="G27" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H27" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I27" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J27" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K27" s="3" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;enum('itemserial', ['Yes','No'])-&gt;default('No');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" hidden="1">
+      <c r="A28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C28" s="33" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>enum(</v>
+      </c>
+      <c r="D28" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
         <v>'type'</v>
       </c>
-      <c r="E27" s="34" t="str">
+      <c r="E28" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
         <v>, ['Public','Protected','System'])</v>
       </c>
-      <c r="F27" s="33" t="str">
+      <c r="F28" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
         <v>-&gt;default('Public')</v>
       </c>
-      <c r="G27" s="33" t="str">
+      <c r="G28" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
         <v/>
       </c>
-      <c r="H27" s="33" t="str">
+      <c r="H28" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
         <v/>
       </c>
-      <c r="I27" s="33" t="str">
+      <c r="I28" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
         <v/>
       </c>
-      <c r="J27" s="33" t="str">
+      <c r="J28" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
         <v/>
       </c>
-      <c r="K27" s="33" t="str">
+      <c r="K28" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
         <v>$table-&gt;enum('type', ['Public','Protected','System'])-&gt;default('Public');</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="C28" s="33" t="str">
-        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
-      </c>
-      <c r="D28" s="33" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_01'</v>
-      </c>
-      <c r="E28" s="34" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
-      </c>
-      <c r="F28" s="33" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
-      </c>
-      <c r="G28" s="33" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
-      </c>
-      <c r="H28" s="33" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
-      </c>
-      <c r="I28" s="33" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
-      </c>
-      <c r="J28" s="33" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
-        <v/>
-      </c>
-      <c r="K28" s="33" t="str">
-        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_01')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" hidden="1">
       <c r="A29" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>355</v>
+      <c r="B29" s="3" t="s">
+        <v>354</v>
       </c>
       <c r="C29" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8712,7 +8752,7 @@
       </c>
       <c r="D29" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_02'</v>
+        <v>'category_01'</v>
       </c>
       <c r="E29" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8740,15 +8780,15 @@
       </c>
       <c r="K29" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_02')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>$table-&gt;unsignedInteger('category_01')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" hidden="1">
       <c r="A30" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C30" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8756,7 +8796,7 @@
       </c>
       <c r="D30" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_03'</v>
+        <v>'category_02'</v>
       </c>
       <c r="E30" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8784,15 +8824,15 @@
       </c>
       <c r="K30" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_03')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>$table-&gt;unsignedInteger('category_02')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" hidden="1">
       <c r="A31" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C31" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8800,7 +8840,7 @@
       </c>
       <c r="D31" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_04'</v>
+        <v>'category_03'</v>
       </c>
       <c r="E31" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8828,15 +8868,15 @@
       </c>
       <c r="K31" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_04')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>$table-&gt;unsignedInteger('category_03')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" hidden="1">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C32" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8844,7 +8884,7 @@
       </c>
       <c r="D32" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_05'</v>
+        <v>'category_04'</v>
       </c>
       <c r="E32" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8872,15 +8912,15 @@
       </c>
       <c r="K32" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_05')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>$table-&gt;unsignedInteger('category_04')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" hidden="1">
       <c r="A33" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C33" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8888,7 +8928,7 @@
       </c>
       <c r="D33" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_06'</v>
+        <v>'category_05'</v>
       </c>
       <c r="E33" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8916,15 +8956,15 @@
       </c>
       <c r="K33" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_06')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>$table-&gt;unsignedInteger('category_05')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" hidden="1">
       <c r="A34" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C34" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8932,7 +8972,7 @@
       </c>
       <c r="D34" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_07'</v>
+        <v>'category_06'</v>
       </c>
       <c r="E34" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -8960,15 +9000,15 @@
       </c>
       <c r="K34" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_07')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>$table-&gt;unsignedInteger('category_06')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" hidden="1">
       <c r="A35" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C35" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -8976,7 +9016,7 @@
       </c>
       <c r="D35" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_08'</v>
+        <v>'category_07'</v>
       </c>
       <c r="E35" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9004,15 +9044,15 @@
       </c>
       <c r="K35" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_08')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>$table-&gt;unsignedInteger('category_07')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" hidden="1">
       <c r="A36" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C36" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9020,7 +9060,7 @@
       </c>
       <c r="D36" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_09'</v>
+        <v>'category_08'</v>
       </c>
       <c r="E36" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9048,15 +9088,15 @@
       </c>
       <c r="K36" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_09')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>$table-&gt;unsignedInteger('category_08')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" hidden="1">
       <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C37" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9064,7 +9104,7 @@
       </c>
       <c r="D37" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_10'</v>
+        <v>'category_09'</v>
       </c>
       <c r="E37" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9092,31 +9132,31 @@
       </c>
       <c r="K37" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('category_10')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="2" t="s">
+        <v>$table-&gt;unsignedInteger('category_09')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" hidden="1">
+      <c r="A38" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>223</v>
+      <c r="B38" s="4" t="s">
+        <v>363</v>
       </c>
       <c r="C38" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>enum(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D38" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'status'</v>
+        <v>'category_10'</v>
       </c>
       <c r="E38" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Active','Inactive'])</v>
+        <v>)</v>
       </c>
       <c r="F38" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Active')</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G38" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -9136,35 +9176,35 @@
       </c>
       <c r="K38" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <v>$table-&gt;unsignedInteger('category_10')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" hidden="1">
       <c r="A39" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="C39" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D39" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'status'</v>
       </c>
       <c r="E39" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Active','Inactive'])</v>
       </c>
       <c r="F39" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('Active')</v>
       </c>
       <c r="G39" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H39" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -9180,23 +9220,23 @@
       </c>
       <c r="K39" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" hidden="1">
       <c r="A40" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>365</v>
+      <c r="B40" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C40" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D40" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_01'</v>
+        <v/>
       </c>
       <c r="E40" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9204,19 +9244,19 @@
       </c>
       <c r="F40" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G40" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('item_group_master')</v>
+        <v/>
       </c>
       <c r="H40" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I40" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('set null')</v>
+        <v/>
       </c>
       <c r="J40" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -9224,15 +9264,15 @@
       </c>
       <c r="K40" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('category_01')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" hidden="1">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C41" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9240,7 +9280,7 @@
       </c>
       <c r="D41" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_02'</v>
+        <v>'category_01'</v>
       </c>
       <c r="E41" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9268,15 +9308,15 @@
       </c>
       <c r="K41" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('category_02')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+        <v>$table-&gt;foreign('category_01')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" hidden="1">
       <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C42" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9284,7 +9324,7 @@
       </c>
       <c r="D42" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_03'</v>
+        <v>'category_02'</v>
       </c>
       <c r="E42" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9312,15 +9352,15 @@
       </c>
       <c r="K42" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('category_03')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+        <v>$table-&gt;foreign('category_02')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" hidden="1">
       <c r="A43" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C43" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9328,7 +9368,7 @@
       </c>
       <c r="D43" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_04'</v>
+        <v>'category_03'</v>
       </c>
       <c r="E43" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9356,15 +9396,15 @@
       </c>
       <c r="K43" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('category_04')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+        <v>$table-&gt;foreign('category_03')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" hidden="1">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C44" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9372,7 +9412,7 @@
       </c>
       <c r="D44" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_05'</v>
+        <v>'category_04'</v>
       </c>
       <c r="E44" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9400,15 +9440,15 @@
       </c>
       <c r="K44" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('category_05')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+        <v>$table-&gt;foreign('category_04')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" hidden="1">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C45" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9416,7 +9456,7 @@
       </c>
       <c r="D45" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_06'</v>
+        <v>'category_05'</v>
       </c>
       <c r="E45" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9444,15 +9484,15 @@
       </c>
       <c r="K45" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('category_06')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+        <v>$table-&gt;foreign('category_05')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" hidden="1">
       <c r="A46" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C46" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9460,7 +9500,7 @@
       </c>
       <c r="D46" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_07'</v>
+        <v>'category_06'</v>
       </c>
       <c r="E46" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9488,15 +9528,15 @@
       </c>
       <c r="K46" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('category_07')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
+        <v>$table-&gt;foreign('category_06')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" hidden="1">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C47" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9504,7 +9544,7 @@
       </c>
       <c r="D47" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_08'</v>
+        <v>'category_07'</v>
       </c>
       <c r="E47" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9532,15 +9572,15 @@
       </c>
       <c r="K47" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('category_08')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+        <v>$table-&gt;foreign('category_07')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" hidden="1">
       <c r="A48" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C48" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9548,7 +9588,7 @@
       </c>
       <c r="D48" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_09'</v>
+        <v>'category_08'</v>
       </c>
       <c r="E48" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9576,15 +9616,15 @@
       </c>
       <c r="K48" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('category_09')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
+        <v>$table-&gt;foreign('category_08')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" hidden="1">
       <c r="A49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>375</v>
+      <c r="B49" s="1" t="s">
+        <v>374</v>
       </c>
       <c r="C49" s="33" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9592,7 +9632,7 @@
       </c>
       <c r="D49" s="33" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'category_10'</v>
+        <v>'category_09'</v>
       </c>
       <c r="E49" s="34" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9620,115 +9660,115 @@
       </c>
       <c r="K49" s="33" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('category_09')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" hidden="1">
+      <c r="A50" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C50" s="33" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D50" s="33" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'category_10'</v>
+      </c>
+      <c r="E50" s="34" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F50" s="33" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G50" s="33" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('item_group_master')</v>
+      </c>
+      <c r="H50" s="33" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I50" s="33" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('set null')</v>
+      </c>
+      <c r="J50" s="33" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K50" s="33" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
         <v>$table-&gt;foreign('category_10')-&gt;references('id')-&gt;on('item_group_master')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="3" t="s">
+    <row r="51" spans="1:11" hidden="1">
+      <c r="A51" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="3" t="str">
+      <c r="C51" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
         <v>increments(</v>
       </c>
-      <c r="D50" s="3" t="str">
+      <c r="D51" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
         <v>'id'</v>
       </c>
-      <c r="E50" s="6" t="str">
+      <c r="E51" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
         <v>)</v>
       </c>
-      <c r="F50" s="3" t="str">
+      <c r="F51" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
         <v/>
       </c>
-      <c r="G50" s="3" t="str">
+      <c r="G51" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
         <v/>
       </c>
-      <c r="H50" s="3" t="str">
+      <c r="H51" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
         <v/>
       </c>
-      <c r="I50" s="3" t="str">
+      <c r="I51" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
         <v/>
       </c>
-      <c r="J50" s="3" t="str">
+      <c r="J51" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
         <v/>
       </c>
-      <c r="K50" s="3" t="str">
+      <c r="K51" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="3" t="s">
+    <row r="52" spans="1:11" hidden="1">
+      <c r="A52" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C51" s="3" t="str">
+      <c r="C52" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
         <v>string(</v>
       </c>
-      <c r="D51" s="3" t="str">
+      <c r="D52" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
         <v>'name'</v>
       </c>
-      <c r="E51" s="6" t="str">
+      <c r="E52" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
         <v>, 64)</v>
-      </c>
-      <c r="F51" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
-      </c>
-      <c r="G51" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
-      </c>
-      <c r="H51" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
-      </c>
-      <c r="I51" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
-      </c>
-      <c r="J51" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
-        <v/>
-      </c>
-      <c r="K51" s="3" t="str">
-        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('name', 64)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C52" s="3" t="str">
-        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
-      </c>
-      <c r="D52" s="3" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'product'</v>
-      </c>
-      <c r="E52" s="6" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
       </c>
       <c r="F52" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -9736,7 +9776,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H52" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -9752,27 +9792,27 @@
       </c>
       <c r="K52" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('product')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
+        <v>$table-&gt;string('name', 64)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" hidden="1">
       <c r="A53" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C53" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>string(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D53" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'image'</v>
+        <v>'product'</v>
       </c>
       <c r="E53" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 128)</v>
+        <v>)</v>
       </c>
       <c r="F53" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -9780,7 +9820,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H53" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -9796,35 +9836,35 @@
       </c>
       <c r="K53" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('image', 128)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
+        <v>$table-&gt;unsignedInteger('product')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" hidden="1">
       <c r="A54" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C54" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>enum(</v>
+        <v>string(</v>
       </c>
       <c r="D54" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'default'</v>
+        <v>'image'</v>
       </c>
       <c r="E54" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Yes','No'])</v>
+        <v>, 128)</v>
       </c>
       <c r="F54" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Yes')</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G54" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H54" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -9840,15 +9880,15 @@
       </c>
       <c r="K54" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('default', ['Yes','No'])-&gt;default('Yes')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
+        <v>$table-&gt;string('image', 128)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" hidden="1">
       <c r="A55" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="C55" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -9856,15 +9896,15 @@
       </c>
       <c r="D55" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'status'</v>
+        <v>'default'</v>
       </c>
       <c r="E55" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Active','Inactive'])</v>
+        <v>, ['Yes','No'])</v>
       </c>
       <c r="F55" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Active')</v>
+        <v>-&gt;default('Yes')</v>
       </c>
       <c r="G55" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -9884,35 +9924,35 @@
       </c>
       <c r="K55" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
+        <v>$table-&gt;enum('default', ['Yes','No'])-&gt;default('Yes')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" hidden="1">
       <c r="A56" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="C56" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D56" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'status'</v>
       </c>
       <c r="E56" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Active','Inactive'])</v>
       </c>
       <c r="F56" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('Active')</v>
       </c>
       <c r="G56" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H56" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -9928,23 +9968,23 @@
       </c>
       <c r="K56" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
+        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" hidden="1">
       <c r="A57" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>264</v>
+        <v>12</v>
       </c>
       <c r="C57" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D57" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'product'</v>
+        <v/>
       </c>
       <c r="E57" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9952,19 +9992,19 @@
       </c>
       <c r="F57" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G57" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('products')</v>
+        <v/>
       </c>
       <c r="H57" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I57" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('cascade')</v>
+        <v/>
       </c>
       <c r="J57" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -9972,23 +10012,23 @@
       </c>
       <c r="K57" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('product')-&gt;references('id')-&gt;on('products')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" hidden="1">
       <c r="A58" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>10</v>
+        <v>264</v>
       </c>
       <c r="C58" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>increments(</v>
+        <v>foreign(</v>
       </c>
       <c r="D58" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'id'</v>
+        <v>'product'</v>
       </c>
       <c r="E58" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -9996,19 +10036,19 @@
       </c>
       <c r="F58" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;references('id')</v>
       </c>
       <c r="G58" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;on('products')</v>
       </c>
       <c r="H58" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
+        <v>-&gt;onUpdate('cascade')</v>
       </c>
       <c r="I58" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
+        <v>-&gt;onDelete('cascade')</v>
       </c>
       <c r="J58" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -10016,31 +10056,31 @@
       </c>
       <c r="K58" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;increments('id');</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
+        <v>$table-&gt;foreign('product')-&gt;references('id')-&gt;on('products')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" hidden="1">
       <c r="A59" s="3" t="s">
         <v>208</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="C59" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>string(</v>
+        <v>increments(</v>
       </c>
       <c r="D59" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'name'</v>
+        <v>'id'</v>
       </c>
       <c r="E59" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 64)</v>
+        <v>)</v>
       </c>
       <c r="F59" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="G59" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -10060,15 +10100,15 @@
       </c>
       <c r="K59" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('name', 64)-&gt;index();</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" hidden="1">
       <c r="A60" s="3" t="s">
         <v>208</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>167</v>
+        <v>94</v>
       </c>
       <c r="C60" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -10076,15 +10116,15 @@
       </c>
       <c r="D60" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'email'</v>
+        <v>'name'</v>
       </c>
       <c r="E60" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 256)</v>
+        <v>, 64)</v>
       </c>
       <c r="F60" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
+        <v>-&gt;index()</v>
       </c>
       <c r="G60" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -10104,15 +10144,15 @@
       </c>
       <c r="K60" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('email', 256)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
+        <v>$table-&gt;string('name', 64)-&gt;index();</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" hidden="1">
       <c r="A61" s="3" t="s">
         <v>208</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
       <c r="C61" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -10120,11 +10160,11 @@
       </c>
       <c r="D61" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'number'</v>
+        <v>'email'</v>
       </c>
       <c r="E61" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 64)</v>
+        <v>, 256)</v>
       </c>
       <c r="F61" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -10148,31 +10188,31 @@
       </c>
       <c r="K61" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('number', 64)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
+        <v>$table-&gt;string('email', 256)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" hidden="1">
       <c r="A62" s="3" t="s">
         <v>208</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="C62" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>string(</v>
       </c>
       <c r="D62" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'number'</v>
       </c>
       <c r="E62" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, 64)</v>
       </c>
       <c r="F62" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G62" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -10192,23 +10232,23 @@
       </c>
       <c r="K62" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
+        <v>$table-&gt;string('number', 64)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" hidden="1">
       <c r="A63" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C63" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>increments(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D63" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'id'</v>
+        <v/>
       </c>
       <c r="E63" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -10236,31 +10276,31 @@
       </c>
       <c r="K63" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;increments('id');</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11">
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" hidden="1">
       <c r="A64" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="C64" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>string(</v>
+        <v>increments(</v>
       </c>
       <c r="D64" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'name'</v>
+        <v>'id'</v>
       </c>
       <c r="E64" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 64)</v>
+        <v>)</v>
       </c>
       <c r="F64" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="G64" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -10280,15 +10320,15 @@
       </c>
       <c r="K64" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('name', 64)-&gt;index();</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" hidden="1">
       <c r="A65" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C65" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -10296,15 +10336,15 @@
       </c>
       <c r="D65" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'description'</v>
+        <v>'name'</v>
       </c>
       <c r="E65" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 1024)</v>
+        <v>, 64)</v>
       </c>
       <c r="F65" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
+        <v>-&gt;index()</v>
       </c>
       <c r="G65" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -10324,27 +10364,27 @@
       </c>
       <c r="K65" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('description', 1024)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
+        <v>$table-&gt;string('name', 64)-&gt;index();</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" hidden="1">
       <c r="A66" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>220</v>
+        <v>95</v>
       </c>
       <c r="C66" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
+        <v>string(</v>
       </c>
       <c r="D66" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'author'</v>
+        <v>'description'</v>
       </c>
       <c r="E66" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, 1024)</v>
       </c>
       <c r="F66" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -10352,7 +10392,7 @@
       </c>
       <c r="G66" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H66" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -10368,31 +10408,31 @@
       </c>
       <c r="K66" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('author')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
+        <v>$table-&gt;string('description', 1024)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" hidden="1">
       <c r="A67" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C67" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>enum(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D67" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'status'</v>
+        <v>'author'</v>
       </c>
       <c r="E67" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Active','Inactive'])</v>
+        <v>)</v>
       </c>
       <c r="F67" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Active')</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G67" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -10412,35 +10452,35 @@
       </c>
       <c r="K67" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
+        <v>$table-&gt;unsignedInteger('author')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" hidden="1">
       <c r="A68" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="C68" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D68" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'status'</v>
       </c>
       <c r="E68" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Active','Inactive'])</v>
       </c>
       <c r="F68" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('Active')</v>
       </c>
       <c r="G68" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H68" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -10456,23 +10496,23 @@
       </c>
       <c r="K68" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
+        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" hidden="1">
       <c r="A69" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>268</v>
+        <v>12</v>
       </c>
       <c r="C69" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D69" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'author'</v>
+        <v/>
       </c>
       <c r="E69" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -10480,19 +10520,19 @@
       </c>
       <c r="F69" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G69" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('visitors')</v>
+        <v/>
       </c>
       <c r="H69" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I69" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('set null')</v>
+        <v/>
       </c>
       <c r="J69" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -10500,23 +10540,23 @@
       </c>
       <c r="K69" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('author')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" hidden="1">
       <c r="A70" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>10</v>
+        <v>268</v>
       </c>
       <c r="C70" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>increments(</v>
+        <v>foreign(</v>
       </c>
       <c r="D70" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'id'</v>
+        <v>'author'</v>
       </c>
       <c r="E70" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -10524,19 +10564,19 @@
       </c>
       <c r="F70" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;references('id')</v>
       </c>
       <c r="G70" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;on('visitors')</v>
       </c>
       <c r="H70" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
+        <v>-&gt;onUpdate('cascade')</v>
       </c>
       <c r="I70" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
+        <v>-&gt;onDelete('set null')</v>
       </c>
       <c r="J70" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -10544,23 +10584,23 @@
       </c>
       <c r="K70" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;increments('id');</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11">
+        <v>$table-&gt;foreign('author')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" hidden="1">
       <c r="A71" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="C71" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
+        <v>increments(</v>
       </c>
       <c r="D71" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'visitor'</v>
+        <v>'id'</v>
       </c>
       <c r="E71" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -10568,11 +10608,11 @@
       </c>
       <c r="F71" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
+        <v/>
       </c>
       <c r="G71" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H71" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -10588,15 +10628,15 @@
       </c>
       <c r="K71" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('visitor')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" hidden="1">
       <c r="A72" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="C72" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -10604,7 +10644,7 @@
       </c>
       <c r="D72" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist'</v>
+        <v>'visitor'</v>
       </c>
       <c r="E72" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -10632,31 +10672,31 @@
       </c>
       <c r="K72" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11">
+        <v>$table-&gt;unsignedInteger('visitor')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" hidden="1">
       <c r="A73" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>251</v>
+        <v>209</v>
       </c>
       <c r="C73" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>enum(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D73" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'viewed'</v>
+        <v>'wishlist'</v>
       </c>
       <c r="E73" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Yes','No'])</v>
+        <v>)</v>
       </c>
       <c r="F73" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('No')</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G73" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -10676,15 +10716,15 @@
       </c>
       <c r="K73" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('viewed', ['Yes','No'])-&gt;default('No')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11">
+        <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" hidden="1">
       <c r="A74" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="C74" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -10692,15 +10732,15 @@
       </c>
       <c r="D74" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'status'</v>
+        <v>'viewed'</v>
       </c>
       <c r="E74" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Active','Inactive'])</v>
+        <v>, ['Yes','No'])</v>
       </c>
       <c r="F74" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Active')</v>
+        <v>-&gt;default('No')</v>
       </c>
       <c r="G74" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -10720,35 +10760,35 @@
       </c>
       <c r="K74" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11">
+        <v>$table-&gt;enum('viewed', ['Yes','No'])-&gt;default('No')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" hidden="1">
       <c r="A75" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="C75" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D75" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'status'</v>
       </c>
       <c r="E75" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Active','Inactive'])</v>
       </c>
       <c r="F75" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('Active')</v>
       </c>
       <c r="G75" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H75" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -10764,23 +10804,23 @@
       </c>
       <c r="K75" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11">
+        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" hidden="1">
       <c r="A76" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>266</v>
+        <v>12</v>
       </c>
       <c r="C76" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D76" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'visitor'</v>
+        <v/>
       </c>
       <c r="E76" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -10788,19 +10828,19 @@
       </c>
       <c r="F76" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G76" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('visitors')</v>
+        <v/>
       </c>
       <c r="H76" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I76" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('set null')</v>
+        <v/>
       </c>
       <c r="J76" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -10808,15 +10848,15 @@
       </c>
       <c r="K76" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('visitor')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11">
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" hidden="1">
       <c r="A77" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C77" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -10824,7 +10864,7 @@
       </c>
       <c r="D77" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist'</v>
+        <v>'visitor'</v>
       </c>
       <c r="E77" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -10836,7 +10876,7 @@
       </c>
       <c r="G77" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('wishlists')</v>
+        <v>-&gt;on('visitors')</v>
       </c>
       <c r="H77" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -10844,7 +10884,7 @@
       </c>
       <c r="I77" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('cascade')</v>
+        <v>-&gt;onDelete('set null')</v>
       </c>
       <c r="J77" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -10852,23 +10892,23 @@
       </c>
       <c r="K77" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11">
+        <v>$table-&gt;foreign('visitor')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" hidden="1">
       <c r="A78" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>10</v>
+        <v>269</v>
       </c>
       <c r="C78" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>increments(</v>
+        <v>foreign(</v>
       </c>
       <c r="D78" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'id'</v>
+        <v>'wishlist'</v>
       </c>
       <c r="E78" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -10876,19 +10916,19 @@
       </c>
       <c r="F78" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;references('id')</v>
       </c>
       <c r="G78" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;on('wishlists')</v>
       </c>
       <c r="H78" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
+        <v>-&gt;onUpdate('cascade')</v>
       </c>
       <c r="I78" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
+        <v>-&gt;onDelete('cascade')</v>
       </c>
       <c r="J78" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -10896,23 +10936,23 @@
       </c>
       <c r="K78" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;increments('id');</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11">
+        <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" hidden="1">
       <c r="A79" s="3" t="s">
         <v>214</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>209</v>
+        <v>10</v>
       </c>
       <c r="C79" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
+        <v>increments(</v>
       </c>
       <c r="D79" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist'</v>
+        <v>'id'</v>
       </c>
       <c r="E79" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -10920,11 +10960,11 @@
       </c>
       <c r="F79" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
+        <v/>
       </c>
       <c r="G79" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H79" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -10940,27 +10980,27 @@
       </c>
       <c r="K79" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11">
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" hidden="1">
       <c r="A80" s="3" t="s">
         <v>214</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>253</v>
+        <v>209</v>
       </c>
       <c r="C80" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>string(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D80" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'note'</v>
+        <v>'wishlist'</v>
       </c>
       <c r="E80" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 512)</v>
+        <v>)</v>
       </c>
       <c r="F80" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -10968,7 +11008,7 @@
       </c>
       <c r="G80" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H80" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -10984,27 +11024,27 @@
       </c>
       <c r="K80" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('note', 512)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11">
+        <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" hidden="1">
       <c r="A81" s="3" t="s">
         <v>214</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="C81" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
+        <v>string(</v>
       </c>
       <c r="D81" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'author'</v>
+        <v>'note'</v>
       </c>
       <c r="E81" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, 512)</v>
       </c>
       <c r="F81" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -11012,7 +11052,7 @@
       </c>
       <c r="G81" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H81" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11028,31 +11068,31 @@
       </c>
       <c r="K81" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('author')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11">
+        <v>$table-&gt;string('note', 512)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" hidden="1">
       <c r="A82" s="3" t="s">
         <v>214</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>223</v>
+        <v>273</v>
       </c>
       <c r="C82" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>enum(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D82" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'status'</v>
+        <v>'author'</v>
       </c>
       <c r="E82" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Active','Inactive'])</v>
+        <v>)</v>
       </c>
       <c r="F82" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Active')</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G82" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -11072,35 +11112,35 @@
       </c>
       <c r="K82" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11">
+        <v>$table-&gt;unsignedInteger('author')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" hidden="1">
       <c r="A83" s="3" t="s">
         <v>214</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="C83" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D83" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'status'</v>
       </c>
       <c r="E83" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Active','Inactive'])</v>
       </c>
       <c r="F83" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('Active')</v>
       </c>
       <c r="G83" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H83" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11116,23 +11156,23 @@
       </c>
       <c r="K83" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11">
+        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" hidden="1">
       <c r="A84" s="3" t="s">
         <v>214</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>269</v>
+        <v>12</v>
       </c>
       <c r="C84" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D84" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist'</v>
+        <v/>
       </c>
       <c r="E84" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11140,19 +11180,19 @@
       </c>
       <c r="F84" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G84" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('wishlists')</v>
+        <v/>
       </c>
       <c r="H84" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I84" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('cascade')</v>
+        <v/>
       </c>
       <c r="J84" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -11160,15 +11200,15 @@
       </c>
       <c r="K84" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11">
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" hidden="1">
       <c r="A85" s="3" t="s">
         <v>214</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C85" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -11176,7 +11216,7 @@
       </c>
       <c r="D85" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'author'</v>
+        <v>'wishlist'</v>
       </c>
       <c r="E85" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11188,7 +11228,7 @@
       </c>
       <c r="G85" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('visitors')</v>
+        <v>-&gt;on('wishlists')</v>
       </c>
       <c r="H85" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11196,7 +11236,7 @@
       </c>
       <c r="I85" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('set null')</v>
+        <v>-&gt;onDelete('cascade')</v>
       </c>
       <c r="J85" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -11204,23 +11244,23 @@
       </c>
       <c r="K85" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('author')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11">
+        <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" hidden="1">
       <c r="A86" s="3" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>10</v>
+        <v>268</v>
       </c>
       <c r="C86" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>increments(</v>
+        <v>foreign(</v>
       </c>
       <c r="D86" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'id'</v>
+        <v>'author'</v>
       </c>
       <c r="E86" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11228,19 +11268,19 @@
       </c>
       <c r="F86" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;references('id')</v>
       </c>
       <c r="G86" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;on('visitors')</v>
       </c>
       <c r="H86" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
+        <v>-&gt;onUpdate('cascade')</v>
       </c>
       <c r="I86" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
+        <v>-&gt;onDelete('set null')</v>
       </c>
       <c r="J86" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -11248,23 +11288,23 @@
       </c>
       <c r="K86" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;increments('id');</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11">
+        <v>$table-&gt;foreign('author')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" hidden="1">
       <c r="A87" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>209</v>
+        <v>10</v>
       </c>
       <c r="C87" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
+        <v>increments(</v>
       </c>
       <c r="D87" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist'</v>
+        <v>'id'</v>
       </c>
       <c r="E87" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11272,11 +11312,11 @@
       </c>
       <c r="F87" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
+        <v/>
       </c>
       <c r="G87" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H87" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11292,15 +11332,15 @@
       </c>
       <c r="K87" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11">
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" hidden="1">
       <c r="A88" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="C88" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -11308,7 +11348,7 @@
       </c>
       <c r="D88" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'product'</v>
+        <v>'wishlist'</v>
       </c>
       <c r="E88" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11336,15 +11376,15 @@
       </c>
       <c r="K88" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('product')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11">
+        <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" hidden="1">
       <c r="A89" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C89" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -11352,7 +11392,7 @@
       </c>
       <c r="D89" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'added_by'</v>
+        <v>'product'</v>
       </c>
       <c r="E89" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11380,23 +11420,23 @@
       </c>
       <c r="K89" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('added_by')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11">
+        <v>$table-&gt;unsignedInteger('product')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" hidden="1">
       <c r="A90" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C90" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamp(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D90" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'added_on'</v>
+        <v>'added_by'</v>
       </c>
       <c r="E90" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11404,11 +11444,11 @@
       </c>
       <c r="F90" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default(DB::raw('CURRENT_TIMESTAMP'))</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G90" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H90" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11424,23 +11464,23 @@
       </c>
       <c r="K90" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamp('added_on')-&gt;default(DB::raw('CURRENT_TIMESTAMP'));</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11">
+        <v>$table-&gt;unsignedInteger('added_by')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" hidden="1">
       <c r="A91" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C91" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
+        <v>timestamp(</v>
       </c>
       <c r="D91" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'removed_by'</v>
+        <v>'added_on'</v>
       </c>
       <c r="E91" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11448,11 +11488,11 @@
       </c>
       <c r="F91" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
+        <v>-&gt;default(DB::raw('CURRENT_TIMESTAMP'))</v>
       </c>
       <c r="G91" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H91" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11468,23 +11508,23 @@
       </c>
       <c r="K91" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('removed_by')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11">
+        <v>$table-&gt;timestamp('added_on')-&gt;default(DB::raw('CURRENT_TIMESTAMP'));</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" hidden="1">
       <c r="A92" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C92" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamp(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D92" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'removed_on'</v>
+        <v>'removed_by'</v>
       </c>
       <c r="E92" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11492,11 +11532,11 @@
       </c>
       <c r="F92" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default(DB::raw('CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP'))</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G92" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H92" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11512,35 +11552,35 @@
       </c>
       <c r="K92" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamp('removed_on')-&gt;default(DB::raw('CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP'));</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11">
+        <v>$table-&gt;unsignedInteger('removed_by')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" hidden="1">
       <c r="A93" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C93" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>enum(</v>
+        <v>timestamp(</v>
       </c>
       <c r="D93" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'product_status'</v>
+        <v>'removed_on'</v>
       </c>
       <c r="E93" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Active','Inactive'])</v>
+        <v>)</v>
       </c>
       <c r="F93" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Active')</v>
+        <v>-&gt;default(DB::raw('CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP'))</v>
       </c>
       <c r="G93" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H93" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11556,15 +11596,15 @@
       </c>
       <c r="K93" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('product_status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11">
+        <v>$table-&gt;timestamp('removed_on')-&gt;default(DB::raw('CURRENT_TIMESTAMP ON UPDATE CURRENT_TIMESTAMP'));</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" hidden="1">
       <c r="A94" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="C94" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -11572,7 +11612,7 @@
       </c>
       <c r="D94" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'status'</v>
+        <v>'product_status'</v>
       </c>
       <c r="E94" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11600,35 +11640,35 @@
       </c>
       <c r="K94" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11">
+        <v>$table-&gt;enum('product_status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" hidden="1">
       <c r="A95" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="C95" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D95" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'status'</v>
       </c>
       <c r="E95" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Active','Inactive'])</v>
       </c>
       <c r="F95" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('Active')</v>
       </c>
       <c r="G95" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H95" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11644,23 +11684,23 @@
       </c>
       <c r="K95" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11">
+        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" hidden="1">
       <c r="A96" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>269</v>
+        <v>12</v>
       </c>
       <c r="C96" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D96" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist'</v>
+        <v/>
       </c>
       <c r="E96" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11668,19 +11708,19 @@
       </c>
       <c r="F96" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G96" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('wishlists')</v>
+        <v/>
       </c>
       <c r="H96" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I96" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('cascade')</v>
+        <v/>
       </c>
       <c r="J96" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -11688,15 +11728,15 @@
       </c>
       <c r="K96" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11">
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" hidden="1">
       <c r="A97" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="C97" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -11704,7 +11744,7 @@
       </c>
       <c r="D97" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'product'</v>
+        <v>'wishlist'</v>
       </c>
       <c r="E97" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11716,7 +11756,7 @@
       </c>
       <c r="G97" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('products')</v>
+        <v>-&gt;on('wishlists')</v>
       </c>
       <c r="H97" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11732,15 +11772,15 @@
       </c>
       <c r="K97" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('product')-&gt;references('id')-&gt;on('products')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11">
+        <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" hidden="1">
       <c r="A98" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C98" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -11748,7 +11788,7 @@
       </c>
       <c r="D98" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'added_by'</v>
+        <v>'product'</v>
       </c>
       <c r="E98" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11760,7 +11800,7 @@
       </c>
       <c r="G98" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('visitors')</v>
+        <v>-&gt;on('products')</v>
       </c>
       <c r="H98" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11768,7 +11808,7 @@
       </c>
       <c r="I98" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('set null')</v>
+        <v>-&gt;onDelete('cascade')</v>
       </c>
       <c r="J98" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -11776,15 +11816,15 @@
       </c>
       <c r="K98" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('added_by')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11">
+        <v>$table-&gt;foreign('product')-&gt;references('id')-&gt;on('products')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" hidden="1">
       <c r="A99" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C99" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -11792,7 +11832,7 @@
       </c>
       <c r="D99" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'removed_by'</v>
+        <v>'added_by'</v>
       </c>
       <c r="E99" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11820,23 +11860,23 @@
       </c>
       <c r="K99" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('removed_by')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11">
+        <v>$table-&gt;foreign('added_by')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" hidden="1">
       <c r="A100" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>10</v>
+        <v>275</v>
       </c>
       <c r="C100" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>increments(</v>
+        <v>foreign(</v>
       </c>
       <c r="D100" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'id'</v>
+        <v>'removed_by'</v>
       </c>
       <c r="E100" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11844,19 +11884,19 @@
       </c>
       <c r="F100" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;references('id')</v>
       </c>
       <c r="G100" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;on('visitors')</v>
       </c>
       <c r="H100" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
+        <v>-&gt;onUpdate('cascade')</v>
       </c>
       <c r="I100" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
+        <v>-&gt;onDelete('set null')</v>
       </c>
       <c r="J100" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -11864,23 +11904,23 @@
       </c>
       <c r="K100" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;increments('id');</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11">
+        <v>$table-&gt;foreign('removed_by')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" hidden="1">
       <c r="A101" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>254</v>
+        <v>10</v>
       </c>
       <c r="C101" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
+        <v>increments(</v>
       </c>
       <c r="D101" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist_product'</v>
+        <v>'id'</v>
       </c>
       <c r="E101" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -11888,11 +11928,11 @@
       </c>
       <c r="F101" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
+        <v/>
       </c>
       <c r="G101" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H101" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11908,27 +11948,27 @@
       </c>
       <c r="K101" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('wishlist_product')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11">
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" hidden="1">
       <c r="A102" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C102" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>string(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D102" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'note'</v>
+        <v>'wishlist_product'</v>
       </c>
       <c r="E102" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 512)</v>
+        <v>)</v>
       </c>
       <c r="F102" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -11936,7 +11976,7 @@
       </c>
       <c r="G102" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H102" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11952,27 +11992,27 @@
       </c>
       <c r="K102" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('note', 512)-&gt;nullable();</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11">
+        <v>$table-&gt;unsignedInteger('wishlist_product')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" hidden="1">
       <c r="A103" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="C103" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
+        <v>string(</v>
       </c>
       <c r="D103" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'author'</v>
+        <v>'note'</v>
       </c>
       <c r="E103" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, 512)</v>
       </c>
       <c r="F103" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -11980,7 +12020,7 @@
       </c>
       <c r="G103" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H103" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -11996,31 +12036,31 @@
       </c>
       <c r="K103" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('author')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11">
+        <v>$table-&gt;string('note', 512)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" hidden="1">
       <c r="A104" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>223</v>
+        <v>273</v>
       </c>
       <c r="C104" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>enum(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D104" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'status'</v>
+        <v>'author'</v>
       </c>
       <c r="E104" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Active','Inactive'])</v>
+        <v>)</v>
       </c>
       <c r="F104" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Active')</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G104" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -12040,35 +12080,35 @@
       </c>
       <c r="K104" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11">
+        <v>$table-&gt;unsignedInteger('author')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" hidden="1">
       <c r="A105" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="C105" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D105" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'status'</v>
       </c>
       <c r="E105" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Active','Inactive'])</v>
       </c>
       <c r="F105" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('Active')</v>
       </c>
       <c r="G105" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H105" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -12084,23 +12124,23 @@
       </c>
       <c r="K105" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11">
+        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" hidden="1">
       <c r="A106" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>271</v>
+        <v>12</v>
       </c>
       <c r="C106" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D106" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist_product'</v>
+        <v/>
       </c>
       <c r="E106" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -12108,19 +12148,19 @@
       </c>
       <c r="F106" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G106" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('wishlist_products')</v>
+        <v/>
       </c>
       <c r="H106" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I106" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('cascade')</v>
+        <v/>
       </c>
       <c r="J106" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -12128,15 +12168,15 @@
       </c>
       <c r="K106" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('wishlist_product')-&gt;references('id')-&gt;on('wishlist_products')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11">
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" hidden="1">
       <c r="A107" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C107" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -12144,7 +12184,7 @@
       </c>
       <c r="D107" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'author'</v>
+        <v>'wishlist_product'</v>
       </c>
       <c r="E107" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -12156,7 +12196,7 @@
       </c>
       <c r="G107" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('visitors')</v>
+        <v>-&gt;on('wishlist_products')</v>
       </c>
       <c r="H107" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -12164,7 +12204,7 @@
       </c>
       <c r="I107" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('set null')</v>
+        <v>-&gt;onDelete('cascade')</v>
       </c>
       <c r="J107" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -12172,23 +12212,23 @@
       </c>
       <c r="K107" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;foreign('author')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11">
+        <v>$table-&gt;foreign('wishlist_product')-&gt;references('id')-&gt;on('wishlist_products')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" hidden="1">
       <c r="A108" s="3" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>10</v>
+        <v>268</v>
       </c>
       <c r="C108" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>increments(</v>
+        <v>foreign(</v>
       </c>
       <c r="D108" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'id'</v>
+        <v>'author'</v>
       </c>
       <c r="E108" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -12196,19 +12236,19 @@
       </c>
       <c r="F108" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;references('id')</v>
       </c>
       <c r="G108" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;on('visitors')</v>
       </c>
       <c r="H108" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
+        <v>-&gt;onUpdate('cascade')</v>
       </c>
       <c r="I108" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
+        <v>-&gt;onDelete('set null')</v>
       </c>
       <c r="J108" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
@@ -12216,23 +12256,23 @@
       </c>
       <c r="K108" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;increments('id');</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11">
+        <v>$table-&gt;foreign('author')-&gt;references('id')-&gt;on('visitors')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" hidden="1">
       <c r="A109" s="3" t="s">
         <v>213</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>209</v>
+        <v>10</v>
       </c>
       <c r="C109" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>unsignedInteger(</v>
+        <v>increments(</v>
       </c>
       <c r="D109" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist'</v>
+        <v>'id'</v>
       </c>
       <c r="E109" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -12240,11 +12280,11 @@
       </c>
       <c r="F109" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;nullable()</v>
+        <v/>
       </c>
       <c r="G109" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;index()</v>
+        <v/>
       </c>
       <c r="H109" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -12260,31 +12300,31 @@
       </c>
       <c r="K109" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11">
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" hidden="1">
       <c r="A110" s="3" t="s">
         <v>213</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="C110" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>enum(</v>
+        <v>unsignedInteger(</v>
       </c>
       <c r="D110" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'status'</v>
+        <v>'wishlist'</v>
       </c>
       <c r="E110" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Active','Inactive'])</v>
+        <v>)</v>
       </c>
       <c r="F110" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('Active')</v>
+        <v>-&gt;nullable()</v>
       </c>
       <c r="G110" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -12304,15 +12344,15 @@
       </c>
       <c r="K110" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11">
+        <v>$table-&gt;unsignedInteger('wishlist')-&gt;nullable()-&gt;index();</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" hidden="1">
       <c r="A111" s="3" t="s">
         <v>213</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="C111" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -12320,15 +12360,15 @@
       </c>
       <c r="D111" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'viewed'</v>
+        <v>'status'</v>
       </c>
       <c r="E111" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Yes','No'])</v>
+        <v>, ['Active','Inactive'])</v>
       </c>
       <c r="F111" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;default('No')</v>
+        <v>-&gt;default('Active')</v>
       </c>
       <c r="G111" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -12348,35 +12388,35 @@
       </c>
       <c r="K111" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('viewed', ['Yes','No'])-&gt;default('No')-&gt;index();</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" s="16" customFormat="1">
+        <v>$table-&gt;enum('status', ['Active','Inactive'])-&gt;default('Active')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" s="16" customFormat="1" hidden="1">
       <c r="A112" s="3" t="s">
         <v>213</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>12</v>
+        <v>251</v>
       </c>
       <c r="C112" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D112" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'viewed'</v>
       </c>
       <c r="E112" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Yes','No'])</v>
       </c>
       <c r="F112" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('No')</v>
       </c>
       <c r="G112" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
+        <v>-&gt;index()</v>
       </c>
       <c r="H112" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
@@ -12392,23 +12432,23 @@
       </c>
       <c r="K112" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11">
+        <v>$table-&gt;enum('viewed', ['Yes','No'])-&gt;default('No')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" hidden="1">
       <c r="A113" s="3" t="s">
         <v>213</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>269</v>
+        <v>12</v>
       </c>
       <c r="C113" s="3" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D113" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'wishlist'</v>
+        <v/>
       </c>
       <c r="E113" s="6" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -12416,25 +12456,69 @@
       </c>
       <c r="F113" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G113" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('wishlists')</v>
+        <v/>
       </c>
       <c r="H113" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I113" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('cascade')</v>
+        <v/>
       </c>
       <c r="J113" s="3" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
         <v/>
       </c>
       <c r="K113" s="3" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" hidden="1">
+      <c r="A114" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C114" s="3" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D114" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'wishlist'</v>
+      </c>
+      <c r="E114" s="6" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F114" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G114" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('wishlists')</v>
+      </c>
+      <c r="H114" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I114" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('cascade')</v>
+      </c>
+      <c r="J114" s="3" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K114" s="3" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
         <v>$table-&gt;foreign('wishlist')-&gt;references('id')-&gt;on('wishlists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
@@ -12520,10 +12604,10 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B114">
       <formula1>AvailableFields</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A114">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -25609,7 +25693,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B49">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E49">
@@ -25631,7 +25715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New scope web added
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2057" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="609">
   <si>
     <t>Name</t>
   </si>
@@ -1851,6 +1851,15 @@
   </si>
   <si>
     <t>list</t>
+  </si>
+  <si>
+    <t>ItemGroupWeb</t>
+  </si>
+  <si>
+    <t>Item group which are listable on web</t>
+  </si>
+  <si>
+    <t>web</t>
   </si>
 </sst>
 </file>
@@ -2071,19 +2080,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="64">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="63">
     <dxf>
       <font>
         <strike val="0"/>
@@ -2990,37 +2987,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J54" totalsRowShown="0" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J54" totalsRowShown="0" dataDxfId="62">
   <autoFilter ref="A1:J54">
     <filterColumn colId="3"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="62"/>
-    <tableColumn id="10" name="Table" dataDxfId="61">
+    <tableColumn id="2" name="Name" dataDxfId="61"/>
+    <tableColumn id="10" name="Table" dataDxfId="60">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="60">
+    <tableColumn id="5" name="Singular Name" dataDxfId="59">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="59">
+    <tableColumn id="8" name="Model NS" dataDxfId="58">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="58">
+    <tableColumn id="4" name="Class Name" dataDxfId="57">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="57">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="56">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="56">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="55">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="55">
+    <tableColumn id="3" name="Model Statement" dataDxfId="54">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="54">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="53">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="53">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="52">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3029,25 +3026,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I82" totalsRowShown="0" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I82" totalsRowShown="0" dataDxfId="50">
   <autoFilter ref="A1:I82"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="50"/>
-    <tableColumn id="2" name="Type" dataDxfId="49"/>
-    <tableColumn id="3" name="Name" dataDxfId="48"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="47"/>
-    <tableColumn id="5" name="Method1" dataDxfId="46"/>
-    <tableColumn id="6" name="Method2" dataDxfId="45"/>
-    <tableColumn id="7" name="Method3" dataDxfId="44"/>
-    <tableColumn id="8" name="Method4" dataDxfId="43"/>
-    <tableColumn id="9" name="Method5" dataDxfId="42"/>
+    <tableColumn id="1" name="Column" dataDxfId="49"/>
+    <tableColumn id="2" name="Type" dataDxfId="48"/>
+    <tableColumn id="3" name="Name" dataDxfId="47"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="46"/>
+    <tableColumn id="5" name="Method1" dataDxfId="45"/>
+    <tableColumn id="6" name="Method2" dataDxfId="44"/>
+    <tableColumn id="7" name="Method3" dataDxfId="43"/>
+    <tableColumn id="8" name="Method4" dataDxfId="42"/>
+    <tableColumn id="9" name="Method5" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K114" totalsRowShown="0" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K114" totalsRowShown="0" dataDxfId="40">
   <autoFilter ref="A1:K114">
     <filterColumn colId="0">
       <filters>
@@ -3056,33 +3053,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="40"/>
-    <tableColumn id="3" name="Field" dataDxfId="39"/>
-    <tableColumn id="5" name="Type" dataDxfId="38">
+    <tableColumn id="2" name="Table" dataDxfId="39"/>
+    <tableColumn id="3" name="Field" dataDxfId="38"/>
+    <tableColumn id="5" name="Type" dataDxfId="37">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="37">
+    <tableColumn id="4" name="Name" dataDxfId="36">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="36">
+    <tableColumn id="6" name="Arg2" dataDxfId="35">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="35">
+    <tableColumn id="7" name="Method1" dataDxfId="34">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="34">
+    <tableColumn id="8" name="Method2" dataDxfId="33">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="33">
+    <tableColumn id="9" name="Method3" dataDxfId="32">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="32">
+    <tableColumn id="10" name="Method4" dataDxfId="31">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="31">
+    <tableColumn id="11" name="Method5" dataDxfId="30">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="30">
+    <tableColumn id="12" name="Statement" dataDxfId="29">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3091,60 +3088,60 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R330" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:R330">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R331" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:R331">
     <filterColumn colId="1">
       <filters>
-        <filter val="Resource Form Field Data"/>
+        <filter val="Resource Scopes"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="27">
+    <tableColumn id="19" name="TRCode" dataDxfId="26">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="26"/>
-    <tableColumn id="2" name="Record No" dataDxfId="25">
+    <tableColumn id="1" name="Table Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Record No" dataDxfId="24">
       <calculatedColumnFormula>IF(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])=1,0,IF(ISNUMBER(VLOOKUP([Table Name],SeedMap[],6,0)),COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])+VLOOKUP([Table Name],SeedMap[],6,0)-1,COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="24"/>
-    <tableColumn id="4" name="2" dataDxfId="23"/>
-    <tableColumn id="5" name="3" dataDxfId="22"/>
-    <tableColumn id="6" name="4" dataDxfId="21"/>
-    <tableColumn id="7" name="5" dataDxfId="20"/>
-    <tableColumn id="8" name="6" dataDxfId="19"/>
-    <tableColumn id="9" name="7" dataDxfId="18"/>
-    <tableColumn id="10" name="8" dataDxfId="17"/>
-    <tableColumn id="11" name="9" dataDxfId="16"/>
-    <tableColumn id="12" name="10" dataDxfId="15"/>
-    <tableColumn id="13" name="11" dataDxfId="14"/>
-    <tableColumn id="14" name="12" dataDxfId="13"/>
-    <tableColumn id="15" name="13" dataDxfId="12"/>
-    <tableColumn id="16" name="14" dataDxfId="11"/>
-    <tableColumn id="17" name="15" dataDxfId="10"/>
+    <tableColumn id="3" name="1" dataDxfId="23"/>
+    <tableColumn id="4" name="2" dataDxfId="22"/>
+    <tableColumn id="5" name="3" dataDxfId="21"/>
+    <tableColumn id="6" name="4" dataDxfId="20"/>
+    <tableColumn id="7" name="5" dataDxfId="19"/>
+    <tableColumn id="8" name="6" dataDxfId="18"/>
+    <tableColumn id="9" name="7" dataDxfId="17"/>
+    <tableColumn id="10" name="8" dataDxfId="16"/>
+    <tableColumn id="11" name="9" dataDxfId="15"/>
+    <tableColumn id="12" name="10" dataDxfId="14"/>
+    <tableColumn id="13" name="11" dataDxfId="13"/>
+    <tableColumn id="14" name="12" dataDxfId="12"/>
+    <tableColumn id="15" name="13" dataDxfId="11"/>
+    <tableColumn id="16" name="14" dataDxfId="10"/>
+    <tableColumn id="17" name="15" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:G49" totalsRowShown="0" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:G49" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:G49">
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="7"/>
-    <tableColumn id="3" name="Table Name" dataDxfId="6"/>
-    <tableColumn id="20" name="NS" dataDxfId="5">
+    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="3" name="Table Name" dataDxfId="5"/>
+    <tableColumn id="20" name="NS" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP([Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="4">
+    <tableColumn id="21" name="Model" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP([Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="3"/>
-    <tableColumn id="2" name="Last ID" dataDxfId="2"/>
-    <tableColumn id="5" name="AI Change Query" dataDxfId="1">
+    <tableColumn id="4" name="Query Method" dataDxfId="2"/>
+    <tableColumn id="2" name="Last ID" dataDxfId="1"/>
+    <tableColumn id="5" name="AI Change Query" dataDxfId="0">
       <calculatedColumnFormula>IF(ISNUMBER([Last ID]),"ALTER TABLE `" &amp; [Table Name] &amp; "`  AUTO_INCREMENT=" &amp; [Last ID]+1,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7490,7 +7487,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A82">
-    <cfRule type="duplicateValues" dxfId="52" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="29"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -7504,7 +7501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2:K10"/>
     </sheetView>
   </sheetViews>
@@ -12621,10 +12618,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R330"/>
+  <dimension ref="A1:R331"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E173" sqref="E173"/>
+      <selection activeCell="D331" sqref="D331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12911,7 +12908,7 @@
       <c r="Q7" s="32"/>
       <c r="R7" s="32"/>
     </row>
-    <row r="8" spans="1:18" hidden="1">
+    <row r="8" spans="1:18">
       <c r="A8" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Scopes-0</v>
@@ -13093,7 +13090,7 @@
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" hidden="1">
       <c r="A13" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-0</v>
@@ -14931,7 +14928,7 @@
       <c r="Q59" s="32"/>
       <c r="R59" s="32"/>
     </row>
-    <row r="60" spans="1:18" hidden="1">
+    <row r="60" spans="1:18">
       <c r="A60" s="38" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Scopes-1</v>
@@ -14967,7 +14964,7 @@
       <c r="Q60" s="37"/>
       <c r="R60" s="37"/>
     </row>
-    <row r="61" spans="1:18" hidden="1">
+    <row r="61" spans="1:18">
       <c r="A61" s="38" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Scopes-2</v>
@@ -15003,7 +15000,7 @@
       <c r="Q61" s="37"/>
       <c r="R61" s="37"/>
     </row>
-    <row r="62" spans="1:18" hidden="1">
+    <row r="62" spans="1:18">
       <c r="A62" s="38" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Scopes-3</v>
@@ -15039,7 +15036,7 @@
       <c r="Q62" s="37"/>
       <c r="R62" s="37"/>
     </row>
-    <row r="63" spans="1:18" hidden="1">
+    <row r="63" spans="1:18">
       <c r="A63" s="38" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Scopes-4</v>
@@ -15795,7 +15792,7 @@
       <c r="Q81" s="37"/>
       <c r="R81" s="37"/>
     </row>
-    <row r="82" spans="1:18" hidden="1">
+    <row r="82" spans="1:18">
       <c r="A82" s="38" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Scopes-5</v>
@@ -18121,7 +18118,7 @@
       <c r="Q147" s="42"/>
       <c r="R147" s="42"/>
     </row>
-    <row r="148" spans="1:18">
+    <row r="148" spans="1:18" hidden="1">
       <c r="A148" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-1</v>
@@ -18153,7 +18150,7 @@
       <c r="Q148" s="42"/>
       <c r="R148" s="42"/>
     </row>
-    <row r="149" spans="1:18">
+    <row r="149" spans="1:18" hidden="1">
       <c r="A149" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-2</v>
@@ -18185,7 +18182,7 @@
       <c r="Q149" s="42"/>
       <c r="R149" s="42"/>
     </row>
-    <row r="150" spans="1:18">
+    <row r="150" spans="1:18" hidden="1">
       <c r="A150" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-3</v>
@@ -18217,7 +18214,7 @@
       <c r="Q150" s="42"/>
       <c r="R150" s="42"/>
     </row>
-    <row r="151" spans="1:18">
+    <row r="151" spans="1:18" hidden="1">
       <c r="A151" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-4</v>
@@ -18323,7 +18320,7 @@
       <c r="Q153" s="42"/>
       <c r="R153" s="42"/>
     </row>
-    <row r="154" spans="1:18">
+    <row r="154" spans="1:18" hidden="1">
       <c r="A154" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-5</v>
@@ -18567,7 +18564,7 @@
       <c r="Q160" s="42"/>
       <c r="R160" s="42"/>
     </row>
-    <row r="161" spans="1:18">
+    <row r="161" spans="1:18" hidden="1">
       <c r="A161" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-6</v>
@@ -18599,7 +18596,7 @@
       <c r="Q161" s="42"/>
       <c r="R161" s="42"/>
     </row>
-    <row r="162" spans="1:18">
+    <row r="162" spans="1:18" hidden="1">
       <c r="A162" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-7</v>
@@ -18631,7 +18628,7 @@
       <c r="Q162" s="42"/>
       <c r="R162" s="42"/>
     </row>
-    <row r="163" spans="1:18">
+    <row r="163" spans="1:18" hidden="1">
       <c r="A163" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-8</v>
@@ -18911,7 +18908,7 @@
       <c r="Q170" s="42"/>
       <c r="R170" s="42"/>
     </row>
-    <row r="171" spans="1:18">
+    <row r="171" spans="1:18" hidden="1">
       <c r="A171" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-9</v>
@@ -18943,7 +18940,7 @@
       <c r="Q171" s="42"/>
       <c r="R171" s="42"/>
     </row>
-    <row r="172" spans="1:18" s="16" customFormat="1">
+    <row r="172" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A172" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-10</v>
@@ -18975,7 +18972,7 @@
       <c r="Q172" s="42"/>
       <c r="R172" s="42"/>
     </row>
-    <row r="173" spans="1:18">
+    <row r="173" spans="1:18" hidden="1">
       <c r="A173" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-11</v>
@@ -19119,7 +19116,7 @@
       <c r="Q176" s="40"/>
       <c r="R176" s="40"/>
     </row>
-    <row r="177" spans="1:18">
+    <row r="177" spans="1:18" hidden="1">
       <c r="A177" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-12</v>
@@ -19151,7 +19148,7 @@
       <c r="Q177" s="40"/>
       <c r="R177" s="40"/>
     </row>
-    <row r="178" spans="1:18">
+    <row r="178" spans="1:18" hidden="1">
       <c r="A178" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-13</v>
@@ -19293,7 +19290,7 @@
       <c r="Q181" s="42"/>
       <c r="R181" s="42"/>
     </row>
-    <row r="182" spans="1:18">
+    <row r="182" spans="1:18" hidden="1">
       <c r="A182" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-14</v>
@@ -19325,7 +19322,7 @@
       <c r="Q182" s="40"/>
       <c r="R182" s="40"/>
     </row>
-    <row r="183" spans="1:18">
+    <row r="183" spans="1:18" hidden="1">
       <c r="A183" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-15</v>
@@ -19503,7 +19500,7 @@
       <c r="Q187" s="42"/>
       <c r="R187" s="42"/>
     </row>
-    <row r="188" spans="1:18">
+    <row r="188" spans="1:18" hidden="1">
       <c r="A188" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-16</v>
@@ -19535,7 +19532,7 @@
       <c r="Q188" s="40"/>
       <c r="R188" s="40"/>
     </row>
-    <row r="189" spans="1:18">
+    <row r="189" spans="1:18" hidden="1">
       <c r="A189" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Form Field Data-17</v>
@@ -20089,7 +20086,7 @@
       <c r="Q204" s="42"/>
       <c r="R204" s="42"/>
     </row>
-    <row r="205" spans="1:18" hidden="1">
+    <row r="205" spans="1:18">
       <c r="A205" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Scopes-6</v>
@@ -24442,6 +24439,42 @@
       <c r="P330" s="42"/>
       <c r="Q330" s="42"/>
       <c r="R330" s="42"/>
+    </row>
+    <row r="331" spans="1:18">
+      <c r="A331" s="41" t="str">
+        <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
+        <v>Resource Scopes-7</v>
+      </c>
+      <c r="B331" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C331" s="41">
+        <f>IF(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])=1,0,IF(ISNUMBER(VLOOKUP([Table Name],SeedMap[],6,0)),COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])+VLOOKUP([Table Name],SeedMap[],6,0)-1,COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1))</f>
+        <v>507</v>
+      </c>
+      <c r="D331" s="42">
+        <v>301</v>
+      </c>
+      <c r="E331" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="F331" s="42" t="s">
+        <v>607</v>
+      </c>
+      <c r="G331" s="42" t="s">
+        <v>608</v>
+      </c>
+      <c r="H331" s="42"/>
+      <c r="I331" s="42"/>
+      <c r="J331" s="42"/>
+      <c r="K331" s="42"/>
+      <c r="L331" s="42"/>
+      <c r="M331" s="42"/>
+      <c r="N331" s="42"/>
+      <c r="O331" s="42"/>
+      <c r="P331" s="42"/>
+      <c r="Q331" s="42"/>
+      <c r="R331" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25693,7 +25726,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B49">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E49">
@@ -25715,8 +25748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T208"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25726,14 +25759,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="50" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldData::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceScope::query()</v>
       </c>
       <c r="F1" s="50"/>
       <c r="G1" s="50"/>
@@ -25881,27 +25914,27 @@
       </c>
       <c r="D5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>form_field</v>
+        <v>resource</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>attribute</v>
+        <v>name</v>
       </c>
       <c r="F5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"id",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>relation</v>
+        <v>description</v>
       </c>
       <c r="G5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>nest_relation1</v>
+        <v>method</v>
       </c>
       <c r="H5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>nest_relation2</v>
+        <v/>
       </c>
       <c r="I5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>nest_relation3</v>
+        <v/>
       </c>
       <c r="J5" s="23" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
@@ -25991,7 +26024,7 @@
       <c r="A8" s="21"/>
       <c r="B8" s="48" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldData::query()</v>
+        <v>\Milestone\Appframe\Model\ResourceScope::query()</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -26024,19 +26057,19 @@
       </c>
       <c r="D9" s="22" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'form_field' =&gt; '501', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'product', </v>
+        <v xml:space="preserve">'name' =&gt; 'ItemGroupCategory', </v>
       </c>
       <c r="F9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Category from Item Group', </v>
       </c>
       <c r="G9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'category', </v>
       </c>
       <c r="H9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26097,19 +26130,19 @@
       </c>
       <c r="D10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '502', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
+        <v xml:space="preserve">'name' =&gt; 'ItemGroupBrand', </v>
       </c>
       <c r="F10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Brand from Item Group', </v>
       </c>
       <c r="G10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'brand', </v>
       </c>
       <c r="H10" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26170,19 +26203,19 @@
       </c>
       <c r="D11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '503', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'image', </v>
+        <v xml:space="preserve">'name' =&gt; 'ItemGroupSize', </v>
       </c>
       <c r="F11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Size from Item Group', </v>
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'size', </v>
       </c>
       <c r="H11" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26243,19 +26276,19 @@
       </c>
       <c r="D12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '504', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'default', </v>
+        <v xml:space="preserve">'name' =&gt; 'ItemGroupColor', </v>
       </c>
       <c r="F12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Color from Item Group', </v>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'color', </v>
       </c>
       <c r="H12" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26316,19 +26349,19 @@
       </c>
       <c r="D13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '505', </v>
+        <v xml:space="preserve">'resource' =&gt; '305', </v>
       </c>
       <c r="E13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'status', </v>
+        <v xml:space="preserve">'name' =&gt; 'WishlistVendorActive', </v>
       </c>
       <c r="F13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Wishlists which are shared with vendor', </v>
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'vendorShare', </v>
       </c>
       <c r="H13" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26389,19 +26422,19 @@
       </c>
       <c r="D14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '506', </v>
+        <v xml:space="preserve">'resource' =&gt; '303', </v>
       </c>
       <c r="E14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
+        <v xml:space="preserve">'name' =&gt; 'ImageStatus', </v>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Get image status', </v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'statusOnly', </v>
       </c>
       <c r="H14" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26462,19 +26495,19 @@
       </c>
       <c r="D15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '507', </v>
+        <v xml:space="preserve">'resource' =&gt; '301', </v>
       </c>
       <c r="E15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'email', </v>
+        <v xml:space="preserve">'name' =&gt; 'ItemGroupWeb', </v>
       </c>
       <c r="F15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Item group which are listable on web', </v>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'web', </v>
       </c>
       <c r="H15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26527,19 +26560,19 @@
       </c>
       <c r="B16" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v>;</v>
       </c>
       <c r="C16" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '508', </v>
+        <v/>
       </c>
       <c r="D16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '508', </v>
+        <v/>
       </c>
       <c r="E16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'number', </v>
+        <v/>
       </c>
       <c r="F16" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26591,7 +26624,7 @@
       </c>
       <c r="R16" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -26600,19 +26633,19 @@
       </c>
       <c r="B17" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C17" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '509', </v>
+        <v/>
       </c>
       <c r="D17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '509', </v>
+        <v/>
       </c>
       <c r="E17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
+        <v/>
       </c>
       <c r="F17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26664,7 +26697,7 @@
       </c>
       <c r="R17" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -26673,19 +26706,19 @@
       </c>
       <c r="B18" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C18" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '510', </v>
+        <v/>
       </c>
       <c r="D18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '510', </v>
+        <v/>
       </c>
       <c r="E18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'description', </v>
+        <v/>
       </c>
       <c r="F18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26737,7 +26770,7 @@
       </c>
       <c r="R18" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -26746,23 +26779,23 @@
       </c>
       <c r="B19" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C19" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '511', </v>
+        <v/>
       </c>
       <c r="D19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '511', </v>
+        <v/>
       </c>
       <c r="E19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'product', </v>
+        <v/>
       </c>
       <c r="F19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relation' =&gt; '518', </v>
+        <v/>
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26810,7 +26843,7 @@
       </c>
       <c r="R19" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -26819,19 +26852,19 @@
       </c>
       <c r="B20" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C20" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '512', </v>
+        <v/>
       </c>
       <c r="D20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '512', </v>
+        <v/>
       </c>
       <c r="E20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
+        <v/>
       </c>
       <c r="F20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26883,7 +26916,7 @@
       </c>
       <c r="R20" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -26892,19 +26925,19 @@
       </c>
       <c r="B21" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C21" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '513', </v>
+        <v/>
       </c>
       <c r="D21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '513', </v>
+        <v/>
       </c>
       <c r="E21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'description', </v>
+        <v/>
       </c>
       <c r="F21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -26956,7 +26989,7 @@
       </c>
       <c r="R21" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -26965,19 +26998,19 @@
       </c>
       <c r="B22" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C22" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '514', </v>
+        <v/>
       </c>
       <c r="D22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '514', </v>
+        <v/>
       </c>
       <c r="E22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'wishlist', </v>
+        <v/>
       </c>
       <c r="F22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27029,7 +27062,7 @@
       </c>
       <c r="R22" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -27038,19 +27071,19 @@
       </c>
       <c r="B23" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C23" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '515', </v>
+        <v/>
       </c>
       <c r="D23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '515', </v>
+        <v/>
       </c>
       <c r="E23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'visitor', </v>
+        <v/>
       </c>
       <c r="F23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27102,7 +27135,7 @@
       </c>
       <c r="R23" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -27111,19 +27144,19 @@
       </c>
       <c r="B24" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C24" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '516', </v>
+        <v/>
       </c>
       <c r="D24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'form_field' =&gt; '516', </v>
+        <v/>
       </c>
       <c r="E24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'attribute' =&gt; 'wishlist', </v>
+        <v/>
       </c>
       <c r="F24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -27175,7 +27208,7 @@
       </c>
       <c r="R24" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -27184,19 +27217,19 @@
       </c>
       <c r="B25" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'id' =&gt; '517', </v>
+        <v/>
       </c>
       <c r="D25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'form_field' =&gt; '517', </v>
+        <v/>
       </c>
       <c r="E25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'attribute' =&gt; 'note', </v>
+        <v/>
       </c>
       <c r="F25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27248,7 +27281,7 @@
       </c>
       <c r="R25" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -27257,7 +27290,7 @@
       </c>
       <c r="B26" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v/>
       </c>
       <c r="C26" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -27330,7 +27363,7 @@
       </c>
       <c r="B27" s="19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v/>
       </c>
       <c r="C27" s="22" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Modified as per requirements
</commit_message>
<xml_diff>
--- a/teeb.xlsx
+++ b/teeb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="623">
   <si>
     <t>Name</t>
   </si>
@@ -1896,6 +1896,12 @@
   </si>
   <si>
     <t>Web List</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -2129,7 +2135,8 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2138,11 +2145,115 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2414,8 +2525,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2424,115 +2534,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="8"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3124,60 +3130,60 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R349" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R349" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:R349">
     <filterColumn colId="1">
       <filters>
-        <filter val="Resource List Layout"/>
+        <filter val="Resource Action Method"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="19">
+    <tableColumn id="19" name="TRCode" dataDxfId="26">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="18"/>
-    <tableColumn id="2" name="Record No" dataDxfId="17">
+    <tableColumn id="1" name="Table Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Record No" dataDxfId="24">
       <calculatedColumnFormula>IF(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])=1,0,IF(ISNUMBER(VLOOKUP([Table Name],SeedMap[],6,0)),COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])+VLOOKUP([Table Name],SeedMap[],6,0)-1,COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="16"/>
-    <tableColumn id="4" name="2" dataDxfId="15"/>
-    <tableColumn id="5" name="3" dataDxfId="14"/>
-    <tableColumn id="6" name="4" dataDxfId="13"/>
-    <tableColumn id="7" name="5" dataDxfId="12"/>
-    <tableColumn id="8" name="6" dataDxfId="11"/>
-    <tableColumn id="9" name="7" dataDxfId="10"/>
-    <tableColumn id="10" name="8" dataDxfId="9"/>
-    <tableColumn id="11" name="9" dataDxfId="8"/>
-    <tableColumn id="12" name="10" dataDxfId="7"/>
-    <tableColumn id="13" name="11" dataDxfId="6"/>
-    <tableColumn id="14" name="12" dataDxfId="5"/>
-    <tableColumn id="15" name="13" dataDxfId="4"/>
-    <tableColumn id="16" name="14" dataDxfId="3"/>
-    <tableColumn id="17" name="15" dataDxfId="2"/>
+    <tableColumn id="3" name="1" dataDxfId="23"/>
+    <tableColumn id="4" name="2" dataDxfId="22"/>
+    <tableColumn id="5" name="3" dataDxfId="21"/>
+    <tableColumn id="6" name="4" dataDxfId="20"/>
+    <tableColumn id="7" name="5" dataDxfId="19"/>
+    <tableColumn id="8" name="6" dataDxfId="18"/>
+    <tableColumn id="9" name="7" dataDxfId="17"/>
+    <tableColumn id="10" name="8" dataDxfId="16"/>
+    <tableColumn id="11" name="9" dataDxfId="15"/>
+    <tableColumn id="12" name="10" dataDxfId="14"/>
+    <tableColumn id="13" name="11" dataDxfId="13"/>
+    <tableColumn id="14" name="12" dataDxfId="12"/>
+    <tableColumn id="15" name="13" dataDxfId="11"/>
+    <tableColumn id="16" name="14" dataDxfId="10"/>
+    <tableColumn id="17" name="15" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:G49" totalsRowShown="0" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:G49" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:G49">
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="Name" dataDxfId="26"/>
-    <tableColumn id="3" name="Table Name" dataDxfId="25"/>
-    <tableColumn id="20" name="NS" dataDxfId="24">
+    <tableColumn id="1" name="Name" dataDxfId="6"/>
+    <tableColumn id="3" name="Table Name" dataDxfId="5"/>
+    <tableColumn id="20" name="NS" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP([Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="23">
+    <tableColumn id="21" name="Model" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP([Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="22"/>
-    <tableColumn id="2" name="Last ID" dataDxfId="21"/>
-    <tableColumn id="5" name="AI Change Query" dataDxfId="20">
+    <tableColumn id="4" name="Query Method" dataDxfId="2"/>
+    <tableColumn id="2" name="Last ID" dataDxfId="1"/>
+    <tableColumn id="5" name="AI Change Query" dataDxfId="0">
       <calculatedColumnFormula>IF(ISNUMBER([Last ID]),"ALTER TABLE `" &amp; [Table Name] &amp; "`  AUTO_INCREMENT=" &amp; [Last ID]+1,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -12656,8 +12662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R349"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D253" sqref="D253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13210,7 +13216,7 @@
       <c r="Q14" s="32"/>
       <c r="R14" s="32"/>
     </row>
-    <row r="15" spans="1:18" hidden="1">
+    <row r="15" spans="1:18">
       <c r="A15" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-0</v>
@@ -13482,7 +13488,7 @@
       <c r="Q21" s="32"/>
       <c r="R21" s="32"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" hidden="1">
       <c r="A22" s="31" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-0</v>
@@ -16940,7 +16946,7 @@
       <c r="Q112" s="42"/>
       <c r="R112" s="42"/>
     </row>
-    <row r="113" spans="1:18" s="16" customFormat="1">
+    <row r="113" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A113" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-1</v>
@@ -16974,7 +16980,7 @@
       <c r="Q113" s="42"/>
       <c r="R113" s="42"/>
     </row>
-    <row r="114" spans="1:18" s="16" customFormat="1">
+    <row r="114" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A114" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-2</v>
@@ -17008,7 +17014,7 @@
       <c r="Q114" s="42"/>
       <c r="R114" s="42"/>
     </row>
-    <row r="115" spans="1:18" s="16" customFormat="1">
+    <row r="115" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A115" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-3</v>
@@ -17042,7 +17048,7 @@
       <c r="Q115" s="42"/>
       <c r="R115" s="42"/>
     </row>
-    <row r="116" spans="1:18" s="16" customFormat="1">
+    <row r="116" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A116" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-4</v>
@@ -17076,7 +17082,7 @@
       <c r="Q116" s="42"/>
       <c r="R116" s="42"/>
     </row>
-    <row r="117" spans="1:18" s="16" customFormat="1">
+    <row r="117" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A117" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-5</v>
@@ -17110,7 +17116,7 @@
       <c r="Q117" s="42"/>
       <c r="R117" s="42"/>
     </row>
-    <row r="118" spans="1:18" s="16" customFormat="1">
+    <row r="118" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A118" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-6</v>
@@ -17144,7 +17150,7 @@
       <c r="Q118" s="42"/>
       <c r="R118" s="42"/>
     </row>
-    <row r="119" spans="1:18" s="16" customFormat="1">
+    <row r="119" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A119" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-7</v>
@@ -17178,7 +17184,7 @@
       <c r="Q119" s="42"/>
       <c r="R119" s="42"/>
     </row>
-    <row r="120" spans="1:18" s="16" customFormat="1">
+    <row r="120" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A120" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-8</v>
@@ -17212,7 +17218,7 @@
       <c r="Q120" s="42"/>
       <c r="R120" s="42"/>
     </row>
-    <row r="121" spans="1:18" s="16" customFormat="1">
+    <row r="121" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A121" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-9</v>
@@ -17246,7 +17252,7 @@
       <c r="Q121" s="42"/>
       <c r="R121" s="42"/>
     </row>
-    <row r="122" spans="1:18" s="16" customFormat="1">
+    <row r="122" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A122" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-10</v>
@@ -17280,7 +17286,7 @@
       <c r="Q122" s="42"/>
       <c r="R122" s="42"/>
     </row>
-    <row r="123" spans="1:18" s="16" customFormat="1">
+    <row r="123" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A123" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-11</v>
@@ -17314,7 +17320,7 @@
       <c r="Q123" s="42"/>
       <c r="R123" s="42"/>
     </row>
-    <row r="124" spans="1:18" s="16" customFormat="1">
+    <row r="124" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A124" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-12</v>
@@ -17348,7 +17354,7 @@
       <c r="Q124" s="42"/>
       <c r="R124" s="42"/>
     </row>
-    <row r="125" spans="1:18" s="16" customFormat="1">
+    <row r="125" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A125" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-13</v>
@@ -17382,7 +17388,7 @@
       <c r="Q125" s="42"/>
       <c r="R125" s="42"/>
     </row>
-    <row r="126" spans="1:18" s="16" customFormat="1">
+    <row r="126" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A126" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-14</v>
@@ -17416,7 +17422,7 @@
       <c r="Q126" s="42"/>
       <c r="R126" s="42"/>
     </row>
-    <row r="127" spans="1:18" s="16" customFormat="1">
+    <row r="127" spans="1:18" s="16" customFormat="1" hidden="1">
       <c r="A127" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-15</v>
@@ -17450,7 +17456,7 @@
       <c r="Q127" s="42"/>
       <c r="R127" s="42"/>
     </row>
-    <row r="128" spans="1:18">
+    <row r="128" spans="1:18" hidden="1">
       <c r="A128" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-16</v>
@@ -17484,7 +17490,7 @@
       <c r="Q128" s="42"/>
       <c r="R128" s="42"/>
     </row>
-    <row r="129" spans="1:18">
+    <row r="129" spans="1:18" hidden="1">
       <c r="A129" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-17</v>
@@ -17505,7 +17511,9 @@
       <c r="F129" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="G129" s="42"/>
+      <c r="G129" s="42">
+        <v>508</v>
+      </c>
       <c r="H129" s="42"/>
       <c r="I129" s="42"/>
       <c r="J129" s="42"/>
@@ -17518,7 +17526,7 @@
       <c r="Q129" s="42"/>
       <c r="R129" s="42"/>
     </row>
-    <row r="130" spans="1:18">
+    <row r="130" spans="1:18" hidden="1">
       <c r="A130" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-18</v>
@@ -17554,7 +17562,7 @@
       <c r="Q130" s="42"/>
       <c r="R130" s="42"/>
     </row>
-    <row r="131" spans="1:18">
+    <row r="131" spans="1:18" hidden="1">
       <c r="A131" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-19</v>
@@ -17590,7 +17598,7 @@
       <c r="Q131" s="42"/>
       <c r="R131" s="42"/>
     </row>
-    <row r="132" spans="1:18">
+    <row r="132" spans="1:18" hidden="1">
       <c r="A132" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-20</v>
@@ -17606,14 +17614,12 @@
         <v>505</v>
       </c>
       <c r="E132" s="42" t="s">
-        <v>400</v>
+        <v>621</v>
       </c>
       <c r="F132" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="G132" s="42">
-        <v>507</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="G132" s="42"/>
       <c r="H132" s="42"/>
       <c r="I132" s="42"/>
       <c r="J132" s="42"/>
@@ -17626,7 +17632,7 @@
       <c r="Q132" s="42"/>
       <c r="R132" s="42"/>
     </row>
-    <row r="133" spans="1:18">
+    <row r="133" spans="1:18" hidden="1">
       <c r="A133" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-21</v>
@@ -17642,14 +17648,12 @@
         <v>505</v>
       </c>
       <c r="E133" s="42" t="s">
-        <v>401</v>
+        <v>622</v>
       </c>
       <c r="F133" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="G133" s="42">
-        <v>508</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="G133" s="42"/>
       <c r="H133" s="42"/>
       <c r="I133" s="42"/>
       <c r="J133" s="42"/>
@@ -17662,7 +17666,7 @@
       <c r="Q133" s="42"/>
       <c r="R133" s="42"/>
     </row>
-    <row r="134" spans="1:18">
+    <row r="134" spans="1:18" hidden="1">
       <c r="A134" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-22</v>
@@ -17696,7 +17700,7 @@
       <c r="Q134" s="42"/>
       <c r="R134" s="42"/>
     </row>
-    <row r="135" spans="1:18">
+    <row r="135" spans="1:18" hidden="1">
       <c r="A135" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-23</v>
@@ -17730,7 +17734,7 @@
       <c r="Q135" s="42"/>
       <c r="R135" s="42"/>
     </row>
-    <row r="136" spans="1:18">
+    <row r="136" spans="1:18" hidden="1">
       <c r="A136" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-24</v>
@@ -17764,7 +17768,7 @@
       <c r="Q136" s="42"/>
       <c r="R136" s="42"/>
     </row>
-    <row r="137" spans="1:18">
+    <row r="137" spans="1:18" hidden="1">
       <c r="A137" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-25</v>
@@ -17798,7 +17802,7 @@
       <c r="Q137" s="42"/>
       <c r="R137" s="42"/>
     </row>
-    <row r="138" spans="1:18">
+    <row r="138" spans="1:18" hidden="1">
       <c r="A138" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-26</v>
@@ -17834,7 +17838,7 @@
       <c r="Q138" s="42"/>
       <c r="R138" s="42"/>
     </row>
-    <row r="139" spans="1:18">
+    <row r="139" spans="1:18" hidden="1">
       <c r="A139" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-27</v>
@@ -17868,7 +17872,7 @@
       <c r="Q139" s="42"/>
       <c r="R139" s="42"/>
     </row>
-    <row r="140" spans="1:18">
+    <row r="140" spans="1:18" hidden="1">
       <c r="A140" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-28</v>
@@ -17902,7 +17906,7 @@
       <c r="Q140" s="40"/>
       <c r="R140" s="40"/>
     </row>
-    <row r="141" spans="1:18">
+    <row r="141" spans="1:18" hidden="1">
       <c r="A141" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-29</v>
@@ -17938,7 +17942,7 @@
       <c r="Q141" s="40"/>
       <c r="R141" s="40"/>
     </row>
-    <row r="142" spans="1:18">
+    <row r="142" spans="1:18" hidden="1">
       <c r="A142" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-30</v>
@@ -17972,7 +17976,7 @@
       <c r="Q142" s="42"/>
       <c r="R142" s="42"/>
     </row>
-    <row r="143" spans="1:18">
+    <row r="143" spans="1:18" hidden="1">
       <c r="A143" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-31</v>
@@ -18006,7 +18010,7 @@
       <c r="Q143" s="42"/>
       <c r="R143" s="42"/>
     </row>
-    <row r="144" spans="1:18">
+    <row r="144" spans="1:18" hidden="1">
       <c r="A144" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-32</v>
@@ -18040,7 +18044,7 @@
       <c r="Q144" s="42"/>
       <c r="R144" s="42"/>
     </row>
-    <row r="145" spans="1:18">
+    <row r="145" spans="1:18" hidden="1">
       <c r="A145" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-33</v>
@@ -21544,7 +21548,7 @@
       <c r="Q246" s="42"/>
       <c r="R246" s="42"/>
     </row>
-    <row r="247" spans="1:18" hidden="1">
+    <row r="247" spans="1:18">
       <c r="A247" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-1</v>
@@ -21616,7 +21620,7 @@
       <c r="Q248" s="40"/>
       <c r="R248" s="40"/>
     </row>
-    <row r="249" spans="1:18" hidden="1">
+    <row r="249" spans="1:18">
       <c r="A249" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-2</v>
@@ -21688,7 +21692,7 @@
       <c r="Q250" s="40"/>
       <c r="R250" s="40"/>
     </row>
-    <row r="251" spans="1:18" hidden="1">
+    <row r="251" spans="1:18">
       <c r="A251" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-3</v>
@@ -21760,7 +21764,7 @@
       <c r="Q252" s="40"/>
       <c r="R252" s="40"/>
     </row>
-    <row r="253" spans="1:18" hidden="1">
+    <row r="253" spans="1:18">
       <c r="A253" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-4</v>
@@ -21832,7 +21836,7 @@
       <c r="Q254" s="40"/>
       <c r="R254" s="40"/>
     </row>
-    <row r="255" spans="1:18" hidden="1">
+    <row r="255" spans="1:18">
       <c r="A255" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-5</v>
@@ -21904,7 +21908,7 @@
       <c r="Q256" s="40"/>
       <c r="R256" s="40"/>
     </row>
-    <row r="257" spans="1:18" hidden="1">
+    <row r="257" spans="1:18">
       <c r="A257" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-6</v>
@@ -21976,7 +21980,7 @@
       <c r="Q258" s="40"/>
       <c r="R258" s="40"/>
     </row>
-    <row r="259" spans="1:18" hidden="1">
+    <row r="259" spans="1:18">
       <c r="A259" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-7</v>
@@ -22048,7 +22052,7 @@
       <c r="Q260" s="40"/>
       <c r="R260" s="40"/>
     </row>
-    <row r="261" spans="1:18" hidden="1">
+    <row r="261" spans="1:18">
       <c r="A261" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-8</v>
@@ -22120,7 +22124,7 @@
       <c r="Q262" s="40"/>
       <c r="R262" s="40"/>
     </row>
-    <row r="263" spans="1:18" hidden="1">
+    <row r="263" spans="1:18">
       <c r="A263" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-9</v>
@@ -22192,7 +22196,7 @@
       <c r="Q264" s="40"/>
       <c r="R264" s="40"/>
     </row>
-    <row r="265" spans="1:18" hidden="1">
+    <row r="265" spans="1:18">
       <c r="A265" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-10</v>
@@ -22370,7 +22374,7 @@
       <c r="Q269" s="40"/>
       <c r="R269" s="40"/>
     </row>
-    <row r="270" spans="1:18" hidden="1">
+    <row r="270" spans="1:18">
       <c r="A270" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-11</v>
@@ -22406,7 +22410,7 @@
       <c r="Q270" s="42"/>
       <c r="R270" s="42"/>
     </row>
-    <row r="271" spans="1:18" hidden="1">
+    <row r="271" spans="1:18">
       <c r="A271" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-12</v>
@@ -22442,7 +22446,7 @@
       <c r="Q271" s="42"/>
       <c r="R271" s="42"/>
     </row>
-    <row r="272" spans="1:18" hidden="1">
+    <row r="272" spans="1:18">
       <c r="A272" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-13</v>
@@ -22478,7 +22482,7 @@
       <c r="Q272" s="42"/>
       <c r="R272" s="42"/>
     </row>
-    <row r="273" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="273" spans="1:18" s="16" customFormat="1">
       <c r="A273" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-14</v>
@@ -22678,7 +22682,7 @@
       <c r="Q278" s="42"/>
       <c r="R278" s="42"/>
     </row>
-    <row r="279" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="279" spans="1:18" s="16" customFormat="1">
       <c r="A279" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-15</v>
@@ -22820,7 +22824,7 @@
       <c r="Q282" s="42"/>
       <c r="R282" s="42"/>
     </row>
-    <row r="283" spans="1:18">
+    <row r="283" spans="1:18" hidden="1">
       <c r="A283" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-34</v>
@@ -22854,7 +22858,7 @@
       <c r="Q283" s="42"/>
       <c r="R283" s="42"/>
     </row>
-    <row r="284" spans="1:18">
+    <row r="284" spans="1:18" hidden="1">
       <c r="A284" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-35</v>
@@ -22888,7 +22892,7 @@
       <c r="Q284" s="42"/>
       <c r="R284" s="42"/>
     </row>
-    <row r="285" spans="1:18" hidden="1">
+    <row r="285" spans="1:18">
       <c r="A285" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-16</v>
@@ -22992,7 +22996,7 @@
       <c r="Q287" s="42"/>
       <c r="R287" s="42"/>
     </row>
-    <row r="288" spans="1:18" hidden="1">
+    <row r="288" spans="1:18">
       <c r="A288" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-17</v>
@@ -23096,7 +23100,7 @@
       <c r="Q290" s="40"/>
       <c r="R290" s="40"/>
     </row>
-    <row r="291" spans="1:18" hidden="1">
+    <row r="291" spans="1:18">
       <c r="A291" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-18</v>
@@ -23200,7 +23204,7 @@
       <c r="Q293" s="40"/>
       <c r="R293" s="40"/>
     </row>
-    <row r="294" spans="1:18" hidden="1">
+    <row r="294" spans="1:18">
       <c r="A294" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-19</v>
@@ -23304,7 +23308,7 @@
       <c r="Q296" s="40"/>
       <c r="R296" s="40"/>
     </row>
-    <row r="297" spans="1:18" hidden="1">
+    <row r="297" spans="1:18">
       <c r="A297" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-20</v>
@@ -23408,7 +23412,7 @@
       <c r="Q299" s="40"/>
       <c r="R299" s="40"/>
     </row>
-    <row r="300" spans="1:18" hidden="1">
+    <row r="300" spans="1:18">
       <c r="A300" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-21</v>
@@ -23608,7 +23612,7 @@
       <c r="Q305" s="42"/>
       <c r="R305" s="42"/>
     </row>
-    <row r="306" spans="1:18">
+    <row r="306" spans="1:18" hidden="1">
       <c r="A306" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-36</v>
@@ -23644,7 +23648,7 @@
       <c r="Q306" s="42"/>
       <c r="R306" s="42"/>
     </row>
-    <row r="307" spans="1:18">
+    <row r="307" spans="1:18" hidden="1">
       <c r="A307" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-37</v>
@@ -23680,7 +23684,7 @@
       <c r="Q307" s="42"/>
       <c r="R307" s="42"/>
     </row>
-    <row r="308" spans="1:18">
+    <row r="308" spans="1:18" hidden="1">
       <c r="A308" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource List Layout-38</v>
@@ -23752,7 +23756,7 @@
       <c r="Q309" s="40"/>
       <c r="R309" s="40"/>
     </row>
-    <row r="310" spans="1:18" hidden="1">
+    <row r="310" spans="1:18">
       <c r="A310" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-22</v>
@@ -23854,7 +23858,7 @@
       <c r="Q312" s="40"/>
       <c r="R312" s="40"/>
     </row>
-    <row r="313" spans="1:18" hidden="1">
+    <row r="313" spans="1:18">
       <c r="A313" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-23</v>
@@ -23958,7 +23962,7 @@
       <c r="Q315" s="40"/>
       <c r="R315" s="40"/>
     </row>
-    <row r="316" spans="1:18" hidden="1">
+    <row r="316" spans="1:18">
       <c r="A316" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-24</v>
@@ -24062,7 +24066,7 @@
       <c r="Q318" s="42"/>
       <c r="R318" s="42"/>
     </row>
-    <row r="319" spans="1:18" s="16" customFormat="1" hidden="1">
+    <row r="319" spans="1:18" s="16" customFormat="1">
       <c r="A319" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-25</v>
@@ -24166,7 +24170,7 @@
       <c r="Q321" s="40"/>
       <c r="R321" s="40"/>
     </row>
-    <row r="322" spans="1:18" hidden="1">
+    <row r="322" spans="1:18">
       <c r="A322" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-26</v>
@@ -24308,7 +24312,7 @@
       <c r="Q325" s="40"/>
       <c r="R325" s="40"/>
     </row>
-    <row r="326" spans="1:18" hidden="1">
+    <row r="326" spans="1:18">
       <c r="A326" s="39" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-27</v>
@@ -24476,7 +24480,7 @@
       <c r="Q330" s="42"/>
       <c r="R330" s="42"/>
     </row>
-    <row r="331" spans="1:18" hidden="1">
+    <row r="331" spans="1:18">
       <c r="A331" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-28</v>
@@ -24960,7 +24964,7 @@
       <c r="Q344" s="42"/>
       <c r="R344" s="42"/>
     </row>
-    <row r="345" spans="1:18" hidden="1">
+    <row r="345" spans="1:18">
       <c r="A345" s="41" t="str">
         <f>[Table Name]&amp;"-"&amp;(COUNTIF($B$1:TableData[[#This Row],[Table Name]],TableData[[#This Row],[Table Name]])-1)</f>
         <v>Resource Action Method-29</v>
@@ -26374,7 +26378,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B49">
-    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E49">
@@ -26396,8 +26400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27885,7 +27889,7 @@
       </c>
       <c r="G25" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'relation' =&gt; '508', </v>
       </c>
       <c r="H25" s="22" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
@@ -28096,15 +28100,15 @@
       </c>
       <c r="E28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'label' =&gt; 'Size', </v>
+        <v xml:space="preserve">'label' =&gt; 'Code', </v>
       </c>
       <c r="F28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'field' =&gt; 'name', </v>
+        <v xml:space="preserve">'field' =&gt; 'code', </v>
       </c>
       <c r="G28" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'relation' =&gt; '507', </v>
+        <v/>
       </c>
       <c r="H28" s="22" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -28169,15 +28173,15 @@
       </c>
       <c r="E29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'label' =&gt; 'Color', </v>
+        <v xml:space="preserve">'label' =&gt; 'Gender', </v>
       </c>
       <c r="F29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'field' =&gt; 'name', </v>
+        <v xml:space="preserve">'field' =&gt; 'narration2', </v>
       </c>
       <c r="G29" s="22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'relation' =&gt; '508', </v>
+        <v/>
       </c>
       <c r="H29" s="22" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>